<commit_message>
Fehlerbehandlungen bei Inkonsitenzen im Import
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="36" windowWidth="13440" windowHeight="9132" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="13440" windowHeight="9132" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stammdaten" sheetId="6" r:id="rId1"/>
@@ -1103,6 +1103,97 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF11E111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6CBCB4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31869B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF11E111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1292,97 +1383,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF11E111"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6CBCB4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF31869B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF007E39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF11E111"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1442,20 +1442,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ErgebnTabelle" displayName="ErgebnTabelle" ref="B10:I300" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ErgebnTabelle" displayName="ErgebnTabelle" ref="B10:I300" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B10:I300"/>
   <sortState ref="B12:E19">
     <sortCondition ref="B11:B19"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Nr." dataDxfId="7"/>
-    <tableColumn id="2" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" name="Bezug" dataDxfId="5"/>
-    <tableColumn id="4" name="StartDatum" dataDxfId="4"/>
-    <tableColumn id="8" name="EndeDatum" dataDxfId="3"/>
-    <tableColumn id="5" name="Ampel" dataDxfId="2"/>
-    <tableColumn id="6" name="Erläuterung " dataDxfId="1"/>
-    <tableColumn id="7" name="Maßnahmen" dataDxfId="0"/>
+    <tableColumn id="1" name="Nr." dataDxfId="20"/>
+    <tableColumn id="2" name="Name" dataDxfId="19"/>
+    <tableColumn id="3" name="Bezug" dataDxfId="18"/>
+    <tableColumn id="4" name="StartDatum" dataDxfId="17"/>
+    <tableColumn id="8" name="EndeDatum" dataDxfId="16"/>
+    <tableColumn id="5" name="Ampel" dataDxfId="15"/>
+    <tableColumn id="6" name="Erläuterung " dataDxfId="14"/>
+    <tableColumn id="7" name="Maßnahmen" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2167,16 +2167,16 @@
     <mergeCell ref="C23:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$C$21=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$C21=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$C21=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>$C21=3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2211,7 +2211,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:GH250"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -48470,9 +48470,6 @@
       <c r="D250" s="46"/>
       <c r="E250" s="46"/>
       <c r="F250" s="46"/>
-      <c r="G250" s="46"/>
-      <c r="H250" s="46"/>
-      <c r="I250" s="46"/>
       <c r="J250" s="46"/>
       <c r="K250" s="46"/>
       <c r="L250" s="46"/>
@@ -48660,22 +48657,22 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B116">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51845,13 +51842,13 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="G11:G300">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>G11=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>G11=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>G11=3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51886,7 +51883,7 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ProjektSteckbrief auf Hierarchie angepasst; Name 'RollenKosten_des_Projekts' geändert
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stammdaten" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="ProjektVorlagen">Settings!$A$4:$A$6</definedName>
     <definedName name="Risiko">Attribute!$E$16</definedName>
     <definedName name="Rollen_Kostenarten">Settings!$A$25:$A$31</definedName>
-    <definedName name="RollenKosten_des_Projekts">Ressourcen!$C$11:$C$250</definedName>
+    <definedName name="RollenKosten_des_Projekts">Ressourcen!$D$11:$D$250</definedName>
     <definedName name="StartDatum">Stammdaten!$C$4</definedName>
     <definedName name="Status">Attribute!$E$11</definedName>
     <definedName name="Strategischer_Fit">Attribute!$C$16</definedName>
@@ -993,6 +993,12 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1005,22 +1011,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1897,8 +1897,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:GI250"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1924,11 +1924,11 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="81">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
-      <c r="D2" s="86"/>
+      <c r="D2" s="82"/>
       <c r="E2" s="65"/>
       <c r="F2" s="65"/>
       <c r="G2" s="65"/>
@@ -1998,10 +1998,10 @@
     </row>
     <row r="9" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:191" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="37"/>
       <c r="E10" s="51">
         <f>StartDatum</f>
@@ -2750,8 +2750,8 @@
       <c r="GI10" s="49"/>
     </row>
     <row r="11" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="37"/>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
@@ -48590,8 +48590,226 @@
       <c r="GH250" s="41"/>
     </row>
   </sheetData>
-  <sheetProtection password="CEBA" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="242">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B221:C221"/>
     <mergeCell ref="B247:C247"/>
     <mergeCell ref="B248:C248"/>
     <mergeCell ref="B249:C249"/>
@@ -48616,224 +48834,6 @@
     <mergeCell ref="B228:C228"/>
     <mergeCell ref="B229:C229"/>
     <mergeCell ref="B230:C230"/>
-    <mergeCell ref="B231:C231"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B221:C221"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B250">
     <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
@@ -48915,11 +48915,11 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="81">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
-      <c r="D2" s="86"/>
+      <c r="D2" s="82"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -49069,8 +49069,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="89"/>
-      <c r="C11" s="90"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="60"/>
@@ -49078,8 +49078,8 @@
       <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="87"/>
-      <c r="C12" s="88"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
       <c r="F12" s="53"/>
@@ -49087,8 +49087,8 @@
       <c r="H12" s="58"/>
     </row>
     <row r="13" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="89"/>
-      <c r="C13" s="90"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="F13" s="60"/>
@@ -49096,8 +49096,8 @@
       <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="87"/>
-      <c r="C14" s="88"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
       <c r="F14" s="53"/>
@@ -49105,8 +49105,8 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="88"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="F15" s="60"/>
@@ -49114,8 +49114,8 @@
       <c r="H15" s="59"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
       <c r="F16" s="53"/>
@@ -49123,8 +49123,8 @@
       <c r="H16" s="58"/>
     </row>
     <row r="17" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="88"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="60"/>
@@ -49132,8 +49132,8 @@
       <c r="H17" s="59"/>
     </row>
     <row r="18" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
       <c r="F18" s="53"/>
@@ -49141,8 +49141,8 @@
       <c r="H18" s="58"/>
     </row>
     <row r="19" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="88"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="F19" s="60"/>
@@ -49150,8 +49150,8 @@
       <c r="H19" s="59"/>
     </row>
     <row r="20" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="87"/>
-      <c r="C20" s="88"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
       <c r="F20" s="53"/>
@@ -49159,8 +49159,8 @@
       <c r="H20" s="58"/>
     </row>
     <row r="21" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="60"/>
@@ -49168,8 +49168,8 @@
       <c r="H21" s="59"/>
     </row>
     <row r="22" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
       <c r="F22" s="53"/>
@@ -49177,8 +49177,8 @@
       <c r="H22" s="58"/>
     </row>
     <row r="23" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
       <c r="F23" s="60"/>
@@ -49186,8 +49186,8 @@
       <c r="H23" s="59"/>
     </row>
     <row r="24" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
       <c r="F24" s="53"/>
@@ -49195,8 +49195,8 @@
       <c r="H24" s="58"/>
     </row>
     <row r="25" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
       <c r="F25" s="60"/>
@@ -49204,8 +49204,8 @@
       <c r="H25" s="59"/>
     </row>
     <row r="26" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
       <c r="F26" s="53"/>
@@ -49213,8 +49213,8 @@
       <c r="H26" s="58"/>
     </row>
     <row r="27" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
       <c r="F27" s="60"/>
@@ -49222,8 +49222,8 @@
       <c r="H27" s="59"/>
     </row>
     <row r="28" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="87"/>
-      <c r="C28" s="88"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
       <c r="F28" s="53"/>
@@ -49231,8 +49231,8 @@
       <c r="H28" s="58"/>
     </row>
     <row r="29" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
       <c r="F29" s="60"/>
@@ -49240,8 +49240,8 @@
       <c r="H29" s="59"/>
     </row>
     <row r="30" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="87"/>
-      <c r="C30" s="88"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="56"/>
       <c r="E30" s="56"/>
       <c r="F30" s="53"/>
@@ -49249,8 +49249,8 @@
       <c r="H30" s="58"/>
     </row>
     <row r="31" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
       <c r="F31" s="60"/>
@@ -49258,8 +49258,8 @@
       <c r="H31" s="59"/>
     </row>
     <row r="32" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="87"/>
-      <c r="C32" s="88"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
       <c r="F32" s="53"/>
@@ -49267,8 +49267,8 @@
       <c r="H32" s="58"/>
     </row>
     <row r="33" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
       <c r="F33" s="60"/>
@@ -49276,8 +49276,8 @@
       <c r="H33" s="59"/>
     </row>
     <row r="34" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="87"/>
-      <c r="C34" s="88"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
       <c r="F34" s="53"/>
@@ -49285,8 +49285,8 @@
       <c r="H34" s="58"/>
     </row>
     <row r="35" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="89"/>
-      <c r="C35" s="90"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="88"/>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
       <c r="F35" s="60"/>
@@ -49294,8 +49294,8 @@
       <c r="H35" s="59"/>
     </row>
     <row r="36" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="87"/>
-      <c r="C36" s="88"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
       <c r="F36" s="53"/>
@@ -49303,8 +49303,8 @@
       <c r="H36" s="58"/>
     </row>
     <row r="37" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="89"/>
-      <c r="C37" s="90"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="88"/>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
       <c r="F37" s="60"/>
@@ -49312,8 +49312,8 @@
       <c r="H37" s="59"/>
     </row>
     <row r="38" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="87"/>
-      <c r="C38" s="88"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
       <c r="F38" s="53"/>
@@ -49321,8 +49321,8 @@
       <c r="H38" s="58"/>
     </row>
     <row r="39" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="89"/>
-      <c r="C39" s="90"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
       <c r="F39" s="60"/>
@@ -49330,8 +49330,8 @@
       <c r="H39" s="59"/>
     </row>
     <row r="40" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="87"/>
-      <c r="C40" s="88"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
       <c r="F40" s="53"/>
@@ -49339,8 +49339,8 @@
       <c r="H40" s="58"/>
     </row>
     <row r="41" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="89"/>
-      <c r="C41" s="90"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="88"/>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
       <c r="F41" s="60"/>
@@ -49348,8 +49348,8 @@
       <c r="H41" s="59"/>
     </row>
     <row r="42" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="87"/>
-      <c r="C42" s="88"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="90"/>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
       <c r="F42" s="53"/>
@@ -49357,8 +49357,8 @@
       <c r="H42" s="58"/>
     </row>
     <row r="43" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="88"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="60"/>
@@ -49366,8 +49366,8 @@
       <c r="H43" s="59"/>
     </row>
     <row r="44" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="87"/>
-      <c r="C44" s="88"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="90"/>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
       <c r="F44" s="53"/>
@@ -49375,8 +49375,8 @@
       <c r="H44" s="58"/>
     </row>
     <row r="45" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="89"/>
-      <c r="C45" s="90"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="88"/>
       <c r="D45" s="55"/>
       <c r="E45" s="55"/>
       <c r="F45" s="60"/>
@@ -49384,8 +49384,8 @@
       <c r="H45" s="59"/>
     </row>
     <row r="46" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="87"/>
-      <c r="C46" s="88"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
       <c r="F46" s="53"/>
@@ -49393,8 +49393,8 @@
       <c r="H46" s="58"/>
     </row>
     <row r="47" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="89"/>
-      <c r="C47" s="90"/>
+      <c r="B47" s="87"/>
+      <c r="C47" s="88"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
       <c r="F47" s="60"/>
@@ -49402,8 +49402,8 @@
       <c r="H47" s="59"/>
     </row>
     <row r="48" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="87"/>
-      <c r="C48" s="88"/>
+      <c r="B48" s="89"/>
+      <c r="C48" s="90"/>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
       <c r="F48" s="53"/>
@@ -49411,8 +49411,8 @@
       <c r="H48" s="58"/>
     </row>
     <row r="49" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="89"/>
-      <c r="C49" s="90"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="88"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
       <c r="F49" s="60"/>
@@ -49420,8 +49420,8 @@
       <c r="H49" s="59"/>
     </row>
     <row r="50" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="87"/>
-      <c r="C50" s="88"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="90"/>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
       <c r="F50" s="53"/>
@@ -49429,8 +49429,8 @@
       <c r="H50" s="58"/>
     </row>
     <row r="51" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="88"/>
       <c r="D51" s="55"/>
       <c r="E51" s="55"/>
       <c r="F51" s="60"/>
@@ -49438,8 +49438,8 @@
       <c r="H51" s="59"/>
     </row>
     <row r="52" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="87"/>
-      <c r="C52" s="88"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="90"/>
       <c r="D52" s="56"/>
       <c r="E52" s="56"/>
       <c r="F52" s="53"/>
@@ -49447,8 +49447,8 @@
       <c r="H52" s="58"/>
     </row>
     <row r="53" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="89"/>
-      <c r="C53" s="90"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="88"/>
       <c r="D53" s="55"/>
       <c r="E53" s="55"/>
       <c r="F53" s="60"/>
@@ -49456,8 +49456,8 @@
       <c r="H53" s="59"/>
     </row>
     <row r="54" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="87"/>
-      <c r="C54" s="88"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="90"/>
       <c r="D54" s="56"/>
       <c r="E54" s="56"/>
       <c r="F54" s="53"/>
@@ -49465,8 +49465,8 @@
       <c r="H54" s="58"/>
     </row>
     <row r="55" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="89"/>
-      <c r="C55" s="90"/>
+      <c r="B55" s="87"/>
+      <c r="C55" s="88"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
       <c r="F55" s="60"/>
@@ -49474,8 +49474,8 @@
       <c r="H55" s="59"/>
     </row>
     <row r="56" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="87"/>
-      <c r="C56" s="88"/>
+      <c r="B56" s="89"/>
+      <c r="C56" s="90"/>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
       <c r="F56" s="53"/>
@@ -49483,8 +49483,8 @@
       <c r="H56" s="58"/>
     </row>
     <row r="57" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="89"/>
-      <c r="C57" s="90"/>
+      <c r="B57" s="87"/>
+      <c r="C57" s="88"/>
       <c r="D57" s="55"/>
       <c r="E57" s="55"/>
       <c r="F57" s="60"/>
@@ -49492,8 +49492,8 @@
       <c r="H57" s="59"/>
     </row>
     <row r="58" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="87"/>
-      <c r="C58" s="88"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="90"/>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
       <c r="F58" s="53"/>
@@ -49501,8 +49501,8 @@
       <c r="H58" s="58"/>
     </row>
     <row r="59" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="89"/>
-      <c r="C59" s="90"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="88"/>
       <c r="D59" s="55"/>
       <c r="E59" s="55"/>
       <c r="F59" s="60"/>
@@ -49510,8 +49510,8 @@
       <c r="H59" s="59"/>
     </row>
     <row r="60" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="87"/>
-      <c r="C60" s="88"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="90"/>
       <c r="D60" s="56"/>
       <c r="E60" s="56"/>
       <c r="F60" s="53"/>
@@ -49519,8 +49519,8 @@
       <c r="H60" s="58"/>
     </row>
     <row r="61" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="89"/>
-      <c r="C61" s="90"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="88"/>
       <c r="D61" s="55"/>
       <c r="E61" s="55"/>
       <c r="F61" s="60"/>
@@ -49528,8 +49528,8 @@
       <c r="H61" s="59"/>
     </row>
     <row r="62" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="87"/>
-      <c r="C62" s="88"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="90"/>
       <c r="D62" s="56"/>
       <c r="E62" s="56"/>
       <c r="F62" s="53"/>
@@ -49537,8 +49537,8 @@
       <c r="H62" s="58"/>
     </row>
     <row r="63" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="89"/>
-      <c r="C63" s="90"/>
+      <c r="B63" s="87"/>
+      <c r="C63" s="88"/>
       <c r="D63" s="55"/>
       <c r="E63" s="55"/>
       <c r="F63" s="60"/>
@@ -49546,8 +49546,8 @@
       <c r="H63" s="59"/>
     </row>
     <row r="64" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="87"/>
-      <c r="C64" s="88"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="90"/>
       <c r="D64" s="56"/>
       <c r="E64" s="56"/>
       <c r="F64" s="53"/>
@@ -49555,8 +49555,8 @@
       <c r="H64" s="58"/>
     </row>
     <row r="65" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="89"/>
-      <c r="C65" s="90"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="88"/>
       <c r="D65" s="55"/>
       <c r="E65" s="55"/>
       <c r="F65" s="60"/>
@@ -49564,8 +49564,8 @@
       <c r="H65" s="59"/>
     </row>
     <row r="66" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="87"/>
-      <c r="C66" s="88"/>
+      <c r="B66" s="89"/>
+      <c r="C66" s="90"/>
       <c r="D66" s="56"/>
       <c r="E66" s="56"/>
       <c r="F66" s="53"/>
@@ -49573,8 +49573,8 @@
       <c r="H66" s="58"/>
     </row>
     <row r="67" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="89"/>
-      <c r="C67" s="90"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="88"/>
       <c r="D67" s="55"/>
       <c r="E67" s="55"/>
       <c r="F67" s="60"/>
@@ -49582,8 +49582,8 @@
       <c r="H67" s="59"/>
     </row>
     <row r="68" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="87"/>
-      <c r="C68" s="88"/>
+      <c r="B68" s="89"/>
+      <c r="C68" s="90"/>
       <c r="D68" s="56"/>
       <c r="E68" s="56"/>
       <c r="F68" s="53"/>
@@ -49591,8 +49591,8 @@
       <c r="H68" s="58"/>
     </row>
     <row r="69" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="89"/>
-      <c r="C69" s="90"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="88"/>
       <c r="D69" s="55"/>
       <c r="E69" s="55"/>
       <c r="F69" s="60"/>
@@ -49600,8 +49600,8 @@
       <c r="H69" s="59"/>
     </row>
     <row r="70" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="87"/>
-      <c r="C70" s="88"/>
+      <c r="B70" s="89"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="56"/>
       <c r="E70" s="56"/>
       <c r="F70" s="53"/>
@@ -49609,8 +49609,8 @@
       <c r="H70" s="58"/>
     </row>
     <row r="71" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="89"/>
-      <c r="C71" s="90"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="88"/>
       <c r="D71" s="55"/>
       <c r="E71" s="55"/>
       <c r="F71" s="60"/>
@@ -49618,8 +49618,8 @@
       <c r="H71" s="59"/>
     </row>
     <row r="72" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="87"/>
-      <c r="C72" s="88"/>
+      <c r="B72" s="89"/>
+      <c r="C72" s="90"/>
       <c r="D72" s="56"/>
       <c r="E72" s="56"/>
       <c r="F72" s="53"/>
@@ -49627,8 +49627,8 @@
       <c r="H72" s="58"/>
     </row>
     <row r="73" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="89"/>
-      <c r="C73" s="90"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="88"/>
       <c r="D73" s="55"/>
       <c r="E73" s="55"/>
       <c r="F73" s="60"/>
@@ -49636,8 +49636,8 @@
       <c r="H73" s="59"/>
     </row>
     <row r="74" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="87"/>
-      <c r="C74" s="88"/>
+      <c r="B74" s="89"/>
+      <c r="C74" s="90"/>
       <c r="D74" s="56"/>
       <c r="E74" s="56"/>
       <c r="F74" s="53"/>
@@ -49645,8 +49645,8 @@
       <c r="H74" s="58"/>
     </row>
     <row r="75" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="89"/>
-      <c r="C75" s="90"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="88"/>
       <c r="D75" s="55"/>
       <c r="E75" s="55"/>
       <c r="F75" s="60"/>
@@ -49654,8 +49654,8 @@
       <c r="H75" s="59"/>
     </row>
     <row r="76" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="87"/>
-      <c r="C76" s="88"/>
+      <c r="B76" s="89"/>
+      <c r="C76" s="90"/>
       <c r="D76" s="56"/>
       <c r="E76" s="56"/>
       <c r="F76" s="53"/>
@@ -49663,8 +49663,8 @@
       <c r="H76" s="58"/>
     </row>
     <row r="77" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="89"/>
-      <c r="C77" s="90"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="88"/>
       <c r="D77" s="55"/>
       <c r="E77" s="55"/>
       <c r="F77" s="60"/>
@@ -49672,8 +49672,8 @@
       <c r="H77" s="59"/>
     </row>
     <row r="78" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="87"/>
-      <c r="C78" s="88"/>
+      <c r="B78" s="89"/>
+      <c r="C78" s="90"/>
       <c r="D78" s="56"/>
       <c r="E78" s="56"/>
       <c r="F78" s="53"/>
@@ -49681,8 +49681,8 @@
       <c r="H78" s="58"/>
     </row>
     <row r="79" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="89"/>
-      <c r="C79" s="90"/>
+      <c r="B79" s="87"/>
+      <c r="C79" s="88"/>
       <c r="D79" s="55"/>
       <c r="E79" s="55"/>
       <c r="F79" s="60"/>
@@ -49690,8 +49690,8 @@
       <c r="H79" s="59"/>
     </row>
     <row r="80" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="87"/>
-      <c r="C80" s="88"/>
+      <c r="B80" s="89"/>
+      <c r="C80" s="90"/>
       <c r="D80" s="56"/>
       <c r="E80" s="56"/>
       <c r="F80" s="53"/>
@@ -49699,8 +49699,8 @@
       <c r="H80" s="58"/>
     </row>
     <row r="81" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="89"/>
-      <c r="C81" s="90"/>
+      <c r="B81" s="87"/>
+      <c r="C81" s="88"/>
       <c r="D81" s="55"/>
       <c r="E81" s="55"/>
       <c r="F81" s="60"/>
@@ -49708,8 +49708,8 @@
       <c r="H81" s="59"/>
     </row>
     <row r="82" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="87"/>
-      <c r="C82" s="88"/>
+      <c r="B82" s="89"/>
+      <c r="C82" s="90"/>
       <c r="D82" s="56"/>
       <c r="E82" s="56"/>
       <c r="F82" s="53"/>
@@ -49717,8 +49717,8 @@
       <c r="H82" s="58"/>
     </row>
     <row r="83" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="89"/>
-      <c r="C83" s="90"/>
+      <c r="B83" s="87"/>
+      <c r="C83" s="88"/>
       <c r="D83" s="55"/>
       <c r="E83" s="55"/>
       <c r="F83" s="60"/>
@@ -49726,8 +49726,8 @@
       <c r="H83" s="59"/>
     </row>
     <row r="84" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="87"/>
-      <c r="C84" s="88"/>
+      <c r="B84" s="89"/>
+      <c r="C84" s="90"/>
       <c r="D84" s="56"/>
       <c r="E84" s="56"/>
       <c r="F84" s="53"/>
@@ -49735,8 +49735,8 @@
       <c r="H84" s="58"/>
     </row>
     <row r="85" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="89"/>
-      <c r="C85" s="90"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="88"/>
       <c r="D85" s="55"/>
       <c r="E85" s="55"/>
       <c r="F85" s="60"/>
@@ -49744,8 +49744,8 @@
       <c r="H85" s="59"/>
     </row>
     <row r="86" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="87"/>
-      <c r="C86" s="88"/>
+      <c r="B86" s="89"/>
+      <c r="C86" s="90"/>
       <c r="D86" s="56"/>
       <c r="E86" s="56"/>
       <c r="F86" s="53"/>
@@ -49753,8 +49753,8 @@
       <c r="H86" s="58"/>
     </row>
     <row r="87" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="89"/>
-      <c r="C87" s="90"/>
+      <c r="B87" s="87"/>
+      <c r="C87" s="88"/>
       <c r="D87" s="55"/>
       <c r="E87" s="55"/>
       <c r="F87" s="60"/>
@@ -49762,8 +49762,8 @@
       <c r="H87" s="59"/>
     </row>
     <row r="88" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="87"/>
-      <c r="C88" s="88"/>
+      <c r="B88" s="89"/>
+      <c r="C88" s="90"/>
       <c r="D88" s="56"/>
       <c r="E88" s="56"/>
       <c r="F88" s="53"/>
@@ -49771,8 +49771,8 @@
       <c r="H88" s="58"/>
     </row>
     <row r="89" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="89"/>
-      <c r="C89" s="90"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="88"/>
       <c r="D89" s="55"/>
       <c r="E89" s="55"/>
       <c r="F89" s="60"/>
@@ -49780,8 +49780,8 @@
       <c r="H89" s="59"/>
     </row>
     <row r="90" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="87"/>
-      <c r="C90" s="88"/>
+      <c r="B90" s="89"/>
+      <c r="C90" s="90"/>
       <c r="D90" s="56"/>
       <c r="E90" s="56"/>
       <c r="F90" s="53"/>
@@ -49789,8 +49789,8 @@
       <c r="H90" s="58"/>
     </row>
     <row r="91" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="89"/>
-      <c r="C91" s="90"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="88"/>
       <c r="D91" s="55"/>
       <c r="E91" s="55"/>
       <c r="F91" s="60"/>
@@ -49798,8 +49798,8 @@
       <c r="H91" s="59"/>
     </row>
     <row r="92" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="87"/>
-      <c r="C92" s="88"/>
+      <c r="B92" s="89"/>
+      <c r="C92" s="90"/>
       <c r="D92" s="56"/>
       <c r="E92" s="56"/>
       <c r="F92" s="53"/>
@@ -49807,8 +49807,8 @@
       <c r="H92" s="58"/>
     </row>
     <row r="93" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="89"/>
-      <c r="C93" s="90"/>
+      <c r="B93" s="87"/>
+      <c r="C93" s="88"/>
       <c r="D93" s="55"/>
       <c r="E93" s="55"/>
       <c r="F93" s="60"/>
@@ -49816,8 +49816,8 @@
       <c r="H93" s="59"/>
     </row>
     <row r="94" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="87"/>
-      <c r="C94" s="88"/>
+      <c r="B94" s="89"/>
+      <c r="C94" s="90"/>
       <c r="D94" s="56"/>
       <c r="E94" s="56"/>
       <c r="F94" s="53"/>
@@ -49825,8 +49825,8 @@
       <c r="H94" s="58"/>
     </row>
     <row r="95" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="89"/>
-      <c r="C95" s="90"/>
+      <c r="B95" s="87"/>
+      <c r="C95" s="88"/>
       <c r="D95" s="55"/>
       <c r="E95" s="55"/>
       <c r="F95" s="60"/>
@@ -49834,8 +49834,8 @@
       <c r="H95" s="59"/>
     </row>
     <row r="96" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="87"/>
-      <c r="C96" s="88"/>
+      <c r="B96" s="89"/>
+      <c r="C96" s="90"/>
       <c r="D96" s="56"/>
       <c r="E96" s="56"/>
       <c r="F96" s="53"/>
@@ -49843,8 +49843,8 @@
       <c r="H96" s="58"/>
     </row>
     <row r="97" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="89"/>
-      <c r="C97" s="90"/>
+      <c r="B97" s="87"/>
+      <c r="C97" s="88"/>
       <c r="D97" s="55"/>
       <c r="E97" s="55"/>
       <c r="F97" s="60"/>
@@ -49852,8 +49852,8 @@
       <c r="H97" s="59"/>
     </row>
     <row r="98" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="87"/>
-      <c r="C98" s="88"/>
+      <c r="B98" s="89"/>
+      <c r="C98" s="90"/>
       <c r="D98" s="56"/>
       <c r="E98" s="56"/>
       <c r="F98" s="53"/>
@@ -49861,8 +49861,8 @@
       <c r="H98" s="58"/>
     </row>
     <row r="99" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="89"/>
-      <c r="C99" s="90"/>
+      <c r="B99" s="87"/>
+      <c r="C99" s="88"/>
       <c r="D99" s="55"/>
       <c r="E99" s="55"/>
       <c r="F99" s="60"/>
@@ -49870,8 +49870,8 @@
       <c r="H99" s="59"/>
     </row>
     <row r="100" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="87"/>
-      <c r="C100" s="88"/>
+      <c r="B100" s="89"/>
+      <c r="C100" s="90"/>
       <c r="D100" s="56"/>
       <c r="E100" s="56"/>
       <c r="F100" s="53"/>
@@ -49879,8 +49879,8 @@
       <c r="H100" s="58"/>
     </row>
     <row r="101" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="89"/>
-      <c r="C101" s="90"/>
+      <c r="B101" s="87"/>
+      <c r="C101" s="88"/>
       <c r="D101" s="55"/>
       <c r="E101" s="55"/>
       <c r="F101" s="60"/>
@@ -49888,8 +49888,8 @@
       <c r="H101" s="59"/>
     </row>
     <row r="102" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="87"/>
-      <c r="C102" s="88"/>
+      <c r="B102" s="89"/>
+      <c r="C102" s="90"/>
       <c r="D102" s="56"/>
       <c r="E102" s="56"/>
       <c r="F102" s="53"/>
@@ -49897,8 +49897,8 @@
       <c r="H102" s="58"/>
     </row>
     <row r="103" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="89"/>
-      <c r="C103" s="90"/>
+      <c r="B103" s="87"/>
+      <c r="C103" s="88"/>
       <c r="D103" s="55"/>
       <c r="E103" s="55"/>
       <c r="F103" s="60"/>
@@ -49906,8 +49906,8 @@
       <c r="H103" s="59"/>
     </row>
     <row r="104" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="87"/>
-      <c r="C104" s="88"/>
+      <c r="B104" s="89"/>
+      <c r="C104" s="90"/>
       <c r="D104" s="56"/>
       <c r="E104" s="56"/>
       <c r="F104" s="53"/>
@@ -49915,8 +49915,8 @@
       <c r="H104" s="58"/>
     </row>
     <row r="105" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="89"/>
-      <c r="C105" s="90"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="88"/>
       <c r="D105" s="55"/>
       <c r="E105" s="55"/>
       <c r="F105" s="60"/>
@@ -49924,8 +49924,8 @@
       <c r="H105" s="59"/>
     </row>
     <row r="106" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="87"/>
-      <c r="C106" s="88"/>
+      <c r="B106" s="89"/>
+      <c r="C106" s="90"/>
       <c r="D106" s="56"/>
       <c r="E106" s="56"/>
       <c r="F106" s="53"/>
@@ -49933,8 +49933,8 @@
       <c r="H106" s="58"/>
     </row>
     <row r="107" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="89"/>
-      <c r="C107" s="90"/>
+      <c r="B107" s="87"/>
+      <c r="C107" s="88"/>
       <c r="D107" s="55"/>
       <c r="E107" s="55"/>
       <c r="F107" s="60"/>
@@ -49942,8 +49942,8 @@
       <c r="H107" s="59"/>
     </row>
     <row r="108" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="87"/>
-      <c r="C108" s="88"/>
+      <c r="B108" s="89"/>
+      <c r="C108" s="90"/>
       <c r="D108" s="56"/>
       <c r="E108" s="56"/>
       <c r="F108" s="53"/>
@@ -49951,8 +49951,8 @@
       <c r="H108" s="58"/>
     </row>
     <row r="109" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="89"/>
-      <c r="C109" s="90"/>
+      <c r="B109" s="87"/>
+      <c r="C109" s="88"/>
       <c r="D109" s="55"/>
       <c r="E109" s="55"/>
       <c r="F109" s="60"/>
@@ -49960,8 +49960,8 @@
       <c r="H109" s="59"/>
     </row>
     <row r="110" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="87"/>
-      <c r="C110" s="88"/>
+      <c r="B110" s="89"/>
+      <c r="C110" s="90"/>
       <c r="D110" s="56"/>
       <c r="E110" s="56"/>
       <c r="F110" s="53"/>
@@ -49969,8 +49969,8 @@
       <c r="H110" s="58"/>
     </row>
     <row r="111" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="89"/>
-      <c r="C111" s="90"/>
+      <c r="B111" s="87"/>
+      <c r="C111" s="88"/>
       <c r="D111" s="55"/>
       <c r="E111" s="55"/>
       <c r="F111" s="60"/>
@@ -49978,8 +49978,8 @@
       <c r="H111" s="59"/>
     </row>
     <row r="112" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="87"/>
-      <c r="C112" s="88"/>
+      <c r="B112" s="89"/>
+      <c r="C112" s="90"/>
       <c r="D112" s="56"/>
       <c r="E112" s="56"/>
       <c r="F112" s="53"/>
@@ -49987,8 +49987,8 @@
       <c r="H112" s="58"/>
     </row>
     <row r="113" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="89"/>
-      <c r="C113" s="90"/>
+      <c r="B113" s="87"/>
+      <c r="C113" s="88"/>
       <c r="D113" s="55"/>
       <c r="E113" s="55"/>
       <c r="F113" s="60"/>
@@ -49996,8 +49996,8 @@
       <c r="H113" s="59"/>
     </row>
     <row r="114" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B114" s="87"/>
-      <c r="C114" s="88"/>
+      <c r="B114" s="89"/>
+      <c r="C114" s="90"/>
       <c r="D114" s="56"/>
       <c r="E114" s="56"/>
       <c r="F114" s="53"/>
@@ -50005,8 +50005,8 @@
       <c r="H114" s="58"/>
     </row>
     <row r="115" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="89"/>
-      <c r="C115" s="90"/>
+      <c r="B115" s="87"/>
+      <c r="C115" s="88"/>
       <c r="D115" s="55"/>
       <c r="E115" s="55"/>
       <c r="F115" s="60"/>
@@ -50014,8 +50014,8 @@
       <c r="H115" s="59"/>
     </row>
     <row r="116" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B116" s="87"/>
-      <c r="C116" s="88"/>
+      <c r="B116" s="89"/>
+      <c r="C116" s="90"/>
       <c r="D116" s="56"/>
       <c r="E116" s="56"/>
       <c r="F116" s="53"/>
@@ -50023,8 +50023,8 @@
       <c r="H116" s="58"/>
     </row>
     <row r="117" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B117" s="89"/>
-      <c r="C117" s="90"/>
+      <c r="B117" s="87"/>
+      <c r="C117" s="88"/>
       <c r="D117" s="55"/>
       <c r="E117" s="55"/>
       <c r="F117" s="60"/>
@@ -50032,8 +50032,8 @@
       <c r="H117" s="59"/>
     </row>
     <row r="118" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="87"/>
-      <c r="C118" s="88"/>
+      <c r="B118" s="89"/>
+      <c r="C118" s="90"/>
       <c r="D118" s="56"/>
       <c r="E118" s="56"/>
       <c r="F118" s="53"/>
@@ -50041,8 +50041,8 @@
       <c r="H118" s="58"/>
     </row>
     <row r="119" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B119" s="89"/>
-      <c r="C119" s="90"/>
+      <c r="B119" s="87"/>
+      <c r="C119" s="88"/>
       <c r="D119" s="55"/>
       <c r="E119" s="55"/>
       <c r="F119" s="60"/>
@@ -50050,8 +50050,8 @@
       <c r="H119" s="59"/>
     </row>
     <row r="120" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B120" s="87"/>
-      <c r="C120" s="88"/>
+      <c r="B120" s="89"/>
+      <c r="C120" s="90"/>
       <c r="D120" s="56"/>
       <c r="E120" s="56"/>
       <c r="F120" s="53"/>
@@ -50059,8 +50059,8 @@
       <c r="H120" s="58"/>
     </row>
     <row r="121" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="89"/>
-      <c r="C121" s="90"/>
+      <c r="B121" s="87"/>
+      <c r="C121" s="88"/>
       <c r="D121" s="55"/>
       <c r="E121" s="55"/>
       <c r="F121" s="60"/>
@@ -50068,8 +50068,8 @@
       <c r="H121" s="59"/>
     </row>
     <row r="122" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="87"/>
-      <c r="C122" s="88"/>
+      <c r="B122" s="89"/>
+      <c r="C122" s="90"/>
       <c r="D122" s="56"/>
       <c r="E122" s="56"/>
       <c r="F122" s="53"/>
@@ -50077,8 +50077,8 @@
       <c r="H122" s="58"/>
     </row>
     <row r="123" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="89"/>
-      <c r="C123" s="90"/>
+      <c r="B123" s="87"/>
+      <c r="C123" s="88"/>
       <c r="D123" s="55"/>
       <c r="E123" s="55"/>
       <c r="F123" s="60"/>
@@ -50086,8 +50086,8 @@
       <c r="H123" s="59"/>
     </row>
     <row r="124" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="87"/>
-      <c r="C124" s="88"/>
+      <c r="B124" s="89"/>
+      <c r="C124" s="90"/>
       <c r="D124" s="56"/>
       <c r="E124" s="56"/>
       <c r="F124" s="53"/>
@@ -50095,8 +50095,8 @@
       <c r="H124" s="58"/>
     </row>
     <row r="125" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="89"/>
-      <c r="C125" s="90"/>
+      <c r="B125" s="87"/>
+      <c r="C125" s="88"/>
       <c r="D125" s="55"/>
       <c r="E125" s="55"/>
       <c r="F125" s="60"/>
@@ -50104,8 +50104,8 @@
       <c r="H125" s="59"/>
     </row>
     <row r="126" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B126" s="87"/>
-      <c r="C126" s="88"/>
+      <c r="B126" s="89"/>
+      <c r="C126" s="90"/>
       <c r="D126" s="56"/>
       <c r="E126" s="56"/>
       <c r="F126" s="53"/>
@@ -50113,8 +50113,8 @@
       <c r="H126" s="58"/>
     </row>
     <row r="127" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="89"/>
-      <c r="C127" s="90"/>
+      <c r="B127" s="87"/>
+      <c r="C127" s="88"/>
       <c r="D127" s="55"/>
       <c r="E127" s="55"/>
       <c r="F127" s="60"/>
@@ -50122,8 +50122,8 @@
       <c r="H127" s="59"/>
     </row>
     <row r="128" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="87"/>
-      <c r="C128" s="88"/>
+      <c r="B128" s="89"/>
+      <c r="C128" s="90"/>
       <c r="D128" s="56"/>
       <c r="E128" s="56"/>
       <c r="F128" s="53"/>
@@ -50131,8 +50131,8 @@
       <c r="H128" s="58"/>
     </row>
     <row r="129" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B129" s="89"/>
-      <c r="C129" s="90"/>
+      <c r="B129" s="87"/>
+      <c r="C129" s="88"/>
       <c r="D129" s="55"/>
       <c r="E129" s="55"/>
       <c r="F129" s="60"/>
@@ -50140,8 +50140,8 @@
       <c r="H129" s="59"/>
     </row>
     <row r="130" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B130" s="87"/>
-      <c r="C130" s="88"/>
+      <c r="B130" s="89"/>
+      <c r="C130" s="90"/>
       <c r="D130" s="56"/>
       <c r="E130" s="56"/>
       <c r="F130" s="53"/>
@@ -50149,8 +50149,8 @@
       <c r="H130" s="58"/>
     </row>
     <row r="131" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B131" s="89"/>
-      <c r="C131" s="90"/>
+      <c r="B131" s="87"/>
+      <c r="C131" s="88"/>
       <c r="D131" s="55"/>
       <c r="E131" s="55"/>
       <c r="F131" s="60"/>
@@ -50158,8 +50158,8 @@
       <c r="H131" s="59"/>
     </row>
     <row r="132" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="87"/>
-      <c r="C132" s="88"/>
+      <c r="B132" s="89"/>
+      <c r="C132" s="90"/>
       <c r="D132" s="56"/>
       <c r="E132" s="56"/>
       <c r="F132" s="53"/>
@@ -50167,8 +50167,8 @@
       <c r="H132" s="58"/>
     </row>
     <row r="133" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="89"/>
-      <c r="C133" s="90"/>
+      <c r="B133" s="87"/>
+      <c r="C133" s="88"/>
       <c r="D133" s="55"/>
       <c r="E133" s="55"/>
       <c r="F133" s="60"/>
@@ -50176,8 +50176,8 @@
       <c r="H133" s="59"/>
     </row>
     <row r="134" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="87"/>
-      <c r="C134" s="88"/>
+      <c r="B134" s="89"/>
+      <c r="C134" s="90"/>
       <c r="D134" s="56"/>
       <c r="E134" s="56"/>
       <c r="F134" s="53"/>
@@ -50185,8 +50185,8 @@
       <c r="H134" s="58"/>
     </row>
     <row r="135" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B135" s="89"/>
-      <c r="C135" s="90"/>
+      <c r="B135" s="87"/>
+      <c r="C135" s="88"/>
       <c r="D135" s="55"/>
       <c r="E135" s="55"/>
       <c r="F135" s="60"/>
@@ -50194,8 +50194,8 @@
       <c r="H135" s="59"/>
     </row>
     <row r="136" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="87"/>
-      <c r="C136" s="88"/>
+      <c r="B136" s="89"/>
+      <c r="C136" s="90"/>
       <c r="D136" s="56"/>
       <c r="E136" s="56"/>
       <c r="F136" s="53"/>
@@ -50203,8 +50203,8 @@
       <c r="H136" s="58"/>
     </row>
     <row r="137" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="89"/>
-      <c r="C137" s="90"/>
+      <c r="B137" s="87"/>
+      <c r="C137" s="88"/>
       <c r="D137" s="55"/>
       <c r="E137" s="55"/>
       <c r="F137" s="60"/>
@@ -50212,8 +50212,8 @@
       <c r="H137" s="59"/>
     </row>
     <row r="138" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B138" s="87"/>
-      <c r="C138" s="88"/>
+      <c r="B138" s="89"/>
+      <c r="C138" s="90"/>
       <c r="D138" s="56"/>
       <c r="E138" s="56"/>
       <c r="F138" s="53"/>
@@ -50221,8 +50221,8 @@
       <c r="H138" s="58"/>
     </row>
     <row r="139" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B139" s="89"/>
-      <c r="C139" s="90"/>
+      <c r="B139" s="87"/>
+      <c r="C139" s="88"/>
       <c r="D139" s="55"/>
       <c r="E139" s="55"/>
       <c r="F139" s="60"/>
@@ -50230,8 +50230,8 @@
       <c r="H139" s="59"/>
     </row>
     <row r="140" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B140" s="87"/>
-      <c r="C140" s="88"/>
+      <c r="B140" s="89"/>
+      <c r="C140" s="90"/>
       <c r="D140" s="56"/>
       <c r="E140" s="56"/>
       <c r="F140" s="53"/>
@@ -50239,8 +50239,8 @@
       <c r="H140" s="58"/>
     </row>
     <row r="141" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B141" s="89"/>
-      <c r="C141" s="90"/>
+      <c r="B141" s="87"/>
+      <c r="C141" s="88"/>
       <c r="D141" s="55"/>
       <c r="E141" s="55"/>
       <c r="F141" s="60"/>
@@ -50248,8 +50248,8 @@
       <c r="H141" s="59"/>
     </row>
     <row r="142" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="87"/>
-      <c r="C142" s="88"/>
+      <c r="B142" s="89"/>
+      <c r="C142" s="90"/>
       <c r="D142" s="56"/>
       <c r="E142" s="56"/>
       <c r="F142" s="53"/>
@@ -50257,8 +50257,8 @@
       <c r="H142" s="58"/>
     </row>
     <row r="143" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B143" s="89"/>
-      <c r="C143" s="90"/>
+      <c r="B143" s="87"/>
+      <c r="C143" s="88"/>
       <c r="D143" s="55"/>
       <c r="E143" s="55"/>
       <c r="F143" s="60"/>
@@ -50266,8 +50266,8 @@
       <c r="H143" s="59"/>
     </row>
     <row r="144" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B144" s="87"/>
-      <c r="C144" s="88"/>
+      <c r="B144" s="89"/>
+      <c r="C144" s="90"/>
       <c r="D144" s="56"/>
       <c r="E144" s="56"/>
       <c r="F144" s="53"/>
@@ -50275,8 +50275,8 @@
       <c r="H144" s="58"/>
     </row>
     <row r="145" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B145" s="89"/>
-      <c r="C145" s="90"/>
+      <c r="B145" s="87"/>
+      <c r="C145" s="88"/>
       <c r="D145" s="55"/>
       <c r="E145" s="55"/>
       <c r="F145" s="60"/>
@@ -50284,8 +50284,8 @@
       <c r="H145" s="59"/>
     </row>
     <row r="146" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B146" s="87"/>
-      <c r="C146" s="88"/>
+      <c r="B146" s="89"/>
+      <c r="C146" s="90"/>
       <c r="D146" s="56"/>
       <c r="E146" s="56"/>
       <c r="F146" s="53"/>
@@ -50293,8 +50293,8 @@
       <c r="H146" s="58"/>
     </row>
     <row r="147" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B147" s="89"/>
-      <c r="C147" s="90"/>
+      <c r="B147" s="87"/>
+      <c r="C147" s="88"/>
       <c r="D147" s="55"/>
       <c r="E147" s="55"/>
       <c r="F147" s="60"/>
@@ -50302,8 +50302,8 @@
       <c r="H147" s="59"/>
     </row>
     <row r="148" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="87"/>
-      <c r="C148" s="88"/>
+      <c r="B148" s="89"/>
+      <c r="C148" s="90"/>
       <c r="D148" s="56"/>
       <c r="E148" s="56"/>
       <c r="F148" s="53"/>
@@ -50311,8 +50311,8 @@
       <c r="H148" s="58"/>
     </row>
     <row r="149" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B149" s="89"/>
-      <c r="C149" s="90"/>
+      <c r="B149" s="87"/>
+      <c r="C149" s="88"/>
       <c r="D149" s="55"/>
       <c r="E149" s="55"/>
       <c r="F149" s="60"/>
@@ -50320,8 +50320,8 @@
       <c r="H149" s="59"/>
     </row>
     <row r="150" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B150" s="87"/>
-      <c r="C150" s="88"/>
+      <c r="B150" s="89"/>
+      <c r="C150" s="90"/>
       <c r="D150" s="56"/>
       <c r="E150" s="56"/>
       <c r="F150" s="53"/>
@@ -50329,8 +50329,8 @@
       <c r="H150" s="58"/>
     </row>
     <row r="151" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="89"/>
-      <c r="C151" s="90"/>
+      <c r="B151" s="87"/>
+      <c r="C151" s="88"/>
       <c r="D151" s="55"/>
       <c r="E151" s="55"/>
       <c r="F151" s="60"/>
@@ -50338,8 +50338,8 @@
       <c r="H151" s="59"/>
     </row>
     <row r="152" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B152" s="87"/>
-      <c r="C152" s="88"/>
+      <c r="B152" s="89"/>
+      <c r="C152" s="90"/>
       <c r="D152" s="56"/>
       <c r="E152" s="56"/>
       <c r="F152" s="53"/>
@@ -50347,8 +50347,8 @@
       <c r="H152" s="58"/>
     </row>
     <row r="153" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B153" s="89"/>
-      <c r="C153" s="90"/>
+      <c r="B153" s="87"/>
+      <c r="C153" s="88"/>
       <c r="D153" s="55"/>
       <c r="E153" s="55"/>
       <c r="F153" s="60"/>
@@ -50356,8 +50356,8 @@
       <c r="H153" s="59"/>
     </row>
     <row r="154" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="87"/>
-      <c r="C154" s="88"/>
+      <c r="B154" s="89"/>
+      <c r="C154" s="90"/>
       <c r="D154" s="56"/>
       <c r="E154" s="56"/>
       <c r="F154" s="53"/>
@@ -50365,8 +50365,8 @@
       <c r="H154" s="58"/>
     </row>
     <row r="155" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B155" s="89"/>
-      <c r="C155" s="90"/>
+      <c r="B155" s="87"/>
+      <c r="C155" s="88"/>
       <c r="D155" s="55"/>
       <c r="E155" s="55"/>
       <c r="F155" s="60"/>
@@ -50374,8 +50374,8 @@
       <c r="H155" s="59"/>
     </row>
     <row r="156" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B156" s="87"/>
-      <c r="C156" s="88"/>
+      <c r="B156" s="89"/>
+      <c r="C156" s="90"/>
       <c r="D156" s="56"/>
       <c r="E156" s="56"/>
       <c r="F156" s="53"/>
@@ -50383,8 +50383,8 @@
       <c r="H156" s="58"/>
     </row>
     <row r="157" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B157" s="89"/>
-      <c r="C157" s="90"/>
+      <c r="B157" s="87"/>
+      <c r="C157" s="88"/>
       <c r="D157" s="55"/>
       <c r="E157" s="55"/>
       <c r="F157" s="60"/>
@@ -50392,8 +50392,8 @@
       <c r="H157" s="59"/>
     </row>
     <row r="158" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B158" s="87"/>
-      <c r="C158" s="88"/>
+      <c r="B158" s="89"/>
+      <c r="C158" s="90"/>
       <c r="D158" s="56"/>
       <c r="E158" s="56"/>
       <c r="F158" s="53"/>
@@ -50401,8 +50401,8 @@
       <c r="H158" s="58"/>
     </row>
     <row r="159" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B159" s="89"/>
-      <c r="C159" s="90"/>
+      <c r="B159" s="87"/>
+      <c r="C159" s="88"/>
       <c r="D159" s="55"/>
       <c r="E159" s="55"/>
       <c r="F159" s="60"/>
@@ -50410,8 +50410,8 @@
       <c r="H159" s="59"/>
     </row>
     <row r="160" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B160" s="87"/>
-      <c r="C160" s="88"/>
+      <c r="B160" s="89"/>
+      <c r="C160" s="90"/>
       <c r="D160" s="56"/>
       <c r="E160" s="56"/>
       <c r="F160" s="53"/>
@@ -50419,8 +50419,8 @@
       <c r="H160" s="58"/>
     </row>
     <row r="161" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B161" s="89"/>
-      <c r="C161" s="90"/>
+      <c r="B161" s="87"/>
+      <c r="C161" s="88"/>
       <c r="D161" s="55"/>
       <c r="E161" s="55"/>
       <c r="F161" s="60"/>
@@ -50428,8 +50428,8 @@
       <c r="H161" s="59"/>
     </row>
     <row r="162" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B162" s="87"/>
-      <c r="C162" s="88"/>
+      <c r="B162" s="89"/>
+      <c r="C162" s="90"/>
       <c r="D162" s="56"/>
       <c r="E162" s="56"/>
       <c r="F162" s="53"/>
@@ -50437,8 +50437,8 @@
       <c r="H162" s="58"/>
     </row>
     <row r="163" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B163" s="89"/>
-      <c r="C163" s="90"/>
+      <c r="B163" s="87"/>
+      <c r="C163" s="88"/>
       <c r="D163" s="55"/>
       <c r="E163" s="55"/>
       <c r="F163" s="60"/>
@@ -50446,8 +50446,8 @@
       <c r="H163" s="59"/>
     </row>
     <row r="164" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="87"/>
-      <c r="C164" s="88"/>
+      <c r="B164" s="89"/>
+      <c r="C164" s="90"/>
       <c r="D164" s="56"/>
       <c r="E164" s="56"/>
       <c r="F164" s="53"/>
@@ -50455,8 +50455,8 @@
       <c r="H164" s="58"/>
     </row>
     <row r="165" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B165" s="89"/>
-      <c r="C165" s="90"/>
+      <c r="B165" s="87"/>
+      <c r="C165" s="88"/>
       <c r="D165" s="55"/>
       <c r="E165" s="55"/>
       <c r="F165" s="60"/>
@@ -50464,8 +50464,8 @@
       <c r="H165" s="59"/>
     </row>
     <row r="166" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="87"/>
-      <c r="C166" s="88"/>
+      <c r="B166" s="89"/>
+      <c r="C166" s="90"/>
       <c r="D166" s="56"/>
       <c r="E166" s="56"/>
       <c r="F166" s="53"/>
@@ -50473,8 +50473,8 @@
       <c r="H166" s="58"/>
     </row>
     <row r="167" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B167" s="89"/>
-      <c r="C167" s="90"/>
+      <c r="B167" s="87"/>
+      <c r="C167" s="88"/>
       <c r="D167" s="55"/>
       <c r="E167" s="55"/>
       <c r="F167" s="60"/>
@@ -50482,8 +50482,8 @@
       <c r="H167" s="59"/>
     </row>
     <row r="168" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B168" s="87"/>
-      <c r="C168" s="88"/>
+      <c r="B168" s="89"/>
+      <c r="C168" s="90"/>
       <c r="D168" s="56"/>
       <c r="E168" s="56"/>
       <c r="F168" s="53"/>
@@ -50491,8 +50491,8 @@
       <c r="H168" s="58"/>
     </row>
     <row r="169" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B169" s="89"/>
-      <c r="C169" s="90"/>
+      <c r="B169" s="87"/>
+      <c r="C169" s="88"/>
       <c r="D169" s="55"/>
       <c r="E169" s="55"/>
       <c r="F169" s="60"/>
@@ -50500,8 +50500,8 @@
       <c r="H169" s="59"/>
     </row>
     <row r="170" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="87"/>
-      <c r="C170" s="88"/>
+      <c r="B170" s="89"/>
+      <c r="C170" s="90"/>
       <c r="D170" s="56"/>
       <c r="E170" s="56"/>
       <c r="F170" s="53"/>
@@ -50509,8 +50509,8 @@
       <c r="H170" s="58"/>
     </row>
     <row r="171" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B171" s="89"/>
-      <c r="C171" s="90"/>
+      <c r="B171" s="87"/>
+      <c r="C171" s="88"/>
       <c r="D171" s="55"/>
       <c r="E171" s="55"/>
       <c r="F171" s="60"/>
@@ -50518,8 +50518,8 @@
       <c r="H171" s="59"/>
     </row>
     <row r="172" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B172" s="87"/>
-      <c r="C172" s="88"/>
+      <c r="B172" s="89"/>
+      <c r="C172" s="90"/>
       <c r="D172" s="56"/>
       <c r="E172" s="56"/>
       <c r="F172" s="53"/>
@@ -50527,8 +50527,8 @@
       <c r="H172" s="58"/>
     </row>
     <row r="173" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B173" s="89"/>
-      <c r="C173" s="90"/>
+      <c r="B173" s="87"/>
+      <c r="C173" s="88"/>
       <c r="D173" s="55"/>
       <c r="E173" s="55"/>
       <c r="F173" s="60"/>
@@ -50536,8 +50536,8 @@
       <c r="H173" s="59"/>
     </row>
     <row r="174" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B174" s="87"/>
-      <c r="C174" s="88"/>
+      <c r="B174" s="89"/>
+      <c r="C174" s="90"/>
       <c r="D174" s="56"/>
       <c r="E174" s="56"/>
       <c r="F174" s="53"/>
@@ -50545,8 +50545,8 @@
       <c r="H174" s="58"/>
     </row>
     <row r="175" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B175" s="89"/>
-      <c r="C175" s="90"/>
+      <c r="B175" s="87"/>
+      <c r="C175" s="88"/>
       <c r="D175" s="55"/>
       <c r="E175" s="55"/>
       <c r="F175" s="60"/>
@@ -50554,8 +50554,8 @@
       <c r="H175" s="59"/>
     </row>
     <row r="176" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B176" s="87"/>
-      <c r="C176" s="88"/>
+      <c r="B176" s="89"/>
+      <c r="C176" s="90"/>
       <c r="D176" s="56"/>
       <c r="E176" s="56"/>
       <c r="F176" s="53"/>
@@ -50563,8 +50563,8 @@
       <c r="H176" s="58"/>
     </row>
     <row r="177" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B177" s="89"/>
-      <c r="C177" s="90"/>
+      <c r="B177" s="87"/>
+      <c r="C177" s="88"/>
       <c r="D177" s="55"/>
       <c r="E177" s="55"/>
       <c r="F177" s="60"/>
@@ -50572,8 +50572,8 @@
       <c r="H177" s="59"/>
     </row>
     <row r="178" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B178" s="87"/>
-      <c r="C178" s="88"/>
+      <c r="B178" s="89"/>
+      <c r="C178" s="90"/>
       <c r="D178" s="56"/>
       <c r="E178" s="56"/>
       <c r="F178" s="53"/>
@@ -50581,8 +50581,8 @@
       <c r="H178" s="58"/>
     </row>
     <row r="179" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B179" s="89"/>
-      <c r="C179" s="90"/>
+      <c r="B179" s="87"/>
+      <c r="C179" s="88"/>
       <c r="D179" s="55"/>
       <c r="E179" s="55"/>
       <c r="F179" s="60"/>
@@ -50590,8 +50590,8 @@
       <c r="H179" s="59"/>
     </row>
     <row r="180" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B180" s="87"/>
-      <c r="C180" s="88"/>
+      <c r="B180" s="89"/>
+      <c r="C180" s="90"/>
       <c r="D180" s="56"/>
       <c r="E180" s="56"/>
       <c r="F180" s="53"/>
@@ -50599,8 +50599,8 @@
       <c r="H180" s="58"/>
     </row>
     <row r="181" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B181" s="89"/>
-      <c r="C181" s="90"/>
+      <c r="B181" s="87"/>
+      <c r="C181" s="88"/>
       <c r="D181" s="55"/>
       <c r="E181" s="55"/>
       <c r="F181" s="60"/>
@@ -50608,8 +50608,8 @@
       <c r="H181" s="59"/>
     </row>
     <row r="182" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B182" s="87"/>
-      <c r="C182" s="88"/>
+      <c r="B182" s="89"/>
+      <c r="C182" s="90"/>
       <c r="D182" s="56"/>
       <c r="E182" s="56"/>
       <c r="F182" s="53"/>
@@ -50617,8 +50617,8 @@
       <c r="H182" s="58"/>
     </row>
     <row r="183" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B183" s="89"/>
-      <c r="C183" s="90"/>
+      <c r="B183" s="87"/>
+      <c r="C183" s="88"/>
       <c r="D183" s="55"/>
       <c r="E183" s="55"/>
       <c r="F183" s="60"/>
@@ -50626,8 +50626,8 @@
       <c r="H183" s="59"/>
     </row>
     <row r="184" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B184" s="87"/>
-      <c r="C184" s="88"/>
+      <c r="B184" s="89"/>
+      <c r="C184" s="90"/>
       <c r="D184" s="56"/>
       <c r="E184" s="56"/>
       <c r="F184" s="53"/>
@@ -50635,8 +50635,8 @@
       <c r="H184" s="58"/>
     </row>
     <row r="185" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B185" s="89"/>
-      <c r="C185" s="90"/>
+      <c r="B185" s="87"/>
+      <c r="C185" s="88"/>
       <c r="D185" s="55"/>
       <c r="E185" s="55"/>
       <c r="F185" s="60"/>
@@ -50644,8 +50644,8 @@
       <c r="H185" s="59"/>
     </row>
     <row r="186" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B186" s="87"/>
-      <c r="C186" s="88"/>
+      <c r="B186" s="89"/>
+      <c r="C186" s="90"/>
       <c r="D186" s="56"/>
       <c r="E186" s="56"/>
       <c r="F186" s="53"/>
@@ -50653,8 +50653,8 @@
       <c r="H186" s="58"/>
     </row>
     <row r="187" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B187" s="89"/>
-      <c r="C187" s="90"/>
+      <c r="B187" s="87"/>
+      <c r="C187" s="88"/>
       <c r="D187" s="55"/>
       <c r="E187" s="55"/>
       <c r="F187" s="60"/>
@@ -50662,8 +50662,8 @@
       <c r="H187" s="59"/>
     </row>
     <row r="188" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B188" s="87"/>
-      <c r="C188" s="88"/>
+      <c r="B188" s="89"/>
+      <c r="C188" s="90"/>
       <c r="D188" s="56"/>
       <c r="E188" s="56"/>
       <c r="F188" s="53"/>
@@ -50671,8 +50671,8 @@
       <c r="H188" s="58"/>
     </row>
     <row r="189" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B189" s="89"/>
-      <c r="C189" s="90"/>
+      <c r="B189" s="87"/>
+      <c r="C189" s="88"/>
       <c r="D189" s="55"/>
       <c r="E189" s="55"/>
       <c r="F189" s="60"/>
@@ -50680,8 +50680,8 @@
       <c r="H189" s="59"/>
     </row>
     <row r="190" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B190" s="87"/>
-      <c r="C190" s="88"/>
+      <c r="B190" s="89"/>
+      <c r="C190" s="90"/>
       <c r="D190" s="56"/>
       <c r="E190" s="56"/>
       <c r="F190" s="53"/>
@@ -50689,8 +50689,8 @@
       <c r="H190" s="58"/>
     </row>
     <row r="191" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B191" s="89"/>
-      <c r="C191" s="90"/>
+      <c r="B191" s="87"/>
+      <c r="C191" s="88"/>
       <c r="D191" s="55"/>
       <c r="E191" s="55"/>
       <c r="F191" s="60"/>
@@ -50698,8 +50698,8 @@
       <c r="H191" s="59"/>
     </row>
     <row r="192" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B192" s="87"/>
-      <c r="C192" s="88"/>
+      <c r="B192" s="89"/>
+      <c r="C192" s="90"/>
       <c r="D192" s="56"/>
       <c r="E192" s="56"/>
       <c r="F192" s="53"/>
@@ -50707,8 +50707,8 @@
       <c r="H192" s="58"/>
     </row>
     <row r="193" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B193" s="89"/>
-      <c r="C193" s="90"/>
+      <c r="B193" s="87"/>
+      <c r="C193" s="88"/>
       <c r="D193" s="55"/>
       <c r="E193" s="55"/>
       <c r="F193" s="60"/>
@@ -50716,8 +50716,8 @@
       <c r="H193" s="59"/>
     </row>
     <row r="194" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B194" s="87"/>
-      <c r="C194" s="88"/>
+      <c r="B194" s="89"/>
+      <c r="C194" s="90"/>
       <c r="D194" s="56"/>
       <c r="E194" s="56"/>
       <c r="F194" s="53"/>
@@ -50725,8 +50725,8 @@
       <c r="H194" s="58"/>
     </row>
     <row r="195" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B195" s="89"/>
-      <c r="C195" s="90"/>
+      <c r="B195" s="87"/>
+      <c r="C195" s="88"/>
       <c r="D195" s="55"/>
       <c r="E195" s="55"/>
       <c r="F195" s="60"/>
@@ -50734,8 +50734,8 @@
       <c r="H195" s="59"/>
     </row>
     <row r="196" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B196" s="87"/>
-      <c r="C196" s="88"/>
+      <c r="B196" s="89"/>
+      <c r="C196" s="90"/>
       <c r="D196" s="56"/>
       <c r="E196" s="56"/>
       <c r="F196" s="53"/>
@@ -50743,8 +50743,8 @@
       <c r="H196" s="58"/>
     </row>
     <row r="197" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B197" s="89"/>
-      <c r="C197" s="90"/>
+      <c r="B197" s="87"/>
+      <c r="C197" s="88"/>
       <c r="D197" s="55"/>
       <c r="E197" s="55"/>
       <c r="F197" s="60"/>
@@ -50752,8 +50752,8 @@
       <c r="H197" s="59"/>
     </row>
     <row r="198" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B198" s="87"/>
-      <c r="C198" s="88"/>
+      <c r="B198" s="89"/>
+      <c r="C198" s="90"/>
       <c r="D198" s="56"/>
       <c r="E198" s="56"/>
       <c r="F198" s="53"/>
@@ -50761,8 +50761,8 @@
       <c r="H198" s="58"/>
     </row>
     <row r="199" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B199" s="89"/>
-      <c r="C199" s="90"/>
+      <c r="B199" s="87"/>
+      <c r="C199" s="88"/>
       <c r="D199" s="55"/>
       <c r="E199" s="55"/>
       <c r="F199" s="60"/>
@@ -50770,8 +50770,8 @@
       <c r="H199" s="59"/>
     </row>
     <row r="200" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B200" s="87"/>
-      <c r="C200" s="88"/>
+      <c r="B200" s="89"/>
+      <c r="C200" s="90"/>
       <c r="D200" s="56"/>
       <c r="E200" s="56"/>
       <c r="F200" s="53"/>
@@ -50779,8 +50779,8 @@
       <c r="H200" s="58"/>
     </row>
     <row r="201" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="89"/>
-      <c r="C201" s="90"/>
+      <c r="B201" s="87"/>
+      <c r="C201" s="88"/>
       <c r="D201" s="55"/>
       <c r="E201" s="55"/>
       <c r="F201" s="60"/>
@@ -50788,8 +50788,8 @@
       <c r="H201" s="59"/>
     </row>
     <row r="202" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B202" s="87"/>
-      <c r="C202" s="88"/>
+      <c r="B202" s="89"/>
+      <c r="C202" s="90"/>
       <c r="D202" s="56"/>
       <c r="E202" s="56"/>
       <c r="F202" s="53"/>
@@ -50797,8 +50797,8 @@
       <c r="H202" s="58"/>
     </row>
     <row r="203" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B203" s="89"/>
-      <c r="C203" s="90"/>
+      <c r="B203" s="87"/>
+      <c r="C203" s="88"/>
       <c r="D203" s="55"/>
       <c r="E203" s="55"/>
       <c r="F203" s="60"/>
@@ -50806,8 +50806,8 @@
       <c r="H203" s="59"/>
     </row>
     <row r="204" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B204" s="87"/>
-      <c r="C204" s="88"/>
+      <c r="B204" s="89"/>
+      <c r="C204" s="90"/>
       <c r="D204" s="56"/>
       <c r="E204" s="56"/>
       <c r="F204" s="53"/>
@@ -50815,8 +50815,8 @@
       <c r="H204" s="58"/>
     </row>
     <row r="205" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B205" s="89"/>
-      <c r="C205" s="90"/>
+      <c r="B205" s="87"/>
+      <c r="C205" s="88"/>
       <c r="D205" s="55"/>
       <c r="E205" s="55"/>
       <c r="F205" s="60"/>
@@ -50824,8 +50824,8 @@
       <c r="H205" s="59"/>
     </row>
     <row r="206" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B206" s="87"/>
-      <c r="C206" s="88"/>
+      <c r="B206" s="89"/>
+      <c r="C206" s="90"/>
       <c r="D206" s="56"/>
       <c r="E206" s="56"/>
       <c r="F206" s="53"/>
@@ -50833,8 +50833,8 @@
       <c r="H206" s="58"/>
     </row>
     <row r="207" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B207" s="89"/>
-      <c r="C207" s="90"/>
+      <c r="B207" s="87"/>
+      <c r="C207" s="88"/>
       <c r="D207" s="55"/>
       <c r="E207" s="55"/>
       <c r="F207" s="60"/>
@@ -50842,8 +50842,8 @@
       <c r="H207" s="59"/>
     </row>
     <row r="208" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B208" s="87"/>
-      <c r="C208" s="88"/>
+      <c r="B208" s="89"/>
+      <c r="C208" s="90"/>
       <c r="D208" s="56"/>
       <c r="E208" s="56"/>
       <c r="F208" s="53"/>
@@ -50851,8 +50851,8 @@
       <c r="H208" s="58"/>
     </row>
     <row r="209" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B209" s="89"/>
-      <c r="C209" s="90"/>
+      <c r="B209" s="87"/>
+      <c r="C209" s="88"/>
       <c r="D209" s="55"/>
       <c r="E209" s="55"/>
       <c r="F209" s="60"/>
@@ -50860,8 +50860,8 @@
       <c r="H209" s="59"/>
     </row>
     <row r="210" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B210" s="87"/>
-      <c r="C210" s="88"/>
+      <c r="B210" s="89"/>
+      <c r="C210" s="90"/>
       <c r="D210" s="56"/>
       <c r="E210" s="56"/>
       <c r="F210" s="53"/>
@@ -50869,8 +50869,8 @@
       <c r="H210" s="58"/>
     </row>
     <row r="211" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B211" s="89"/>
-      <c r="C211" s="90"/>
+      <c r="B211" s="87"/>
+      <c r="C211" s="88"/>
       <c r="D211" s="55"/>
       <c r="E211" s="55"/>
       <c r="F211" s="60"/>
@@ -50878,8 +50878,8 @@
       <c r="H211" s="59"/>
     </row>
     <row r="212" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B212" s="87"/>
-      <c r="C212" s="88"/>
+      <c r="B212" s="89"/>
+      <c r="C212" s="90"/>
       <c r="D212" s="56"/>
       <c r="E212" s="56"/>
       <c r="F212" s="53"/>
@@ -50887,8 +50887,8 @@
       <c r="H212" s="58"/>
     </row>
     <row r="213" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B213" s="89"/>
-      <c r="C213" s="90"/>
+      <c r="B213" s="87"/>
+      <c r="C213" s="88"/>
       <c r="D213" s="55"/>
       <c r="E213" s="55"/>
       <c r="F213" s="60"/>
@@ -50896,8 +50896,8 @@
       <c r="H213" s="59"/>
     </row>
     <row r="214" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B214" s="87"/>
-      <c r="C214" s="88"/>
+      <c r="B214" s="89"/>
+      <c r="C214" s="90"/>
       <c r="D214" s="56"/>
       <c r="E214" s="56"/>
       <c r="F214" s="53"/>
@@ -50905,8 +50905,8 @@
       <c r="H214" s="58"/>
     </row>
     <row r="215" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B215" s="89"/>
-      <c r="C215" s="90"/>
+      <c r="B215" s="87"/>
+      <c r="C215" s="88"/>
       <c r="D215" s="55"/>
       <c r="E215" s="55"/>
       <c r="F215" s="60"/>
@@ -50914,8 +50914,8 @@
       <c r="H215" s="59"/>
     </row>
     <row r="216" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B216" s="87"/>
-      <c r="C216" s="88"/>
+      <c r="B216" s="89"/>
+      <c r="C216" s="90"/>
       <c r="D216" s="56"/>
       <c r="E216" s="56"/>
       <c r="F216" s="53"/>
@@ -50923,8 +50923,8 @@
       <c r="H216" s="58"/>
     </row>
     <row r="217" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B217" s="89"/>
-      <c r="C217" s="90"/>
+      <c r="B217" s="87"/>
+      <c r="C217" s="88"/>
       <c r="D217" s="55"/>
       <c r="E217" s="55"/>
       <c r="F217" s="60"/>
@@ -50932,8 +50932,8 @@
       <c r="H217" s="59"/>
     </row>
     <row r="218" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B218" s="87"/>
-      <c r="C218" s="88"/>
+      <c r="B218" s="89"/>
+      <c r="C218" s="90"/>
       <c r="D218" s="56"/>
       <c r="E218" s="56"/>
       <c r="F218" s="53"/>
@@ -50941,8 +50941,8 @@
       <c r="H218" s="58"/>
     </row>
     <row r="219" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="89"/>
-      <c r="C219" s="90"/>
+      <c r="B219" s="87"/>
+      <c r="C219" s="88"/>
       <c r="D219" s="55"/>
       <c r="E219" s="55"/>
       <c r="F219" s="60"/>
@@ -50950,8 +50950,8 @@
       <c r="H219" s="59"/>
     </row>
     <row r="220" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B220" s="87"/>
-      <c r="C220" s="88"/>
+      <c r="B220" s="89"/>
+      <c r="C220" s="90"/>
       <c r="D220" s="56"/>
       <c r="E220" s="56"/>
       <c r="F220" s="53"/>
@@ -50959,8 +50959,8 @@
       <c r="H220" s="58"/>
     </row>
     <row r="221" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="89"/>
-      <c r="C221" s="90"/>
+      <c r="B221" s="87"/>
+      <c r="C221" s="88"/>
       <c r="D221" s="55"/>
       <c r="E221" s="55"/>
       <c r="F221" s="60"/>
@@ -50968,8 +50968,8 @@
       <c r="H221" s="59"/>
     </row>
     <row r="222" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="87"/>
-      <c r="C222" s="88"/>
+      <c r="B222" s="89"/>
+      <c r="C222" s="90"/>
       <c r="D222" s="56"/>
       <c r="E222" s="56"/>
       <c r="F222" s="53"/>
@@ -50977,8 +50977,8 @@
       <c r="H222" s="58"/>
     </row>
     <row r="223" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="89"/>
-      <c r="C223" s="90"/>
+      <c r="B223" s="87"/>
+      <c r="C223" s="88"/>
       <c r="D223" s="55"/>
       <c r="E223" s="55"/>
       <c r="F223" s="60"/>
@@ -50986,8 +50986,8 @@
       <c r="H223" s="59"/>
     </row>
     <row r="224" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="87"/>
-      <c r="C224" s="88"/>
+      <c r="B224" s="89"/>
+      <c r="C224" s="90"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
       <c r="F224" s="53"/>
@@ -50995,8 +50995,8 @@
       <c r="H224" s="58"/>
     </row>
     <row r="225" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="89"/>
-      <c r="C225" s="90"/>
+      <c r="B225" s="87"/>
+      <c r="C225" s="88"/>
       <c r="D225" s="55"/>
       <c r="E225" s="55"/>
       <c r="F225" s="60"/>
@@ -51004,8 +51004,8 @@
       <c r="H225" s="59"/>
     </row>
     <row r="226" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="87"/>
-      <c r="C226" s="88"/>
+      <c r="B226" s="89"/>
+      <c r="C226" s="90"/>
       <c r="D226" s="56"/>
       <c r="E226" s="56"/>
       <c r="F226" s="53"/>
@@ -51013,8 +51013,8 @@
       <c r="H226" s="58"/>
     </row>
     <row r="227" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="89"/>
-      <c r="C227" s="90"/>
+      <c r="B227" s="87"/>
+      <c r="C227" s="88"/>
       <c r="D227" s="55"/>
       <c r="E227" s="55"/>
       <c r="F227" s="60"/>
@@ -51022,8 +51022,8 @@
       <c r="H227" s="59"/>
     </row>
     <row r="228" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="87"/>
-      <c r="C228" s="88"/>
+      <c r="B228" s="89"/>
+      <c r="C228" s="90"/>
       <c r="D228" s="56"/>
       <c r="E228" s="56"/>
       <c r="F228" s="53"/>
@@ -51031,8 +51031,8 @@
       <c r="H228" s="58"/>
     </row>
     <row r="229" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="89"/>
-      <c r="C229" s="90"/>
+      <c r="B229" s="87"/>
+      <c r="C229" s="88"/>
       <c r="D229" s="55"/>
       <c r="E229" s="55"/>
       <c r="F229" s="60"/>
@@ -51040,8 +51040,8 @@
       <c r="H229" s="59"/>
     </row>
     <row r="230" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="87"/>
-      <c r="C230" s="88"/>
+      <c r="B230" s="89"/>
+      <c r="C230" s="90"/>
       <c r="D230" s="56"/>
       <c r="E230" s="56"/>
       <c r="F230" s="53"/>
@@ -51049,8 +51049,8 @@
       <c r="H230" s="58"/>
     </row>
     <row r="231" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="89"/>
-      <c r="C231" s="90"/>
+      <c r="B231" s="87"/>
+      <c r="C231" s="88"/>
       <c r="D231" s="55"/>
       <c r="E231" s="55"/>
       <c r="F231" s="60"/>
@@ -51058,8 +51058,8 @@
       <c r="H231" s="59"/>
     </row>
     <row r="232" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="87"/>
-      <c r="C232" s="88"/>
+      <c r="B232" s="89"/>
+      <c r="C232" s="90"/>
       <c r="D232" s="56"/>
       <c r="E232" s="56"/>
       <c r="F232" s="53"/>
@@ -51067,8 +51067,8 @@
       <c r="H232" s="58"/>
     </row>
     <row r="233" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="89"/>
-      <c r="C233" s="90"/>
+      <c r="B233" s="87"/>
+      <c r="C233" s="88"/>
       <c r="D233" s="55"/>
       <c r="E233" s="55"/>
       <c r="F233" s="60"/>
@@ -51076,8 +51076,8 @@
       <c r="H233" s="59"/>
     </row>
     <row r="234" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B234" s="87"/>
-      <c r="C234" s="88"/>
+      <c r="B234" s="89"/>
+      <c r="C234" s="90"/>
       <c r="D234" s="56"/>
       <c r="E234" s="56"/>
       <c r="F234" s="53"/>
@@ -51085,8 +51085,8 @@
       <c r="H234" s="58"/>
     </row>
     <row r="235" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B235" s="89"/>
-      <c r="C235" s="90"/>
+      <c r="B235" s="87"/>
+      <c r="C235" s="88"/>
       <c r="D235" s="55"/>
       <c r="E235" s="55"/>
       <c r="F235" s="60"/>
@@ -51094,8 +51094,8 @@
       <c r="H235" s="59"/>
     </row>
     <row r="236" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B236" s="87"/>
-      <c r="C236" s="88"/>
+      <c r="B236" s="89"/>
+      <c r="C236" s="90"/>
       <c r="D236" s="56"/>
       <c r="E236" s="56"/>
       <c r="F236" s="53"/>
@@ -51103,8 +51103,8 @@
       <c r="H236" s="58"/>
     </row>
     <row r="237" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="89"/>
-      <c r="C237" s="90"/>
+      <c r="B237" s="87"/>
+      <c r="C237" s="88"/>
       <c r="D237" s="55"/>
       <c r="E237" s="55"/>
       <c r="F237" s="60"/>
@@ -51112,8 +51112,8 @@
       <c r="H237" s="59"/>
     </row>
     <row r="238" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="87"/>
-      <c r="C238" s="88"/>
+      <c r="B238" s="89"/>
+      <c r="C238" s="90"/>
       <c r="D238" s="56"/>
       <c r="E238" s="56"/>
       <c r="F238" s="53"/>
@@ -51121,8 +51121,8 @@
       <c r="H238" s="58"/>
     </row>
     <row r="239" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="89"/>
-      <c r="C239" s="90"/>
+      <c r="B239" s="87"/>
+      <c r="C239" s="88"/>
       <c r="D239" s="55"/>
       <c r="E239" s="55"/>
       <c r="F239" s="60"/>
@@ -51130,8 +51130,8 @@
       <c r="H239" s="59"/>
     </row>
     <row r="240" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B240" s="87"/>
-      <c r="C240" s="88"/>
+      <c r="B240" s="89"/>
+      <c r="C240" s="90"/>
       <c r="D240" s="56"/>
       <c r="E240" s="56"/>
       <c r="F240" s="53"/>
@@ -51139,8 +51139,8 @@
       <c r="H240" s="58"/>
     </row>
     <row r="241" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="89"/>
-      <c r="C241" s="90"/>
+      <c r="B241" s="87"/>
+      <c r="C241" s="88"/>
       <c r="D241" s="55"/>
       <c r="E241" s="55"/>
       <c r="F241" s="60"/>
@@ -51148,8 +51148,8 @@
       <c r="H241" s="59"/>
     </row>
     <row r="242" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="87"/>
-      <c r="C242" s="88"/>
+      <c r="B242" s="89"/>
+      <c r="C242" s="90"/>
       <c r="D242" s="56"/>
       <c r="E242" s="56"/>
       <c r="F242" s="53"/>
@@ -51157,8 +51157,8 @@
       <c r="H242" s="58"/>
     </row>
     <row r="243" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="89"/>
-      <c r="C243" s="90"/>
+      <c r="B243" s="87"/>
+      <c r="C243" s="88"/>
       <c r="D243" s="55"/>
       <c r="E243" s="55"/>
       <c r="F243" s="60"/>
@@ -51166,8 +51166,8 @@
       <c r="H243" s="59"/>
     </row>
     <row r="244" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="87"/>
-      <c r="C244" s="88"/>
+      <c r="B244" s="89"/>
+      <c r="C244" s="90"/>
       <c r="D244" s="56"/>
       <c r="E244" s="56"/>
       <c r="F244" s="53"/>
@@ -51175,8 +51175,8 @@
       <c r="H244" s="58"/>
     </row>
     <row r="245" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="89"/>
-      <c r="C245" s="90"/>
+      <c r="B245" s="87"/>
+      <c r="C245" s="88"/>
       <c r="D245" s="55"/>
       <c r="E245" s="55"/>
       <c r="F245" s="60"/>
@@ -51184,8 +51184,8 @@
       <c r="H245" s="59"/>
     </row>
     <row r="246" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="87"/>
-      <c r="C246" s="88"/>
+      <c r="B246" s="89"/>
+      <c r="C246" s="90"/>
       <c r="D246" s="56"/>
       <c r="E246" s="56"/>
       <c r="F246" s="53"/>
@@ -51193,8 +51193,8 @@
       <c r="H246" s="58"/>
     </row>
     <row r="247" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="89"/>
-      <c r="C247" s="90"/>
+      <c r="B247" s="87"/>
+      <c r="C247" s="88"/>
       <c r="D247" s="55"/>
       <c r="E247" s="55"/>
       <c r="F247" s="60"/>
@@ -51202,8 +51202,8 @@
       <c r="H247" s="59"/>
     </row>
     <row r="248" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="87"/>
-      <c r="C248" s="88"/>
+      <c r="B248" s="89"/>
+      <c r="C248" s="90"/>
       <c r="D248" s="56"/>
       <c r="E248" s="56"/>
       <c r="F248" s="53"/>
@@ -51211,8 +51211,8 @@
       <c r="H248" s="58"/>
     </row>
     <row r="249" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="89"/>
-      <c r="C249" s="90"/>
+      <c r="B249" s="87"/>
+      <c r="C249" s="88"/>
       <c r="D249" s="55"/>
       <c r="E249" s="55"/>
       <c r="F249" s="60"/>
@@ -51220,8 +51220,8 @@
       <c r="H249" s="59"/>
     </row>
     <row r="250" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="87"/>
-      <c r="C250" s="88"/>
+      <c r="B250" s="89"/>
+      <c r="C250" s="90"/>
       <c r="D250" s="56"/>
       <c r="E250" s="56"/>
       <c r="F250" s="53"/>
@@ -51229,8 +51229,8 @@
       <c r="H250" s="58"/>
     </row>
     <row r="251" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="89"/>
-      <c r="C251" s="90"/>
+      <c r="B251" s="87"/>
+      <c r="C251" s="88"/>
       <c r="D251" s="55"/>
       <c r="E251" s="55"/>
       <c r="F251" s="60"/>
@@ -51238,8 +51238,8 @@
       <c r="H251" s="59"/>
     </row>
     <row r="252" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B252" s="87"/>
-      <c r="C252" s="88"/>
+      <c r="B252" s="89"/>
+      <c r="C252" s="90"/>
       <c r="D252" s="56"/>
       <c r="E252" s="56"/>
       <c r="F252" s="53"/>
@@ -51247,8 +51247,8 @@
       <c r="H252" s="58"/>
     </row>
     <row r="253" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="89"/>
-      <c r="C253" s="90"/>
+      <c r="B253" s="87"/>
+      <c r="C253" s="88"/>
       <c r="D253" s="55"/>
       <c r="E253" s="55"/>
       <c r="F253" s="60"/>
@@ -51256,8 +51256,8 @@
       <c r="H253" s="59"/>
     </row>
     <row r="254" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="87"/>
-      <c r="C254" s="88"/>
+      <c r="B254" s="89"/>
+      <c r="C254" s="90"/>
       <c r="D254" s="56"/>
       <c r="E254" s="56"/>
       <c r="F254" s="53"/>
@@ -51265,8 +51265,8 @@
       <c r="H254" s="58"/>
     </row>
     <row r="255" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B255" s="89"/>
-      <c r="C255" s="90"/>
+      <c r="B255" s="87"/>
+      <c r="C255" s="88"/>
       <c r="D255" s="55"/>
       <c r="E255" s="55"/>
       <c r="F255" s="60"/>
@@ -51274,8 +51274,8 @@
       <c r="H255" s="59"/>
     </row>
     <row r="256" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B256" s="87"/>
-      <c r="C256" s="88"/>
+      <c r="B256" s="89"/>
+      <c r="C256" s="90"/>
       <c r="D256" s="56"/>
       <c r="E256" s="56"/>
       <c r="F256" s="53"/>
@@ -51283,8 +51283,8 @@
       <c r="H256" s="58"/>
     </row>
     <row r="257" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="89"/>
-      <c r="C257" s="90"/>
+      <c r="B257" s="87"/>
+      <c r="C257" s="88"/>
       <c r="D257" s="55"/>
       <c r="E257" s="55"/>
       <c r="F257" s="60"/>
@@ -51292,8 +51292,8 @@
       <c r="H257" s="59"/>
     </row>
     <row r="258" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="87"/>
-      <c r="C258" s="88"/>
+      <c r="B258" s="89"/>
+      <c r="C258" s="90"/>
       <c r="D258" s="56"/>
       <c r="E258" s="56"/>
       <c r="F258" s="53"/>
@@ -51301,8 +51301,8 @@
       <c r="H258" s="58"/>
     </row>
     <row r="259" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="89"/>
-      <c r="C259" s="90"/>
+      <c r="B259" s="87"/>
+      <c r="C259" s="88"/>
       <c r="D259" s="55"/>
       <c r="E259" s="55"/>
       <c r="F259" s="60"/>
@@ -51310,8 +51310,8 @@
       <c r="H259" s="59"/>
     </row>
     <row r="260" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="87"/>
-      <c r="C260" s="88"/>
+      <c r="B260" s="89"/>
+      <c r="C260" s="90"/>
       <c r="D260" s="56"/>
       <c r="E260" s="56"/>
       <c r="F260" s="53"/>
@@ -51319,8 +51319,8 @@
       <c r="H260" s="58"/>
     </row>
     <row r="261" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="89"/>
-      <c r="C261" s="90"/>
+      <c r="B261" s="87"/>
+      <c r="C261" s="88"/>
       <c r="D261" s="55"/>
       <c r="E261" s="55"/>
       <c r="F261" s="60"/>
@@ -51328,8 +51328,8 @@
       <c r="H261" s="59"/>
     </row>
     <row r="262" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="87"/>
-      <c r="C262" s="88"/>
+      <c r="B262" s="89"/>
+      <c r="C262" s="90"/>
       <c r="D262" s="56"/>
       <c r="E262" s="56"/>
       <c r="F262" s="53"/>
@@ -51337,8 +51337,8 @@
       <c r="H262" s="58"/>
     </row>
     <row r="263" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="89"/>
-      <c r="C263" s="90"/>
+      <c r="B263" s="87"/>
+      <c r="C263" s="88"/>
       <c r="D263" s="55"/>
       <c r="E263" s="55"/>
       <c r="F263" s="60"/>
@@ -51346,8 +51346,8 @@
       <c r="H263" s="59"/>
     </row>
     <row r="264" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="87"/>
-      <c r="C264" s="88"/>
+      <c r="B264" s="89"/>
+      <c r="C264" s="90"/>
       <c r="D264" s="56"/>
       <c r="E264" s="56"/>
       <c r="F264" s="53"/>
@@ -51355,8 +51355,8 @@
       <c r="H264" s="58"/>
     </row>
     <row r="265" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="89"/>
-      <c r="C265" s="90"/>
+      <c r="B265" s="87"/>
+      <c r="C265" s="88"/>
       <c r="D265" s="55"/>
       <c r="E265" s="55"/>
       <c r="F265" s="60"/>
@@ -51364,8 +51364,8 @@
       <c r="H265" s="59"/>
     </row>
     <row r="266" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="87"/>
-      <c r="C266" s="88"/>
+      <c r="B266" s="89"/>
+      <c r="C266" s="90"/>
       <c r="D266" s="56"/>
       <c r="E266" s="56"/>
       <c r="F266" s="53"/>
@@ -51373,8 +51373,8 @@
       <c r="H266" s="58"/>
     </row>
     <row r="267" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B267" s="89"/>
-      <c r="C267" s="90"/>
+      <c r="B267" s="87"/>
+      <c r="C267" s="88"/>
       <c r="D267" s="55"/>
       <c r="E267" s="55"/>
       <c r="F267" s="60"/>
@@ -51382,8 +51382,8 @@
       <c r="H267" s="59"/>
     </row>
     <row r="268" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B268" s="87"/>
-      <c r="C268" s="88"/>
+      <c r="B268" s="89"/>
+      <c r="C268" s="90"/>
       <c r="D268" s="56"/>
       <c r="E268" s="56"/>
       <c r="F268" s="53"/>
@@ -51391,8 +51391,8 @@
       <c r="H268" s="58"/>
     </row>
     <row r="269" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B269" s="89"/>
-      <c r="C269" s="90"/>
+      <c r="B269" s="87"/>
+      <c r="C269" s="88"/>
       <c r="D269" s="55"/>
       <c r="E269" s="55"/>
       <c r="F269" s="60"/>
@@ -51400,8 +51400,8 @@
       <c r="H269" s="59"/>
     </row>
     <row r="270" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B270" s="87"/>
-      <c r="C270" s="88"/>
+      <c r="B270" s="89"/>
+      <c r="C270" s="90"/>
       <c r="D270" s="56"/>
       <c r="E270" s="56"/>
       <c r="F270" s="53"/>
@@ -51409,8 +51409,8 @@
       <c r="H270" s="58"/>
     </row>
     <row r="271" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="89"/>
-      <c r="C271" s="90"/>
+      <c r="B271" s="87"/>
+      <c r="C271" s="88"/>
       <c r="D271" s="55"/>
       <c r="E271" s="55"/>
       <c r="F271" s="60"/>
@@ -51418,8 +51418,8 @@
       <c r="H271" s="59"/>
     </row>
     <row r="272" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="87"/>
-      <c r="C272" s="88"/>
+      <c r="B272" s="89"/>
+      <c r="C272" s="90"/>
       <c r="D272" s="56"/>
       <c r="E272" s="56"/>
       <c r="F272" s="53"/>
@@ -51427,8 +51427,8 @@
       <c r="H272" s="58"/>
     </row>
     <row r="273" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="89"/>
-      <c r="C273" s="90"/>
+      <c r="B273" s="87"/>
+      <c r="C273" s="88"/>
       <c r="D273" s="55"/>
       <c r="E273" s="55"/>
       <c r="F273" s="60"/>
@@ -51436,8 +51436,8 @@
       <c r="H273" s="59"/>
     </row>
     <row r="274" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="87"/>
-      <c r="C274" s="88"/>
+      <c r="B274" s="89"/>
+      <c r="C274" s="90"/>
       <c r="D274" s="56"/>
       <c r="E274" s="56"/>
       <c r="F274" s="53"/>
@@ -51445,8 +51445,8 @@
       <c r="H274" s="58"/>
     </row>
     <row r="275" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="89"/>
-      <c r="C275" s="90"/>
+      <c r="B275" s="87"/>
+      <c r="C275" s="88"/>
       <c r="D275" s="55"/>
       <c r="E275" s="55"/>
       <c r="F275" s="60"/>
@@ -51454,8 +51454,8 @@
       <c r="H275" s="59"/>
     </row>
     <row r="276" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="87"/>
-      <c r="C276" s="88"/>
+      <c r="B276" s="89"/>
+      <c r="C276" s="90"/>
       <c r="D276" s="56"/>
       <c r="E276" s="56"/>
       <c r="F276" s="53"/>
@@ -51463,8 +51463,8 @@
       <c r="H276" s="58"/>
     </row>
     <row r="277" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B277" s="89"/>
-      <c r="C277" s="90"/>
+      <c r="B277" s="87"/>
+      <c r="C277" s="88"/>
       <c r="D277" s="55"/>
       <c r="E277" s="55"/>
       <c r="F277" s="60"/>
@@ -51472,8 +51472,8 @@
       <c r="H277" s="59"/>
     </row>
     <row r="278" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B278" s="87"/>
-      <c r="C278" s="88"/>
+      <c r="B278" s="89"/>
+      <c r="C278" s="90"/>
       <c r="D278" s="56"/>
       <c r="E278" s="56"/>
       <c r="F278" s="53"/>
@@ -51481,8 +51481,8 @@
       <c r="H278" s="58"/>
     </row>
     <row r="279" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="89"/>
-      <c r="C279" s="90"/>
+      <c r="B279" s="87"/>
+      <c r="C279" s="88"/>
       <c r="D279" s="55"/>
       <c r="E279" s="55"/>
       <c r="F279" s="60"/>
@@ -51490,8 +51490,8 @@
       <c r="H279" s="59"/>
     </row>
     <row r="280" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="87"/>
-      <c r="C280" s="88"/>
+      <c r="B280" s="89"/>
+      <c r="C280" s="90"/>
       <c r="D280" s="56"/>
       <c r="E280" s="56"/>
       <c r="F280" s="53"/>
@@ -51499,8 +51499,8 @@
       <c r="H280" s="58"/>
     </row>
     <row r="281" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B281" s="89"/>
-      <c r="C281" s="90"/>
+      <c r="B281" s="87"/>
+      <c r="C281" s="88"/>
       <c r="D281" s="55"/>
       <c r="E281" s="55"/>
       <c r="F281" s="60"/>
@@ -51508,8 +51508,8 @@
       <c r="H281" s="59"/>
     </row>
     <row r="282" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B282" s="87"/>
-      <c r="C282" s="88"/>
+      <c r="B282" s="89"/>
+      <c r="C282" s="90"/>
       <c r="D282" s="56"/>
       <c r="E282" s="56"/>
       <c r="F282" s="53"/>
@@ -51517,8 +51517,8 @@
       <c r="H282" s="58"/>
     </row>
     <row r="283" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="89"/>
-      <c r="C283" s="90"/>
+      <c r="B283" s="87"/>
+      <c r="C283" s="88"/>
       <c r="D283" s="55"/>
       <c r="E283" s="55"/>
       <c r="F283" s="60"/>
@@ -51526,8 +51526,8 @@
       <c r="H283" s="59"/>
     </row>
     <row r="284" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="87"/>
-      <c r="C284" s="88"/>
+      <c r="B284" s="89"/>
+      <c r="C284" s="90"/>
       <c r="D284" s="56"/>
       <c r="E284" s="56"/>
       <c r="F284" s="53"/>
@@ -51535,8 +51535,8 @@
       <c r="H284" s="58"/>
     </row>
     <row r="285" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B285" s="89"/>
-      <c r="C285" s="90"/>
+      <c r="B285" s="87"/>
+      <c r="C285" s="88"/>
       <c r="D285" s="55"/>
       <c r="E285" s="55"/>
       <c r="F285" s="60"/>
@@ -51544,8 +51544,8 @@
       <c r="H285" s="59"/>
     </row>
     <row r="286" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="87"/>
-      <c r="C286" s="88"/>
+      <c r="B286" s="89"/>
+      <c r="C286" s="90"/>
       <c r="D286" s="56"/>
       <c r="E286" s="56"/>
       <c r="F286" s="53"/>
@@ -51553,8 +51553,8 @@
       <c r="H286" s="58"/>
     </row>
     <row r="287" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="89"/>
-      <c r="C287" s="90"/>
+      <c r="B287" s="87"/>
+      <c r="C287" s="88"/>
       <c r="D287" s="55"/>
       <c r="E287" s="55"/>
       <c r="F287" s="60"/>
@@ -51562,8 +51562,8 @@
       <c r="H287" s="59"/>
     </row>
     <row r="288" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="87"/>
-      <c r="C288" s="88"/>
+      <c r="B288" s="89"/>
+      <c r="C288" s="90"/>
       <c r="D288" s="56"/>
       <c r="E288" s="56"/>
       <c r="F288" s="53"/>
@@ -51571,8 +51571,8 @@
       <c r="H288" s="58"/>
     </row>
     <row r="289" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="89"/>
-      <c r="C289" s="90"/>
+      <c r="B289" s="87"/>
+      <c r="C289" s="88"/>
       <c r="D289" s="55"/>
       <c r="E289" s="55"/>
       <c r="F289" s="60"/>
@@ -51580,8 +51580,8 @@
       <c r="H289" s="59"/>
     </row>
     <row r="290" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B290" s="87"/>
-      <c r="C290" s="88"/>
+      <c r="B290" s="89"/>
+      <c r="C290" s="90"/>
       <c r="D290" s="56"/>
       <c r="E290" s="56"/>
       <c r="F290" s="53"/>
@@ -51589,8 +51589,8 @@
       <c r="H290" s="58"/>
     </row>
     <row r="291" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B291" s="89"/>
-      <c r="C291" s="90"/>
+      <c r="B291" s="87"/>
+      <c r="C291" s="88"/>
       <c r="D291" s="55"/>
       <c r="E291" s="55"/>
       <c r="F291" s="60"/>
@@ -51598,8 +51598,8 @@
       <c r="H291" s="59"/>
     </row>
     <row r="292" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B292" s="87"/>
-      <c r="C292" s="88"/>
+      <c r="B292" s="89"/>
+      <c r="C292" s="90"/>
       <c r="D292" s="56"/>
       <c r="E292" s="56"/>
       <c r="F292" s="53"/>
@@ -51607,8 +51607,8 @@
       <c r="H292" s="58"/>
     </row>
     <row r="293" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B293" s="89"/>
-      <c r="C293" s="90"/>
+      <c r="B293" s="87"/>
+      <c r="C293" s="88"/>
       <c r="D293" s="55"/>
       <c r="E293" s="55"/>
       <c r="F293" s="60"/>
@@ -51616,8 +51616,8 @@
       <c r="H293" s="59"/>
     </row>
     <row r="294" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B294" s="87"/>
-      <c r="C294" s="88"/>
+      <c r="B294" s="89"/>
+      <c r="C294" s="90"/>
       <c r="D294" s="56"/>
       <c r="E294" s="56"/>
       <c r="F294" s="53"/>
@@ -51625,8 +51625,8 @@
       <c r="H294" s="58"/>
     </row>
     <row r="295" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B295" s="89"/>
-      <c r="C295" s="90"/>
+      <c r="B295" s="87"/>
+      <c r="C295" s="88"/>
       <c r="D295" s="55"/>
       <c r="E295" s="55"/>
       <c r="F295" s="60"/>
@@ -51634,8 +51634,8 @@
       <c r="H295" s="59"/>
     </row>
     <row r="296" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B296" s="87"/>
-      <c r="C296" s="88"/>
+      <c r="B296" s="89"/>
+      <c r="C296" s="90"/>
       <c r="D296" s="56"/>
       <c r="E296" s="56"/>
       <c r="F296" s="53"/>
@@ -51643,8 +51643,8 @@
       <c r="H296" s="58"/>
     </row>
     <row r="297" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B297" s="89"/>
-      <c r="C297" s="90"/>
+      <c r="B297" s="87"/>
+      <c r="C297" s="88"/>
       <c r="D297" s="55"/>
       <c r="E297" s="55"/>
       <c r="F297" s="60"/>
@@ -51652,8 +51652,8 @@
       <c r="H297" s="59"/>
     </row>
     <row r="298" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="87"/>
-      <c r="C298" s="88"/>
+      <c r="B298" s="89"/>
+      <c r="C298" s="90"/>
       <c r="D298" s="56"/>
       <c r="E298" s="56"/>
       <c r="F298" s="53"/>
@@ -51661,8 +51661,8 @@
       <c r="H298" s="58"/>
     </row>
     <row r="299" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B299" s="89"/>
-      <c r="C299" s="90"/>
+      <c r="B299" s="87"/>
+      <c r="C299" s="88"/>
       <c r="D299" s="55"/>
       <c r="E299" s="55"/>
       <c r="F299" s="60"/>
@@ -51670,8 +51670,8 @@
       <c r="H299" s="59"/>
     </row>
     <row r="300" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B300" s="87"/>
-      <c r="C300" s="88"/>
+      <c r="B300" s="89"/>
+      <c r="C300" s="90"/>
       <c r="D300" s="56"/>
       <c r="E300" s="56"/>
       <c r="F300" s="53"/>
@@ -51681,6 +51681,286 @@
   </sheetData>
   <sheetProtection password="CEBA" sheet="1" objects="1" scenarios="1" formatCells="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <mergeCells count="292">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B227:C227"/>
+    <mergeCell ref="B228:C228"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B221:C221"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B234:C234"/>
+    <mergeCell ref="B235:C235"/>
+    <mergeCell ref="B236:C236"/>
+    <mergeCell ref="B237:C237"/>
+    <mergeCell ref="B238:C238"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="B230:C230"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="B232:C232"/>
+    <mergeCell ref="B233:C233"/>
+    <mergeCell ref="B244:C244"/>
+    <mergeCell ref="B245:C245"/>
+    <mergeCell ref="B246:C246"/>
+    <mergeCell ref="B247:C247"/>
+    <mergeCell ref="B248:C248"/>
+    <mergeCell ref="B239:C239"/>
+    <mergeCell ref="B240:C240"/>
+    <mergeCell ref="B241:C241"/>
+    <mergeCell ref="B242:C242"/>
+    <mergeCell ref="B243:C243"/>
+    <mergeCell ref="B254:C254"/>
+    <mergeCell ref="B255:C255"/>
+    <mergeCell ref="B256:C256"/>
+    <mergeCell ref="B257:C257"/>
+    <mergeCell ref="B258:C258"/>
+    <mergeCell ref="B249:C249"/>
+    <mergeCell ref="B250:C250"/>
+    <mergeCell ref="B251:C251"/>
+    <mergeCell ref="B252:C252"/>
+    <mergeCell ref="B253:C253"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B265:C265"/>
+    <mergeCell ref="B266:C266"/>
+    <mergeCell ref="B267:C267"/>
+    <mergeCell ref="B268:C268"/>
+    <mergeCell ref="B259:C259"/>
+    <mergeCell ref="B260:C260"/>
+    <mergeCell ref="B261:C261"/>
+    <mergeCell ref="B262:C262"/>
+    <mergeCell ref="B263:C263"/>
+    <mergeCell ref="B274:C274"/>
+    <mergeCell ref="B275:C275"/>
+    <mergeCell ref="B276:C276"/>
+    <mergeCell ref="B277:C277"/>
+    <mergeCell ref="B278:C278"/>
+    <mergeCell ref="B269:C269"/>
+    <mergeCell ref="B270:C270"/>
+    <mergeCell ref="B271:C271"/>
+    <mergeCell ref="B272:C272"/>
+    <mergeCell ref="B273:C273"/>
+    <mergeCell ref="B284:C284"/>
+    <mergeCell ref="B285:C285"/>
+    <mergeCell ref="B286:C286"/>
+    <mergeCell ref="B287:C287"/>
+    <mergeCell ref="B288:C288"/>
+    <mergeCell ref="B279:C279"/>
+    <mergeCell ref="B280:C280"/>
+    <mergeCell ref="B281:C281"/>
+    <mergeCell ref="B282:C282"/>
+    <mergeCell ref="B283:C283"/>
     <mergeCell ref="B299:C299"/>
     <mergeCell ref="B300:C300"/>
     <mergeCell ref="B294:C294"/>
@@ -51693,286 +51973,6 @@
     <mergeCell ref="B291:C291"/>
     <mergeCell ref="B292:C292"/>
     <mergeCell ref="B293:C293"/>
-    <mergeCell ref="B284:C284"/>
-    <mergeCell ref="B285:C285"/>
-    <mergeCell ref="B286:C286"/>
-    <mergeCell ref="B287:C287"/>
-    <mergeCell ref="B288:C288"/>
-    <mergeCell ref="B279:C279"/>
-    <mergeCell ref="B280:C280"/>
-    <mergeCell ref="B281:C281"/>
-    <mergeCell ref="B282:C282"/>
-    <mergeCell ref="B283:C283"/>
-    <mergeCell ref="B274:C274"/>
-    <mergeCell ref="B275:C275"/>
-    <mergeCell ref="B276:C276"/>
-    <mergeCell ref="B277:C277"/>
-    <mergeCell ref="B278:C278"/>
-    <mergeCell ref="B269:C269"/>
-    <mergeCell ref="B270:C270"/>
-    <mergeCell ref="B271:C271"/>
-    <mergeCell ref="B272:C272"/>
-    <mergeCell ref="B273:C273"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B265:C265"/>
-    <mergeCell ref="B266:C266"/>
-    <mergeCell ref="B267:C267"/>
-    <mergeCell ref="B268:C268"/>
-    <mergeCell ref="B259:C259"/>
-    <mergeCell ref="B260:C260"/>
-    <mergeCell ref="B261:C261"/>
-    <mergeCell ref="B262:C262"/>
-    <mergeCell ref="B263:C263"/>
-    <mergeCell ref="B254:C254"/>
-    <mergeCell ref="B255:C255"/>
-    <mergeCell ref="B256:C256"/>
-    <mergeCell ref="B257:C257"/>
-    <mergeCell ref="B258:C258"/>
-    <mergeCell ref="B249:C249"/>
-    <mergeCell ref="B250:C250"/>
-    <mergeCell ref="B251:C251"/>
-    <mergeCell ref="B252:C252"/>
-    <mergeCell ref="B253:C253"/>
-    <mergeCell ref="B244:C244"/>
-    <mergeCell ref="B245:C245"/>
-    <mergeCell ref="B246:C246"/>
-    <mergeCell ref="B247:C247"/>
-    <mergeCell ref="B248:C248"/>
-    <mergeCell ref="B239:C239"/>
-    <mergeCell ref="B240:C240"/>
-    <mergeCell ref="B241:C241"/>
-    <mergeCell ref="B242:C242"/>
-    <mergeCell ref="B243:C243"/>
-    <mergeCell ref="B234:C234"/>
-    <mergeCell ref="B235:C235"/>
-    <mergeCell ref="B236:C236"/>
-    <mergeCell ref="B237:C237"/>
-    <mergeCell ref="B238:C238"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="B230:C230"/>
-    <mergeCell ref="B231:C231"/>
-    <mergeCell ref="B232:C232"/>
-    <mergeCell ref="B233:C233"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B227:C227"/>
-    <mergeCell ref="B228:C228"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B221:C221"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F300">
     <cfRule type="expression" dxfId="2" priority="1">
@@ -52010,7 +52010,7 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" defaultGridColor="0" colorId="22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" defaultGridColor="0" colorId="22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -52032,12 +52032,12 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="81">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
       <c r="D2" s="93"/>
-      <c r="E2" s="86"/>
+      <c r="E2" s="82"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>

</xml_diff>

<commit_message>
Steckbrief angepasst, so dass Zeilenhöhe so gewählt wird, dass alle Inhalte angezeigt werden Wenn im Steckbrief bei Erläuterung "Linefeed" angegeben wird, so ist das im Info-Fenster derProjekt-Tafel auch so dargestellt Diagramm-Titel in PRC Doagrammen wird ebi Update nicht mehr verändert Projekt-Steckbrief von den Überschriften her geändert
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stammdaten" sheetId="6" r:id="rId1"/>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Projektleiter</t>
-  </si>
-  <si>
-    <t>Ergebnisse</t>
   </si>
   <si>
     <t xml:space="preserve">Projekt Name </t>
@@ -166,9 +163,6 @@
     <t>Ampel</t>
   </si>
   <si>
-    <t>Maßnahmen</t>
-  </si>
-  <si>
     <t>Budget in T€</t>
   </si>
   <si>
@@ -200,12 +194,6 @@
   </si>
   <si>
     <t>Tester</t>
-  </si>
-  <si>
-    <t>StartDatum</t>
-  </si>
-  <si>
-    <t>EndeDatum</t>
   </si>
   <si>
     <t>Project-Vorlagen</t>
@@ -284,6 +272,18 @@
   </si>
   <si>
     <t xml:space="preserve">  Zeitleiste</t>
+  </si>
+  <si>
+    <t>Lieferumfänge</t>
+  </si>
+  <si>
+    <t>Ende-Datum</t>
+  </si>
+  <si>
+    <t>Start-Datum</t>
+  </si>
+  <si>
+    <t>Termine</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="2" spans="2:7" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="68"/>
@@ -1470,7 +1470,7 @@
     <row r="3" spans="2:7" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:7" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="21">
         <v>1</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="6" spans="2:7" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="21">
         <v>2958465</v>
@@ -1515,7 +1515,7 @@
     <row r="11" spans="2:7" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:7" s="13" customFormat="1" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="24"/>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="21" spans="2:5" s="13" customFormat="1" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="48"/>
       <c r="D21" s="30"/>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="23" spans="2:5" s="13" customFormat="1" ht="18.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B23" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="70"/>
       <c r="D23" s="71"/>
@@ -1897,7 +1897,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:GI250"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="2" spans="1:191" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="81">
         <f>Projekt_Name</f>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="4" spans="1:191" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="11">
         <f>StartDatum</f>
@@ -1973,7 +1973,7 @@
     <row r="6" spans="1:191" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="11">
         <f>EndeDatum</f>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="8" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1999,7 +1999,7 @@
     <row r="9" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:191" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="83" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C10" s="84"/>
       <c r="D10" s="37"/>
@@ -48882,8 +48882,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:M300"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48892,7 +48892,8 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="10" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="94.85546875" customWidth="1"/>
+    <col min="8" max="10" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -48913,7 +48914,7 @@
     <row r="2" spans="1:13" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="81">
         <f>Projekt_Name</f>
@@ -48948,7 +48949,7 @@
     <row r="4" spans="1:13" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="11">
         <f>StartDatum</f>
@@ -48983,7 +48984,7 @@
     <row r="6" spans="1:13" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="11">
         <f>EndeDatum</f>
@@ -49018,7 +49019,7 @@
     <row r="8" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -49049,23 +49050,23 @@
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="91" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" s="92"/>
       <c r="D10" s="54" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="H10" s="54" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -52030,7 +52031,7 @@
     <row r="1" spans="2:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="81">
         <f>Projekt_Name</f>
@@ -52046,7 +52047,7 @@
     <row r="3" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="18">
         <f>StartDatum</f>
@@ -52063,7 +52064,7 @@
     </row>
     <row r="6" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="18">
         <f>EndeDatum</f>
@@ -52083,17 +52084,17 @@
     </row>
     <row r="9" spans="2:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="62"/>
       <c r="D11" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="52"/>
       <c r="F11" s="17"/>
@@ -52103,7 +52104,7 @@
     <row r="13" spans="2:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="62"/>
       <c r="D14" s="17"/>
@@ -52111,11 +52112,11 @@
     <row r="15" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="62"/>
       <c r="D16" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="63"/>
       <c r="G16" s="20"/>
@@ -52123,13 +52124,13 @@
     <row r="17" spans="2:4" ht="18.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:4" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="61" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="62"/>
       <c r="D22" s="17"/>
@@ -52137,7 +52138,7 @@
     <row r="23" spans="2:4" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:4" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="62"/>
       <c r="D24" s="17"/>
@@ -52145,7 +52146,7 @@
     <row r="25" spans="2:4" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:4" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="62"/>
       <c r="D26" s="17"/>
@@ -52208,196 +52209,196 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="36"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="44"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="45"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="36"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="36"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="44"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="44"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="32"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="46"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="45"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="43"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="44"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="43"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>56</v>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
       </c>
-      <c r="B9" s="36"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>54</v>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
       </c>
-      <c r="B10" s="44"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="45"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="36"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="36"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="44"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="44"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="32"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="46"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="45"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="43"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="44"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="43"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>26</v>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report: Es gibt jetzt auch Projektphasen (nicht nur Teilprojekte) Bewertung im Datenmodell MEilenstein wurde um "Deliverables" ergänzt (Bedarf für Re-Engineering!; Bewertung von Deliverables trennen) PRojekt-Steckbrief:  kann jetzt auch Lieferumfänge im Steckbrief importieren/exportieren   ; das Datenmodell kann in der Datenbank gelesen / gespeichert werden; es gibt keine Probleme, wenn das "alte" Datenmodell in de rdatenbank gelesen wird Tabelle Ziele im Einzelprojekt bericht wurde um eine Spalte "Deliverables" ergänzt in der Multiprojekt Reporting Routine den Fehler korrigiert, der auftritt, wenn der gesuchte Meilenstein nicht auftritt
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Projekt-Steckbrief.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="13440" windowHeight="9135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stammdaten" sheetId="6" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -274,9 +274,6 @@
     <t xml:space="preserve">  Zeitleiste</t>
   </si>
   <si>
-    <t>Lieferumfänge</t>
-  </si>
-  <si>
     <t>Ende-Datum</t>
   </si>
   <si>
@@ -284,6 +281,12 @@
   </si>
   <si>
     <t>Termine</t>
+  </si>
+  <si>
+    <t>Ampel-Erläuterung</t>
+  </si>
+  <si>
+    <t>Ergebnisse</t>
   </si>
 </sst>
 </file>
@@ -993,12 +996,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1011,16 +1008,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1897,7 +1900,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:GI250"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1924,11 +1927,11 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="85">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
-      <c r="D2" s="82"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="65"/>
       <c r="F2" s="65"/>
       <c r="G2" s="65"/>
@@ -1998,10 +2001,10 @@
     </row>
     <row r="9" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:191" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="37"/>
       <c r="E10" s="51">
         <f>StartDatum</f>
@@ -2750,8 +2753,8 @@
       <c r="GI10" s="49"/>
     </row>
     <row r="11" spans="1:191" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="37"/>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
@@ -48592,224 +48595,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="242">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B231:C231"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B221:C221"/>
     <mergeCell ref="B247:C247"/>
     <mergeCell ref="B248:C248"/>
     <mergeCell ref="B249:C249"/>
@@ -48834,6 +48619,224 @@
     <mergeCell ref="B228:C228"/>
     <mergeCell ref="B229:C229"/>
     <mergeCell ref="B230:C230"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B221:C221"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B250">
     <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
@@ -48882,8 +48885,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:M300"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48892,8 +48895,9 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="94.85546875" customWidth="1"/>
-    <col min="8" max="10" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="70.7109375" customWidth="1"/>
+    <col min="8" max="8" width="57.5703125" customWidth="1"/>
+    <col min="9" max="10" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -48916,11 +48920,11 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="85">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
-      <c r="D2" s="82"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -49019,7 +49023,7 @@
     <row r="8" spans="1:13" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -49054,24 +49058,24 @@
       </c>
       <c r="C10" s="92"/>
       <c r="D10" s="54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="54" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H10" s="54" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="60"/>
@@ -49079,8 +49083,8 @@
       <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="89"/>
-      <c r="C12" s="90"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
       <c r="F12" s="53"/>
@@ -49088,8 +49092,8 @@
       <c r="H12" s="58"/>
     </row>
     <row r="13" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="87"/>
-      <c r="C13" s="88"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="F13" s="60"/>
@@ -49097,8 +49101,8 @@
       <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="89"/>
-      <c r="C14" s="90"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
       <c r="F14" s="53"/>
@@ -49106,8 +49110,8 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="90"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="F15" s="60"/>
@@ -49115,8 +49119,8 @@
       <c r="H15" s="59"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="89"/>
-      <c r="C16" s="90"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
       <c r="F16" s="53"/>
@@ -49124,8 +49128,8 @@
       <c r="H16" s="58"/>
     </row>
     <row r="17" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="60"/>
@@ -49133,8 +49137,8 @@
       <c r="H17" s="59"/>
     </row>
     <row r="18" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="88"/>
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
       <c r="F18" s="53"/>
@@ -49142,8 +49146,8 @@
       <c r="H18" s="58"/>
     </row>
     <row r="19" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="F19" s="60"/>
@@ -49151,8 +49155,8 @@
       <c r="H19" s="59"/>
     </row>
     <row r="20" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
       <c r="F20" s="53"/>
@@ -49160,8 +49164,8 @@
       <c r="H20" s="58"/>
     </row>
     <row r="21" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="60"/>
@@ -49169,8 +49173,8 @@
       <c r="H21" s="59"/>
     </row>
     <row r="22" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
       <c r="F22" s="53"/>
@@ -49178,8 +49182,8 @@
       <c r="H22" s="58"/>
     </row>
     <row r="23" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
       <c r="F23" s="60"/>
@@ -49187,8 +49191,8 @@
       <c r="H23" s="59"/>
     </row>
     <row r="24" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
       <c r="F24" s="53"/>
@@ -49196,8 +49200,8 @@
       <c r="H24" s="58"/>
     </row>
     <row r="25" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
       <c r="F25" s="60"/>
@@ -49205,8 +49209,8 @@
       <c r="H25" s="59"/>
     </row>
     <row r="26" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
       <c r="F26" s="53"/>
@@ -49214,8 +49218,8 @@
       <c r="H26" s="58"/>
     </row>
     <row r="27" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
       <c r="F27" s="60"/>
@@ -49223,8 +49227,8 @@
       <c r="H27" s="59"/>
     </row>
     <row r="28" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="56"/>
       <c r="E28" s="56"/>
       <c r="F28" s="53"/>
@@ -49232,8 +49236,8 @@
       <c r="H28" s="58"/>
     </row>
     <row r="29" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="87"/>
-      <c r="C29" s="88"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90"/>
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
       <c r="F29" s="60"/>
@@ -49241,8 +49245,8 @@
       <c r="H29" s="59"/>
     </row>
     <row r="30" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
       <c r="D30" s="56"/>
       <c r="E30" s="56"/>
       <c r="F30" s="53"/>
@@ -49250,8 +49254,8 @@
       <c r="H30" s="58"/>
     </row>
     <row r="31" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="55"/>
       <c r="E31" s="55"/>
       <c r="F31" s="60"/>
@@ -49259,8 +49263,8 @@
       <c r="H31" s="59"/>
     </row>
     <row r="32" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="56"/>
       <c r="E32" s="56"/>
       <c r="F32" s="53"/>
@@ -49268,8 +49272,8 @@
       <c r="H32" s="58"/>
     </row>
     <row r="33" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="87"/>
-      <c r="C33" s="88"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="55"/>
       <c r="E33" s="55"/>
       <c r="F33" s="60"/>
@@ -49277,8 +49281,8 @@
       <c r="H33" s="59"/>
     </row>
     <row r="34" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="88"/>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
       <c r="F34" s="53"/>
@@ -49286,8 +49290,8 @@
       <c r="H34" s="58"/>
     </row>
     <row r="35" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="87"/>
-      <c r="C35" s="88"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="90"/>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
       <c r="F35" s="60"/>
@@ -49295,8 +49299,8 @@
       <c r="H35" s="59"/>
     </row>
     <row r="36" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="88"/>
       <c r="D36" s="56"/>
       <c r="E36" s="56"/>
       <c r="F36" s="53"/>
@@ -49304,8 +49308,8 @@
       <c r="H36" s="58"/>
     </row>
     <row r="37" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="87"/>
-      <c r="C37" s="88"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="90"/>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
       <c r="F37" s="60"/>
@@ -49313,8 +49317,8 @@
       <c r="H37" s="59"/>
     </row>
     <row r="38" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="88"/>
       <c r="D38" s="56"/>
       <c r="E38" s="56"/>
       <c r="F38" s="53"/>
@@ -49322,8 +49326,8 @@
       <c r="H38" s="58"/>
     </row>
     <row r="39" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="87"/>
-      <c r="C39" s="88"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="55"/>
       <c r="E39" s="55"/>
       <c r="F39" s="60"/>
@@ -49331,8 +49335,8 @@
       <c r="H39" s="59"/>
     </row>
     <row r="40" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="89"/>
-      <c r="C40" s="90"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="88"/>
       <c r="D40" s="56"/>
       <c r="E40" s="56"/>
       <c r="F40" s="53"/>
@@ -49340,8 +49344,8 @@
       <c r="H40" s="58"/>
     </row>
     <row r="41" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="87"/>
-      <c r="C41" s="88"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="90"/>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
       <c r="F41" s="60"/>
@@ -49349,8 +49353,8 @@
       <c r="H41" s="59"/>
     </row>
     <row r="42" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="88"/>
       <c r="D42" s="56"/>
       <c r="E42" s="56"/>
       <c r="F42" s="53"/>
@@ -49358,8 +49362,8 @@
       <c r="H42" s="58"/>
     </row>
     <row r="43" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="87"/>
-      <c r="C43" s="88"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="90"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
       <c r="F43" s="60"/>
@@ -49367,8 +49371,8 @@
       <c r="H43" s="59"/>
     </row>
     <row r="44" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="89"/>
-      <c r="C44" s="90"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="88"/>
       <c r="D44" s="56"/>
       <c r="E44" s="56"/>
       <c r="F44" s="53"/>
@@ -49376,8 +49380,8 @@
       <c r="H44" s="58"/>
     </row>
     <row r="45" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="87"/>
-      <c r="C45" s="88"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="90"/>
       <c r="D45" s="55"/>
       <c r="E45" s="55"/>
       <c r="F45" s="60"/>
@@ -49385,8 +49389,8 @@
       <c r="H45" s="59"/>
     </row>
     <row r="46" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="88"/>
       <c r="D46" s="56"/>
       <c r="E46" s="56"/>
       <c r="F46" s="53"/>
@@ -49394,8 +49398,8 @@
       <c r="H46" s="58"/>
     </row>
     <row r="47" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="87"/>
-      <c r="C47" s="88"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="90"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
       <c r="F47" s="60"/>
@@ -49403,8 +49407,8 @@
       <c r="H47" s="59"/>
     </row>
     <row r="48" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="89"/>
-      <c r="C48" s="90"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="88"/>
       <c r="D48" s="56"/>
       <c r="E48" s="56"/>
       <c r="F48" s="53"/>
@@ -49412,8 +49416,8 @@
       <c r="H48" s="58"/>
     </row>
     <row r="49" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="87"/>
-      <c r="C49" s="88"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="90"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
       <c r="F49" s="60"/>
@@ -49421,8 +49425,8 @@
       <c r="H49" s="59"/>
     </row>
     <row r="50" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="89"/>
-      <c r="C50" s="90"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="88"/>
       <c r="D50" s="56"/>
       <c r="E50" s="56"/>
       <c r="F50" s="53"/>
@@ -49430,8 +49434,8 @@
       <c r="H50" s="58"/>
     </row>
     <row r="51" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="87"/>
-      <c r="C51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="90"/>
       <c r="D51" s="55"/>
       <c r="E51" s="55"/>
       <c r="F51" s="60"/>
@@ -49439,8 +49443,8 @@
       <c r="H51" s="59"/>
     </row>
     <row r="52" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="88"/>
       <c r="D52" s="56"/>
       <c r="E52" s="56"/>
       <c r="F52" s="53"/>
@@ -49448,8 +49452,8 @@
       <c r="H52" s="58"/>
     </row>
     <row r="53" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="87"/>
-      <c r="C53" s="88"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="90"/>
       <c r="D53" s="55"/>
       <c r="E53" s="55"/>
       <c r="F53" s="60"/>
@@ -49457,8 +49461,8 @@
       <c r="H53" s="59"/>
     </row>
     <row r="54" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="89"/>
-      <c r="C54" s="90"/>
+      <c r="B54" s="87"/>
+      <c r="C54" s="88"/>
       <c r="D54" s="56"/>
       <c r="E54" s="56"/>
       <c r="F54" s="53"/>
@@ -49466,8 +49470,8 @@
       <c r="H54" s="58"/>
     </row>
     <row r="55" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="87"/>
-      <c r="C55" s="88"/>
+      <c r="B55" s="89"/>
+      <c r="C55" s="90"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
       <c r="F55" s="60"/>
@@ -49475,8 +49479,8 @@
       <c r="H55" s="59"/>
     </row>
     <row r="56" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="89"/>
-      <c r="C56" s="90"/>
+      <c r="B56" s="87"/>
+      <c r="C56" s="88"/>
       <c r="D56" s="56"/>
       <c r="E56" s="56"/>
       <c r="F56" s="53"/>
@@ -49484,8 +49488,8 @@
       <c r="H56" s="58"/>
     </row>
     <row r="57" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="87"/>
-      <c r="C57" s="88"/>
+      <c r="B57" s="89"/>
+      <c r="C57" s="90"/>
       <c r="D57" s="55"/>
       <c r="E57" s="55"/>
       <c r="F57" s="60"/>
@@ -49493,8 +49497,8 @@
       <c r="H57" s="59"/>
     </row>
     <row r="58" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="89"/>
-      <c r="C58" s="90"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="88"/>
       <c r="D58" s="56"/>
       <c r="E58" s="56"/>
       <c r="F58" s="53"/>
@@ -49502,8 +49506,8 @@
       <c r="H58" s="58"/>
     </row>
     <row r="59" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="87"/>
-      <c r="C59" s="88"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="90"/>
       <c r="D59" s="55"/>
       <c r="E59" s="55"/>
       <c r="F59" s="60"/>
@@ -49511,8 +49515,8 @@
       <c r="H59" s="59"/>
     </row>
     <row r="60" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="89"/>
-      <c r="C60" s="90"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="88"/>
       <c r="D60" s="56"/>
       <c r="E60" s="56"/>
       <c r="F60" s="53"/>
@@ -49520,8 +49524,8 @@
       <c r="H60" s="58"/>
     </row>
     <row r="61" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="87"/>
-      <c r="C61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="90"/>
       <c r="D61" s="55"/>
       <c r="E61" s="55"/>
       <c r="F61" s="60"/>
@@ -49529,8 +49533,8 @@
       <c r="H61" s="59"/>
     </row>
     <row r="62" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="89"/>
-      <c r="C62" s="90"/>
+      <c r="B62" s="87"/>
+      <c r="C62" s="88"/>
       <c r="D62" s="56"/>
       <c r="E62" s="56"/>
       <c r="F62" s="53"/>
@@ -49538,8 +49542,8 @@
       <c r="H62" s="58"/>
     </row>
     <row r="63" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="87"/>
-      <c r="C63" s="88"/>
+      <c r="B63" s="89"/>
+      <c r="C63" s="90"/>
       <c r="D63" s="55"/>
       <c r="E63" s="55"/>
       <c r="F63" s="60"/>
@@ -49547,8 +49551,8 @@
       <c r="H63" s="59"/>
     </row>
     <row r="64" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="89"/>
-      <c r="C64" s="90"/>
+      <c r="B64" s="87"/>
+      <c r="C64" s="88"/>
       <c r="D64" s="56"/>
       <c r="E64" s="56"/>
       <c r="F64" s="53"/>
@@ -49556,8 +49560,8 @@
       <c r="H64" s="58"/>
     </row>
     <row r="65" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="87"/>
-      <c r="C65" s="88"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="90"/>
       <c r="D65" s="55"/>
       <c r="E65" s="55"/>
       <c r="F65" s="60"/>
@@ -49565,8 +49569,8 @@
       <c r="H65" s="59"/>
     </row>
     <row r="66" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="89"/>
-      <c r="C66" s="90"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="88"/>
       <c r="D66" s="56"/>
       <c r="E66" s="56"/>
       <c r="F66" s="53"/>
@@ -49574,8 +49578,8 @@
       <c r="H66" s="58"/>
     </row>
     <row r="67" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="87"/>
-      <c r="C67" s="88"/>
+      <c r="B67" s="89"/>
+      <c r="C67" s="90"/>
       <c r="D67" s="55"/>
       <c r="E67" s="55"/>
       <c r="F67" s="60"/>
@@ -49583,8 +49587,8 @@
       <c r="H67" s="59"/>
     </row>
     <row r="68" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="89"/>
-      <c r="C68" s="90"/>
+      <c r="B68" s="87"/>
+      <c r="C68" s="88"/>
       <c r="D68" s="56"/>
       <c r="E68" s="56"/>
       <c r="F68" s="53"/>
@@ -49592,8 +49596,8 @@
       <c r="H68" s="58"/>
     </row>
     <row r="69" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="87"/>
-      <c r="C69" s="88"/>
+      <c r="B69" s="89"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="55"/>
       <c r="E69" s="55"/>
       <c r="F69" s="60"/>
@@ -49601,8 +49605,8 @@
       <c r="H69" s="59"/>
     </row>
     <row r="70" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="89"/>
-      <c r="C70" s="90"/>
+      <c r="B70" s="87"/>
+      <c r="C70" s="88"/>
       <c r="D70" s="56"/>
       <c r="E70" s="56"/>
       <c r="F70" s="53"/>
@@ -49610,8 +49614,8 @@
       <c r="H70" s="58"/>
     </row>
     <row r="71" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="87"/>
-      <c r="C71" s="88"/>
+      <c r="B71" s="89"/>
+      <c r="C71" s="90"/>
       <c r="D71" s="55"/>
       <c r="E71" s="55"/>
       <c r="F71" s="60"/>
@@ -49619,8 +49623,8 @@
       <c r="H71" s="59"/>
     </row>
     <row r="72" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="89"/>
-      <c r="C72" s="90"/>
+      <c r="B72" s="87"/>
+      <c r="C72" s="88"/>
       <c r="D72" s="56"/>
       <c r="E72" s="56"/>
       <c r="F72" s="53"/>
@@ -49628,8 +49632,8 @@
       <c r="H72" s="58"/>
     </row>
     <row r="73" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="87"/>
-      <c r="C73" s="88"/>
+      <c r="B73" s="89"/>
+      <c r="C73" s="90"/>
       <c r="D73" s="55"/>
       <c r="E73" s="55"/>
       <c r="F73" s="60"/>
@@ -49637,8 +49641,8 @@
       <c r="H73" s="59"/>
     </row>
     <row r="74" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="89"/>
-      <c r="C74" s="90"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="88"/>
       <c r="D74" s="56"/>
       <c r="E74" s="56"/>
       <c r="F74" s="53"/>
@@ -49646,8 +49650,8 @@
       <c r="H74" s="58"/>
     </row>
     <row r="75" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="87"/>
-      <c r="C75" s="88"/>
+      <c r="B75" s="89"/>
+      <c r="C75" s="90"/>
       <c r="D75" s="55"/>
       <c r="E75" s="55"/>
       <c r="F75" s="60"/>
@@ -49655,8 +49659,8 @@
       <c r="H75" s="59"/>
     </row>
     <row r="76" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="89"/>
-      <c r="C76" s="90"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="88"/>
       <c r="D76" s="56"/>
       <c r="E76" s="56"/>
       <c r="F76" s="53"/>
@@ -49664,8 +49668,8 @@
       <c r="H76" s="58"/>
     </row>
     <row r="77" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="87"/>
-      <c r="C77" s="88"/>
+      <c r="B77" s="89"/>
+      <c r="C77" s="90"/>
       <c r="D77" s="55"/>
       <c r="E77" s="55"/>
       <c r="F77" s="60"/>
@@ -49673,8 +49677,8 @@
       <c r="H77" s="59"/>
     </row>
     <row r="78" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="89"/>
-      <c r="C78" s="90"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="88"/>
       <c r="D78" s="56"/>
       <c r="E78" s="56"/>
       <c r="F78" s="53"/>
@@ -49682,8 +49686,8 @@
       <c r="H78" s="58"/>
     </row>
     <row r="79" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="87"/>
-      <c r="C79" s="88"/>
+      <c r="B79" s="89"/>
+      <c r="C79" s="90"/>
       <c r="D79" s="55"/>
       <c r="E79" s="55"/>
       <c r="F79" s="60"/>
@@ -49691,8 +49695,8 @@
       <c r="H79" s="59"/>
     </row>
     <row r="80" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="89"/>
-      <c r="C80" s="90"/>
+      <c r="B80" s="87"/>
+      <c r="C80" s="88"/>
       <c r="D80" s="56"/>
       <c r="E80" s="56"/>
       <c r="F80" s="53"/>
@@ -49700,8 +49704,8 @@
       <c r="H80" s="58"/>
     </row>
     <row r="81" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="87"/>
-      <c r="C81" s="88"/>
+      <c r="B81" s="89"/>
+      <c r="C81" s="90"/>
       <c r="D81" s="55"/>
       <c r="E81" s="55"/>
       <c r="F81" s="60"/>
@@ -49709,8 +49713,8 @@
       <c r="H81" s="59"/>
     </row>
     <row r="82" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="89"/>
-      <c r="C82" s="90"/>
+      <c r="B82" s="87"/>
+      <c r="C82" s="88"/>
       <c r="D82" s="56"/>
       <c r="E82" s="56"/>
       <c r="F82" s="53"/>
@@ -49718,8 +49722,8 @@
       <c r="H82" s="58"/>
     </row>
     <row r="83" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="87"/>
-      <c r="C83" s="88"/>
+      <c r="B83" s="89"/>
+      <c r="C83" s="90"/>
       <c r="D83" s="55"/>
       <c r="E83" s="55"/>
       <c r="F83" s="60"/>
@@ -49727,8 +49731,8 @@
       <c r="H83" s="59"/>
     </row>
     <row r="84" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="89"/>
-      <c r="C84" s="90"/>
+      <c r="B84" s="87"/>
+      <c r="C84" s="88"/>
       <c r="D84" s="56"/>
       <c r="E84" s="56"/>
       <c r="F84" s="53"/>
@@ -49736,8 +49740,8 @@
       <c r="H84" s="58"/>
     </row>
     <row r="85" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="87"/>
-      <c r="C85" s="88"/>
+      <c r="B85" s="89"/>
+      <c r="C85" s="90"/>
       <c r="D85" s="55"/>
       <c r="E85" s="55"/>
       <c r="F85" s="60"/>
@@ -49745,8 +49749,8 @@
       <c r="H85" s="59"/>
     </row>
     <row r="86" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="89"/>
-      <c r="C86" s="90"/>
+      <c r="B86" s="87"/>
+      <c r="C86" s="88"/>
       <c r="D86" s="56"/>
       <c r="E86" s="56"/>
       <c r="F86" s="53"/>
@@ -49754,8 +49758,8 @@
       <c r="H86" s="58"/>
     </row>
     <row r="87" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="87"/>
-      <c r="C87" s="88"/>
+      <c r="B87" s="89"/>
+      <c r="C87" s="90"/>
       <c r="D87" s="55"/>
       <c r="E87" s="55"/>
       <c r="F87" s="60"/>
@@ -49763,8 +49767,8 @@
       <c r="H87" s="59"/>
     </row>
     <row r="88" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="89"/>
-      <c r="C88" s="90"/>
+      <c r="B88" s="87"/>
+      <c r="C88" s="88"/>
       <c r="D88" s="56"/>
       <c r="E88" s="56"/>
       <c r="F88" s="53"/>
@@ -49772,8 +49776,8 @@
       <c r="H88" s="58"/>
     </row>
     <row r="89" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="87"/>
-      <c r="C89" s="88"/>
+      <c r="B89" s="89"/>
+      <c r="C89" s="90"/>
       <c r="D89" s="55"/>
       <c r="E89" s="55"/>
       <c r="F89" s="60"/>
@@ -49781,8 +49785,8 @@
       <c r="H89" s="59"/>
     </row>
     <row r="90" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="89"/>
-      <c r="C90" s="90"/>
+      <c r="B90" s="87"/>
+      <c r="C90" s="88"/>
       <c r="D90" s="56"/>
       <c r="E90" s="56"/>
       <c r="F90" s="53"/>
@@ -49790,8 +49794,8 @@
       <c r="H90" s="58"/>
     </row>
     <row r="91" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="87"/>
-      <c r="C91" s="88"/>
+      <c r="B91" s="89"/>
+      <c r="C91" s="90"/>
       <c r="D91" s="55"/>
       <c r="E91" s="55"/>
       <c r="F91" s="60"/>
@@ -49799,8 +49803,8 @@
       <c r="H91" s="59"/>
     </row>
     <row r="92" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="89"/>
-      <c r="C92" s="90"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="88"/>
       <c r="D92" s="56"/>
       <c r="E92" s="56"/>
       <c r="F92" s="53"/>
@@ -49808,8 +49812,8 @@
       <c r="H92" s="58"/>
     </row>
     <row r="93" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="87"/>
-      <c r="C93" s="88"/>
+      <c r="B93" s="89"/>
+      <c r="C93" s="90"/>
       <c r="D93" s="55"/>
       <c r="E93" s="55"/>
       <c r="F93" s="60"/>
@@ -49817,8 +49821,8 @@
       <c r="H93" s="59"/>
     </row>
     <row r="94" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="89"/>
-      <c r="C94" s="90"/>
+      <c r="B94" s="87"/>
+      <c r="C94" s="88"/>
       <c r="D94" s="56"/>
       <c r="E94" s="56"/>
       <c r="F94" s="53"/>
@@ -49826,8 +49830,8 @@
       <c r="H94" s="58"/>
     </row>
     <row r="95" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="87"/>
-      <c r="C95" s="88"/>
+      <c r="B95" s="89"/>
+      <c r="C95" s="90"/>
       <c r="D95" s="55"/>
       <c r="E95" s="55"/>
       <c r="F95" s="60"/>
@@ -49835,8 +49839,8 @@
       <c r="H95" s="59"/>
     </row>
     <row r="96" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="89"/>
-      <c r="C96" s="90"/>
+      <c r="B96" s="87"/>
+      <c r="C96" s="88"/>
       <c r="D96" s="56"/>
       <c r="E96" s="56"/>
       <c r="F96" s="53"/>
@@ -49844,8 +49848,8 @@
       <c r="H96" s="58"/>
     </row>
     <row r="97" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="87"/>
-      <c r="C97" s="88"/>
+      <c r="B97" s="89"/>
+      <c r="C97" s="90"/>
       <c r="D97" s="55"/>
       <c r="E97" s="55"/>
       <c r="F97" s="60"/>
@@ -49853,8 +49857,8 @@
       <c r="H97" s="59"/>
     </row>
     <row r="98" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="89"/>
-      <c r="C98" s="90"/>
+      <c r="B98" s="87"/>
+      <c r="C98" s="88"/>
       <c r="D98" s="56"/>
       <c r="E98" s="56"/>
       <c r="F98" s="53"/>
@@ -49862,8 +49866,8 @@
       <c r="H98" s="58"/>
     </row>
     <row r="99" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="87"/>
-      <c r="C99" s="88"/>
+      <c r="B99" s="89"/>
+      <c r="C99" s="90"/>
       <c r="D99" s="55"/>
       <c r="E99" s="55"/>
       <c r="F99" s="60"/>
@@ -49871,8 +49875,8 @@
       <c r="H99" s="59"/>
     </row>
     <row r="100" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="89"/>
-      <c r="C100" s="90"/>
+      <c r="B100" s="87"/>
+      <c r="C100" s="88"/>
       <c r="D100" s="56"/>
       <c r="E100" s="56"/>
       <c r="F100" s="53"/>
@@ -49880,8 +49884,8 @@
       <c r="H100" s="58"/>
     </row>
     <row r="101" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="87"/>
-      <c r="C101" s="88"/>
+      <c r="B101" s="89"/>
+      <c r="C101" s="90"/>
       <c r="D101" s="55"/>
       <c r="E101" s="55"/>
       <c r="F101" s="60"/>
@@ -49889,8 +49893,8 @@
       <c r="H101" s="59"/>
     </row>
     <row r="102" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="89"/>
-      <c r="C102" s="90"/>
+      <c r="B102" s="87"/>
+      <c r="C102" s="88"/>
       <c r="D102" s="56"/>
       <c r="E102" s="56"/>
       <c r="F102" s="53"/>
@@ -49898,8 +49902,8 @@
       <c r="H102" s="58"/>
     </row>
     <row r="103" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="87"/>
-      <c r="C103" s="88"/>
+      <c r="B103" s="89"/>
+      <c r="C103" s="90"/>
       <c r="D103" s="55"/>
       <c r="E103" s="55"/>
       <c r="F103" s="60"/>
@@ -49907,8 +49911,8 @@
       <c r="H103" s="59"/>
     </row>
     <row r="104" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="89"/>
-      <c r="C104" s="90"/>
+      <c r="B104" s="87"/>
+      <c r="C104" s="88"/>
       <c r="D104" s="56"/>
       <c r="E104" s="56"/>
       <c r="F104" s="53"/>
@@ -49916,8 +49920,8 @@
       <c r="H104" s="58"/>
     </row>
     <row r="105" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="87"/>
-      <c r="C105" s="88"/>
+      <c r="B105" s="89"/>
+      <c r="C105" s="90"/>
       <c r="D105" s="55"/>
       <c r="E105" s="55"/>
       <c r="F105" s="60"/>
@@ -49925,8 +49929,8 @@
       <c r="H105" s="59"/>
     </row>
     <row r="106" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="89"/>
-      <c r="C106" s="90"/>
+      <c r="B106" s="87"/>
+      <c r="C106" s="88"/>
       <c r="D106" s="56"/>
       <c r="E106" s="56"/>
       <c r="F106" s="53"/>
@@ -49934,8 +49938,8 @@
       <c r="H106" s="58"/>
     </row>
     <row r="107" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="87"/>
-      <c r="C107" s="88"/>
+      <c r="B107" s="89"/>
+      <c r="C107" s="90"/>
       <c r="D107" s="55"/>
       <c r="E107" s="55"/>
       <c r="F107" s="60"/>
@@ -49943,8 +49947,8 @@
       <c r="H107" s="59"/>
     </row>
     <row r="108" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="89"/>
-      <c r="C108" s="90"/>
+      <c r="B108" s="87"/>
+      <c r="C108" s="88"/>
       <c r="D108" s="56"/>
       <c r="E108" s="56"/>
       <c r="F108" s="53"/>
@@ -49952,8 +49956,8 @@
       <c r="H108" s="58"/>
     </row>
     <row r="109" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="87"/>
-      <c r="C109" s="88"/>
+      <c r="B109" s="89"/>
+      <c r="C109" s="90"/>
       <c r="D109" s="55"/>
       <c r="E109" s="55"/>
       <c r="F109" s="60"/>
@@ -49961,8 +49965,8 @@
       <c r="H109" s="59"/>
     </row>
     <row r="110" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="89"/>
-      <c r="C110" s="90"/>
+      <c r="B110" s="87"/>
+      <c r="C110" s="88"/>
       <c r="D110" s="56"/>
       <c r="E110" s="56"/>
       <c r="F110" s="53"/>
@@ -49970,8 +49974,8 @@
       <c r="H110" s="58"/>
     </row>
     <row r="111" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="87"/>
-      <c r="C111" s="88"/>
+      <c r="B111" s="89"/>
+      <c r="C111" s="90"/>
       <c r="D111" s="55"/>
       <c r="E111" s="55"/>
       <c r="F111" s="60"/>
@@ -49979,8 +49983,8 @@
       <c r="H111" s="59"/>
     </row>
     <row r="112" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="89"/>
-      <c r="C112" s="90"/>
+      <c r="B112" s="87"/>
+      <c r="C112" s="88"/>
       <c r="D112" s="56"/>
       <c r="E112" s="56"/>
       <c r="F112" s="53"/>
@@ -49988,8 +49992,8 @@
       <c r="H112" s="58"/>
     </row>
     <row r="113" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="87"/>
-      <c r="C113" s="88"/>
+      <c r="B113" s="89"/>
+      <c r="C113" s="90"/>
       <c r="D113" s="55"/>
       <c r="E113" s="55"/>
       <c r="F113" s="60"/>
@@ -49997,8 +50001,8 @@
       <c r="H113" s="59"/>
     </row>
     <row r="114" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B114" s="89"/>
-      <c r="C114" s="90"/>
+      <c r="B114" s="87"/>
+      <c r="C114" s="88"/>
       <c r="D114" s="56"/>
       <c r="E114" s="56"/>
       <c r="F114" s="53"/>
@@ -50006,8 +50010,8 @@
       <c r="H114" s="58"/>
     </row>
     <row r="115" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="87"/>
-      <c r="C115" s="88"/>
+      <c r="B115" s="89"/>
+      <c r="C115" s="90"/>
       <c r="D115" s="55"/>
       <c r="E115" s="55"/>
       <c r="F115" s="60"/>
@@ -50015,8 +50019,8 @@
       <c r="H115" s="59"/>
     </row>
     <row r="116" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B116" s="89"/>
-      <c r="C116" s="90"/>
+      <c r="B116" s="87"/>
+      <c r="C116" s="88"/>
       <c r="D116" s="56"/>
       <c r="E116" s="56"/>
       <c r="F116" s="53"/>
@@ -50024,8 +50028,8 @@
       <c r="H116" s="58"/>
     </row>
     <row r="117" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B117" s="87"/>
-      <c r="C117" s="88"/>
+      <c r="B117" s="89"/>
+      <c r="C117" s="90"/>
       <c r="D117" s="55"/>
       <c r="E117" s="55"/>
       <c r="F117" s="60"/>
@@ -50033,8 +50037,8 @@
       <c r="H117" s="59"/>
     </row>
     <row r="118" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="89"/>
-      <c r="C118" s="90"/>
+      <c r="B118" s="87"/>
+      <c r="C118" s="88"/>
       <c r="D118" s="56"/>
       <c r="E118" s="56"/>
       <c r="F118" s="53"/>
@@ -50042,8 +50046,8 @@
       <c r="H118" s="58"/>
     </row>
     <row r="119" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B119" s="87"/>
-      <c r="C119" s="88"/>
+      <c r="B119" s="89"/>
+      <c r="C119" s="90"/>
       <c r="D119" s="55"/>
       <c r="E119" s="55"/>
       <c r="F119" s="60"/>
@@ -50051,8 +50055,8 @@
       <c r="H119" s="59"/>
     </row>
     <row r="120" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B120" s="89"/>
-      <c r="C120" s="90"/>
+      <c r="B120" s="87"/>
+      <c r="C120" s="88"/>
       <c r="D120" s="56"/>
       <c r="E120" s="56"/>
       <c r="F120" s="53"/>
@@ -50060,8 +50064,8 @@
       <c r="H120" s="58"/>
     </row>
     <row r="121" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="87"/>
-      <c r="C121" s="88"/>
+      <c r="B121" s="89"/>
+      <c r="C121" s="90"/>
       <c r="D121" s="55"/>
       <c r="E121" s="55"/>
       <c r="F121" s="60"/>
@@ -50069,8 +50073,8 @@
       <c r="H121" s="59"/>
     </row>
     <row r="122" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="89"/>
-      <c r="C122" s="90"/>
+      <c r="B122" s="87"/>
+      <c r="C122" s="88"/>
       <c r="D122" s="56"/>
       <c r="E122" s="56"/>
       <c r="F122" s="53"/>
@@ -50078,8 +50082,8 @@
       <c r="H122" s="58"/>
     </row>
     <row r="123" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="87"/>
-      <c r="C123" s="88"/>
+      <c r="B123" s="89"/>
+      <c r="C123" s="90"/>
       <c r="D123" s="55"/>
       <c r="E123" s="55"/>
       <c r="F123" s="60"/>
@@ -50087,8 +50091,8 @@
       <c r="H123" s="59"/>
     </row>
     <row r="124" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="89"/>
-      <c r="C124" s="90"/>
+      <c r="B124" s="87"/>
+      <c r="C124" s="88"/>
       <c r="D124" s="56"/>
       <c r="E124" s="56"/>
       <c r="F124" s="53"/>
@@ -50096,8 +50100,8 @@
       <c r="H124" s="58"/>
     </row>
     <row r="125" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="87"/>
-      <c r="C125" s="88"/>
+      <c r="B125" s="89"/>
+      <c r="C125" s="90"/>
       <c r="D125" s="55"/>
       <c r="E125" s="55"/>
       <c r="F125" s="60"/>
@@ -50105,8 +50109,8 @@
       <c r="H125" s="59"/>
     </row>
     <row r="126" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B126" s="89"/>
-      <c r="C126" s="90"/>
+      <c r="B126" s="87"/>
+      <c r="C126" s="88"/>
       <c r="D126" s="56"/>
       <c r="E126" s="56"/>
       <c r="F126" s="53"/>
@@ -50114,8 +50118,8 @@
       <c r="H126" s="58"/>
     </row>
     <row r="127" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="87"/>
-      <c r="C127" s="88"/>
+      <c r="B127" s="89"/>
+      <c r="C127" s="90"/>
       <c r="D127" s="55"/>
       <c r="E127" s="55"/>
       <c r="F127" s="60"/>
@@ -50123,8 +50127,8 @@
       <c r="H127" s="59"/>
     </row>
     <row r="128" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="89"/>
-      <c r="C128" s="90"/>
+      <c r="B128" s="87"/>
+      <c r="C128" s="88"/>
       <c r="D128" s="56"/>
       <c r="E128" s="56"/>
       <c r="F128" s="53"/>
@@ -50132,8 +50136,8 @@
       <c r="H128" s="58"/>
     </row>
     <row r="129" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B129" s="87"/>
-      <c r="C129" s="88"/>
+      <c r="B129" s="89"/>
+      <c r="C129" s="90"/>
       <c r="D129" s="55"/>
       <c r="E129" s="55"/>
       <c r="F129" s="60"/>
@@ -50141,8 +50145,8 @@
       <c r="H129" s="59"/>
     </row>
     <row r="130" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B130" s="89"/>
-      <c r="C130" s="90"/>
+      <c r="B130" s="87"/>
+      <c r="C130" s="88"/>
       <c r="D130" s="56"/>
       <c r="E130" s="56"/>
       <c r="F130" s="53"/>
@@ -50150,8 +50154,8 @@
       <c r="H130" s="58"/>
     </row>
     <row r="131" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B131" s="87"/>
-      <c r="C131" s="88"/>
+      <c r="B131" s="89"/>
+      <c r="C131" s="90"/>
       <c r="D131" s="55"/>
       <c r="E131" s="55"/>
       <c r="F131" s="60"/>
@@ -50159,8 +50163,8 @@
       <c r="H131" s="59"/>
     </row>
     <row r="132" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="89"/>
-      <c r="C132" s="90"/>
+      <c r="B132" s="87"/>
+      <c r="C132" s="88"/>
       <c r="D132" s="56"/>
       <c r="E132" s="56"/>
       <c r="F132" s="53"/>
@@ -50168,8 +50172,8 @@
       <c r="H132" s="58"/>
     </row>
     <row r="133" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="87"/>
-      <c r="C133" s="88"/>
+      <c r="B133" s="89"/>
+      <c r="C133" s="90"/>
       <c r="D133" s="55"/>
       <c r="E133" s="55"/>
       <c r="F133" s="60"/>
@@ -50177,8 +50181,8 @@
       <c r="H133" s="59"/>
     </row>
     <row r="134" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="89"/>
-      <c r="C134" s="90"/>
+      <c r="B134" s="87"/>
+      <c r="C134" s="88"/>
       <c r="D134" s="56"/>
       <c r="E134" s="56"/>
       <c r="F134" s="53"/>
@@ -50186,8 +50190,8 @@
       <c r="H134" s="58"/>
     </row>
     <row r="135" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B135" s="87"/>
-      <c r="C135" s="88"/>
+      <c r="B135" s="89"/>
+      <c r="C135" s="90"/>
       <c r="D135" s="55"/>
       <c r="E135" s="55"/>
       <c r="F135" s="60"/>
@@ -50195,8 +50199,8 @@
       <c r="H135" s="59"/>
     </row>
     <row r="136" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="89"/>
-      <c r="C136" s="90"/>
+      <c r="B136" s="87"/>
+      <c r="C136" s="88"/>
       <c r="D136" s="56"/>
       <c r="E136" s="56"/>
       <c r="F136" s="53"/>
@@ -50204,8 +50208,8 @@
       <c r="H136" s="58"/>
     </row>
     <row r="137" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="87"/>
-      <c r="C137" s="88"/>
+      <c r="B137" s="89"/>
+      <c r="C137" s="90"/>
       <c r="D137" s="55"/>
       <c r="E137" s="55"/>
       <c r="F137" s="60"/>
@@ -50213,8 +50217,8 @@
       <c r="H137" s="59"/>
     </row>
     <row r="138" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B138" s="89"/>
-      <c r="C138" s="90"/>
+      <c r="B138" s="87"/>
+      <c r="C138" s="88"/>
       <c r="D138" s="56"/>
       <c r="E138" s="56"/>
       <c r="F138" s="53"/>
@@ -50222,8 +50226,8 @@
       <c r="H138" s="58"/>
     </row>
     <row r="139" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B139" s="87"/>
-      <c r="C139" s="88"/>
+      <c r="B139" s="89"/>
+      <c r="C139" s="90"/>
       <c r="D139" s="55"/>
       <c r="E139" s="55"/>
       <c r="F139" s="60"/>
@@ -50231,8 +50235,8 @@
       <c r="H139" s="59"/>
     </row>
     <row r="140" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B140" s="89"/>
-      <c r="C140" s="90"/>
+      <c r="B140" s="87"/>
+      <c r="C140" s="88"/>
       <c r="D140" s="56"/>
       <c r="E140" s="56"/>
       <c r="F140" s="53"/>
@@ -50240,8 +50244,8 @@
       <c r="H140" s="58"/>
     </row>
     <row r="141" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B141" s="87"/>
-      <c r="C141" s="88"/>
+      <c r="B141" s="89"/>
+      <c r="C141" s="90"/>
       <c r="D141" s="55"/>
       <c r="E141" s="55"/>
       <c r="F141" s="60"/>
@@ -50249,8 +50253,8 @@
       <c r="H141" s="59"/>
     </row>
     <row r="142" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="89"/>
-      <c r="C142" s="90"/>
+      <c r="B142" s="87"/>
+      <c r="C142" s="88"/>
       <c r="D142" s="56"/>
       <c r="E142" s="56"/>
       <c r="F142" s="53"/>
@@ -50258,8 +50262,8 @@
       <c r="H142" s="58"/>
     </row>
     <row r="143" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B143" s="87"/>
-      <c r="C143" s="88"/>
+      <c r="B143" s="89"/>
+      <c r="C143" s="90"/>
       <c r="D143" s="55"/>
       <c r="E143" s="55"/>
       <c r="F143" s="60"/>
@@ -50267,8 +50271,8 @@
       <c r="H143" s="59"/>
     </row>
     <row r="144" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B144" s="89"/>
-      <c r="C144" s="90"/>
+      <c r="B144" s="87"/>
+      <c r="C144" s="88"/>
       <c r="D144" s="56"/>
       <c r="E144" s="56"/>
       <c r="F144" s="53"/>
@@ -50276,8 +50280,8 @@
       <c r="H144" s="58"/>
     </row>
     <row r="145" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B145" s="87"/>
-      <c r="C145" s="88"/>
+      <c r="B145" s="89"/>
+      <c r="C145" s="90"/>
       <c r="D145" s="55"/>
       <c r="E145" s="55"/>
       <c r="F145" s="60"/>
@@ -50285,8 +50289,8 @@
       <c r="H145" s="59"/>
     </row>
     <row r="146" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B146" s="89"/>
-      <c r="C146" s="90"/>
+      <c r="B146" s="87"/>
+      <c r="C146" s="88"/>
       <c r="D146" s="56"/>
       <c r="E146" s="56"/>
       <c r="F146" s="53"/>
@@ -50294,8 +50298,8 @@
       <c r="H146" s="58"/>
     </row>
     <row r="147" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B147" s="87"/>
-      <c r="C147" s="88"/>
+      <c r="B147" s="89"/>
+      <c r="C147" s="90"/>
       <c r="D147" s="55"/>
       <c r="E147" s="55"/>
       <c r="F147" s="60"/>
@@ -50303,8 +50307,8 @@
       <c r="H147" s="59"/>
     </row>
     <row r="148" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="89"/>
-      <c r="C148" s="90"/>
+      <c r="B148" s="87"/>
+      <c r="C148" s="88"/>
       <c r="D148" s="56"/>
       <c r="E148" s="56"/>
       <c r="F148" s="53"/>
@@ -50312,8 +50316,8 @@
       <c r="H148" s="58"/>
     </row>
     <row r="149" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B149" s="87"/>
-      <c r="C149" s="88"/>
+      <c r="B149" s="89"/>
+      <c r="C149" s="90"/>
       <c r="D149" s="55"/>
       <c r="E149" s="55"/>
       <c r="F149" s="60"/>
@@ -50321,8 +50325,8 @@
       <c r="H149" s="59"/>
     </row>
     <row r="150" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B150" s="89"/>
-      <c r="C150" s="90"/>
+      <c r="B150" s="87"/>
+      <c r="C150" s="88"/>
       <c r="D150" s="56"/>
       <c r="E150" s="56"/>
       <c r="F150" s="53"/>
@@ -50330,8 +50334,8 @@
       <c r="H150" s="58"/>
     </row>
     <row r="151" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="87"/>
-      <c r="C151" s="88"/>
+      <c r="B151" s="89"/>
+      <c r="C151" s="90"/>
       <c r="D151" s="55"/>
       <c r="E151" s="55"/>
       <c r="F151" s="60"/>
@@ -50339,8 +50343,8 @@
       <c r="H151" s="59"/>
     </row>
     <row r="152" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B152" s="89"/>
-      <c r="C152" s="90"/>
+      <c r="B152" s="87"/>
+      <c r="C152" s="88"/>
       <c r="D152" s="56"/>
       <c r="E152" s="56"/>
       <c r="F152" s="53"/>
@@ -50348,8 +50352,8 @@
       <c r="H152" s="58"/>
     </row>
     <row r="153" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B153" s="87"/>
-      <c r="C153" s="88"/>
+      <c r="B153" s="89"/>
+      <c r="C153" s="90"/>
       <c r="D153" s="55"/>
       <c r="E153" s="55"/>
       <c r="F153" s="60"/>
@@ -50357,8 +50361,8 @@
       <c r="H153" s="59"/>
     </row>
     <row r="154" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B154" s="89"/>
-      <c r="C154" s="90"/>
+      <c r="B154" s="87"/>
+      <c r="C154" s="88"/>
       <c r="D154" s="56"/>
       <c r="E154" s="56"/>
       <c r="F154" s="53"/>
@@ -50366,8 +50370,8 @@
       <c r="H154" s="58"/>
     </row>
     <row r="155" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B155" s="87"/>
-      <c r="C155" s="88"/>
+      <c r="B155" s="89"/>
+      <c r="C155" s="90"/>
       <c r="D155" s="55"/>
       <c r="E155" s="55"/>
       <c r="F155" s="60"/>
@@ -50375,8 +50379,8 @@
       <c r="H155" s="59"/>
     </row>
     <row r="156" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B156" s="89"/>
-      <c r="C156" s="90"/>
+      <c r="B156" s="87"/>
+      <c r="C156" s="88"/>
       <c r="D156" s="56"/>
       <c r="E156" s="56"/>
       <c r="F156" s="53"/>
@@ -50384,8 +50388,8 @@
       <c r="H156" s="58"/>
     </row>
     <row r="157" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B157" s="87"/>
-      <c r="C157" s="88"/>
+      <c r="B157" s="89"/>
+      <c r="C157" s="90"/>
       <c r="D157" s="55"/>
       <c r="E157" s="55"/>
       <c r="F157" s="60"/>
@@ -50393,8 +50397,8 @@
       <c r="H157" s="59"/>
     </row>
     <row r="158" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B158" s="89"/>
-      <c r="C158" s="90"/>
+      <c r="B158" s="87"/>
+      <c r="C158" s="88"/>
       <c r="D158" s="56"/>
       <c r="E158" s="56"/>
       <c r="F158" s="53"/>
@@ -50402,8 +50406,8 @@
       <c r="H158" s="58"/>
     </row>
     <row r="159" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B159" s="87"/>
-      <c r="C159" s="88"/>
+      <c r="B159" s="89"/>
+      <c r="C159" s="90"/>
       <c r="D159" s="55"/>
       <c r="E159" s="55"/>
       <c r="F159" s="60"/>
@@ -50411,8 +50415,8 @@
       <c r="H159" s="59"/>
     </row>
     <row r="160" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B160" s="89"/>
-      <c r="C160" s="90"/>
+      <c r="B160" s="87"/>
+      <c r="C160" s="88"/>
       <c r="D160" s="56"/>
       <c r="E160" s="56"/>
       <c r="F160" s="53"/>
@@ -50420,8 +50424,8 @@
       <c r="H160" s="58"/>
     </row>
     <row r="161" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B161" s="87"/>
-      <c r="C161" s="88"/>
+      <c r="B161" s="89"/>
+      <c r="C161" s="90"/>
       <c r="D161" s="55"/>
       <c r="E161" s="55"/>
       <c r="F161" s="60"/>
@@ -50429,8 +50433,8 @@
       <c r="H161" s="59"/>
     </row>
     <row r="162" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B162" s="89"/>
-      <c r="C162" s="90"/>
+      <c r="B162" s="87"/>
+      <c r="C162" s="88"/>
       <c r="D162" s="56"/>
       <c r="E162" s="56"/>
       <c r="F162" s="53"/>
@@ -50438,8 +50442,8 @@
       <c r="H162" s="58"/>
     </row>
     <row r="163" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B163" s="87"/>
-      <c r="C163" s="88"/>
+      <c r="B163" s="89"/>
+      <c r="C163" s="90"/>
       <c r="D163" s="55"/>
       <c r="E163" s="55"/>
       <c r="F163" s="60"/>
@@ -50447,8 +50451,8 @@
       <c r="H163" s="59"/>
     </row>
     <row r="164" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="89"/>
-      <c r="C164" s="90"/>
+      <c r="B164" s="87"/>
+      <c r="C164" s="88"/>
       <c r="D164" s="56"/>
       <c r="E164" s="56"/>
       <c r="F164" s="53"/>
@@ -50456,8 +50460,8 @@
       <c r="H164" s="58"/>
     </row>
     <row r="165" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B165" s="87"/>
-      <c r="C165" s="88"/>
+      <c r="B165" s="89"/>
+      <c r="C165" s="90"/>
       <c r="D165" s="55"/>
       <c r="E165" s="55"/>
       <c r="F165" s="60"/>
@@ -50465,8 +50469,8 @@
       <c r="H165" s="59"/>
     </row>
     <row r="166" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="89"/>
-      <c r="C166" s="90"/>
+      <c r="B166" s="87"/>
+      <c r="C166" s="88"/>
       <c r="D166" s="56"/>
       <c r="E166" s="56"/>
       <c r="F166" s="53"/>
@@ -50474,8 +50478,8 @@
       <c r="H166" s="58"/>
     </row>
     <row r="167" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B167" s="87"/>
-      <c r="C167" s="88"/>
+      <c r="B167" s="89"/>
+      <c r="C167" s="90"/>
       <c r="D167" s="55"/>
       <c r="E167" s="55"/>
       <c r="F167" s="60"/>
@@ -50483,8 +50487,8 @@
       <c r="H167" s="59"/>
     </row>
     <row r="168" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B168" s="89"/>
-      <c r="C168" s="90"/>
+      <c r="B168" s="87"/>
+      <c r="C168" s="88"/>
       <c r="D168" s="56"/>
       <c r="E168" s="56"/>
       <c r="F168" s="53"/>
@@ -50492,8 +50496,8 @@
       <c r="H168" s="58"/>
     </row>
     <row r="169" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B169" s="87"/>
-      <c r="C169" s="88"/>
+      <c r="B169" s="89"/>
+      <c r="C169" s="90"/>
       <c r="D169" s="55"/>
       <c r="E169" s="55"/>
       <c r="F169" s="60"/>
@@ -50501,8 +50505,8 @@
       <c r="H169" s="59"/>
     </row>
     <row r="170" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="89"/>
-      <c r="C170" s="90"/>
+      <c r="B170" s="87"/>
+      <c r="C170" s="88"/>
       <c r="D170" s="56"/>
       <c r="E170" s="56"/>
       <c r="F170" s="53"/>
@@ -50510,8 +50514,8 @@
       <c r="H170" s="58"/>
     </row>
     <row r="171" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B171" s="87"/>
-      <c r="C171" s="88"/>
+      <c r="B171" s="89"/>
+      <c r="C171" s="90"/>
       <c r="D171" s="55"/>
       <c r="E171" s="55"/>
       <c r="F171" s="60"/>
@@ -50519,8 +50523,8 @@
       <c r="H171" s="59"/>
     </row>
     <row r="172" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B172" s="89"/>
-      <c r="C172" s="90"/>
+      <c r="B172" s="87"/>
+      <c r="C172" s="88"/>
       <c r="D172" s="56"/>
       <c r="E172" s="56"/>
       <c r="F172" s="53"/>
@@ -50528,8 +50532,8 @@
       <c r="H172" s="58"/>
     </row>
     <row r="173" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B173" s="87"/>
-      <c r="C173" s="88"/>
+      <c r="B173" s="89"/>
+      <c r="C173" s="90"/>
       <c r="D173" s="55"/>
       <c r="E173" s="55"/>
       <c r="F173" s="60"/>
@@ -50537,8 +50541,8 @@
       <c r="H173" s="59"/>
     </row>
     <row r="174" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B174" s="89"/>
-      <c r="C174" s="90"/>
+      <c r="B174" s="87"/>
+      <c r="C174" s="88"/>
       <c r="D174" s="56"/>
       <c r="E174" s="56"/>
       <c r="F174" s="53"/>
@@ -50546,8 +50550,8 @@
       <c r="H174" s="58"/>
     </row>
     <row r="175" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B175" s="87"/>
-      <c r="C175" s="88"/>
+      <c r="B175" s="89"/>
+      <c r="C175" s="90"/>
       <c r="D175" s="55"/>
       <c r="E175" s="55"/>
       <c r="F175" s="60"/>
@@ -50555,8 +50559,8 @@
       <c r="H175" s="59"/>
     </row>
     <row r="176" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B176" s="89"/>
-      <c r="C176" s="90"/>
+      <c r="B176" s="87"/>
+      <c r="C176" s="88"/>
       <c r="D176" s="56"/>
       <c r="E176" s="56"/>
       <c r="F176" s="53"/>
@@ -50564,8 +50568,8 @@
       <c r="H176" s="58"/>
     </row>
     <row r="177" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B177" s="87"/>
-      <c r="C177" s="88"/>
+      <c r="B177" s="89"/>
+      <c r="C177" s="90"/>
       <c r="D177" s="55"/>
       <c r="E177" s="55"/>
       <c r="F177" s="60"/>
@@ -50573,8 +50577,8 @@
       <c r="H177" s="59"/>
     </row>
     <row r="178" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B178" s="89"/>
-      <c r="C178" s="90"/>
+      <c r="B178" s="87"/>
+      <c r="C178" s="88"/>
       <c r="D178" s="56"/>
       <c r="E178" s="56"/>
       <c r="F178" s="53"/>
@@ -50582,8 +50586,8 @@
       <c r="H178" s="58"/>
     </row>
     <row r="179" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B179" s="87"/>
-      <c r="C179" s="88"/>
+      <c r="B179" s="89"/>
+      <c r="C179" s="90"/>
       <c r="D179" s="55"/>
       <c r="E179" s="55"/>
       <c r="F179" s="60"/>
@@ -50591,8 +50595,8 @@
       <c r="H179" s="59"/>
     </row>
     <row r="180" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B180" s="89"/>
-      <c r="C180" s="90"/>
+      <c r="B180" s="87"/>
+      <c r="C180" s="88"/>
       <c r="D180" s="56"/>
       <c r="E180" s="56"/>
       <c r="F180" s="53"/>
@@ -50600,8 +50604,8 @@
       <c r="H180" s="58"/>
     </row>
     <row r="181" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B181" s="87"/>
-      <c r="C181" s="88"/>
+      <c r="B181" s="89"/>
+      <c r="C181" s="90"/>
       <c r="D181" s="55"/>
       <c r="E181" s="55"/>
       <c r="F181" s="60"/>
@@ -50609,8 +50613,8 @@
       <c r="H181" s="59"/>
     </row>
     <row r="182" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B182" s="89"/>
-      <c r="C182" s="90"/>
+      <c r="B182" s="87"/>
+      <c r="C182" s="88"/>
       <c r="D182" s="56"/>
       <c r="E182" s="56"/>
       <c r="F182" s="53"/>
@@ -50618,8 +50622,8 @@
       <c r="H182" s="58"/>
     </row>
     <row r="183" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B183" s="87"/>
-      <c r="C183" s="88"/>
+      <c r="B183" s="89"/>
+      <c r="C183" s="90"/>
       <c r="D183" s="55"/>
       <c r="E183" s="55"/>
       <c r="F183" s="60"/>
@@ -50627,8 +50631,8 @@
       <c r="H183" s="59"/>
     </row>
     <row r="184" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B184" s="89"/>
-      <c r="C184" s="90"/>
+      <c r="B184" s="87"/>
+      <c r="C184" s="88"/>
       <c r="D184" s="56"/>
       <c r="E184" s="56"/>
       <c r="F184" s="53"/>
@@ -50636,8 +50640,8 @@
       <c r="H184" s="58"/>
     </row>
     <row r="185" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B185" s="87"/>
-      <c r="C185" s="88"/>
+      <c r="B185" s="89"/>
+      <c r="C185" s="90"/>
       <c r="D185" s="55"/>
       <c r="E185" s="55"/>
       <c r="F185" s="60"/>
@@ -50645,8 +50649,8 @@
       <c r="H185" s="59"/>
     </row>
     <row r="186" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B186" s="89"/>
-      <c r="C186" s="90"/>
+      <c r="B186" s="87"/>
+      <c r="C186" s="88"/>
       <c r="D186" s="56"/>
       <c r="E186" s="56"/>
       <c r="F186" s="53"/>
@@ -50654,8 +50658,8 @@
       <c r="H186" s="58"/>
     </row>
     <row r="187" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B187" s="87"/>
-      <c r="C187" s="88"/>
+      <c r="B187" s="89"/>
+      <c r="C187" s="90"/>
       <c r="D187" s="55"/>
       <c r="E187" s="55"/>
       <c r="F187" s="60"/>
@@ -50663,8 +50667,8 @@
       <c r="H187" s="59"/>
     </row>
     <row r="188" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B188" s="89"/>
-      <c r="C188" s="90"/>
+      <c r="B188" s="87"/>
+      <c r="C188" s="88"/>
       <c r="D188" s="56"/>
       <c r="E188" s="56"/>
       <c r="F188" s="53"/>
@@ -50672,8 +50676,8 @@
       <c r="H188" s="58"/>
     </row>
     <row r="189" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B189" s="87"/>
-      <c r="C189" s="88"/>
+      <c r="B189" s="89"/>
+      <c r="C189" s="90"/>
       <c r="D189" s="55"/>
       <c r="E189" s="55"/>
       <c r="F189" s="60"/>
@@ -50681,8 +50685,8 @@
       <c r="H189" s="59"/>
     </row>
     <row r="190" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B190" s="89"/>
-      <c r="C190" s="90"/>
+      <c r="B190" s="87"/>
+      <c r="C190" s="88"/>
       <c r="D190" s="56"/>
       <c r="E190" s="56"/>
       <c r="F190" s="53"/>
@@ -50690,8 +50694,8 @@
       <c r="H190" s="58"/>
     </row>
     <row r="191" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B191" s="87"/>
-      <c r="C191" s="88"/>
+      <c r="B191" s="89"/>
+      <c r="C191" s="90"/>
       <c r="D191" s="55"/>
       <c r="E191" s="55"/>
       <c r="F191" s="60"/>
@@ -50699,8 +50703,8 @@
       <c r="H191" s="59"/>
     </row>
     <row r="192" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B192" s="89"/>
-      <c r="C192" s="90"/>
+      <c r="B192" s="87"/>
+      <c r="C192" s="88"/>
       <c r="D192" s="56"/>
       <c r="E192" s="56"/>
       <c r="F192" s="53"/>
@@ -50708,8 +50712,8 @@
       <c r="H192" s="58"/>
     </row>
     <row r="193" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B193" s="87"/>
-      <c r="C193" s="88"/>
+      <c r="B193" s="89"/>
+      <c r="C193" s="90"/>
       <c r="D193" s="55"/>
       <c r="E193" s="55"/>
       <c r="F193" s="60"/>
@@ -50717,8 +50721,8 @@
       <c r="H193" s="59"/>
     </row>
     <row r="194" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B194" s="89"/>
-      <c r="C194" s="90"/>
+      <c r="B194" s="87"/>
+      <c r="C194" s="88"/>
       <c r="D194" s="56"/>
       <c r="E194" s="56"/>
       <c r="F194" s="53"/>
@@ -50726,8 +50730,8 @@
       <c r="H194" s="58"/>
     </row>
     <row r="195" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B195" s="87"/>
-      <c r="C195" s="88"/>
+      <c r="B195" s="89"/>
+      <c r="C195" s="90"/>
       <c r="D195" s="55"/>
       <c r="E195" s="55"/>
       <c r="F195" s="60"/>
@@ -50735,8 +50739,8 @@
       <c r="H195" s="59"/>
     </row>
     <row r="196" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B196" s="89"/>
-      <c r="C196" s="90"/>
+      <c r="B196" s="87"/>
+      <c r="C196" s="88"/>
       <c r="D196" s="56"/>
       <c r="E196" s="56"/>
       <c r="F196" s="53"/>
@@ -50744,8 +50748,8 @@
       <c r="H196" s="58"/>
     </row>
     <row r="197" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B197" s="87"/>
-      <c r="C197" s="88"/>
+      <c r="B197" s="89"/>
+      <c r="C197" s="90"/>
       <c r="D197" s="55"/>
       <c r="E197" s="55"/>
       <c r="F197" s="60"/>
@@ -50753,8 +50757,8 @@
       <c r="H197" s="59"/>
     </row>
     <row r="198" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B198" s="89"/>
-      <c r="C198" s="90"/>
+      <c r="B198" s="87"/>
+      <c r="C198" s="88"/>
       <c r="D198" s="56"/>
       <c r="E198" s="56"/>
       <c r="F198" s="53"/>
@@ -50762,8 +50766,8 @@
       <c r="H198" s="58"/>
     </row>
     <row r="199" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B199" s="87"/>
-      <c r="C199" s="88"/>
+      <c r="B199" s="89"/>
+      <c r="C199" s="90"/>
       <c r="D199" s="55"/>
       <c r="E199" s="55"/>
       <c r="F199" s="60"/>
@@ -50771,8 +50775,8 @@
       <c r="H199" s="59"/>
     </row>
     <row r="200" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B200" s="89"/>
-      <c r="C200" s="90"/>
+      <c r="B200" s="87"/>
+      <c r="C200" s="88"/>
       <c r="D200" s="56"/>
       <c r="E200" s="56"/>
       <c r="F200" s="53"/>
@@ -50780,8 +50784,8 @@
       <c r="H200" s="58"/>
     </row>
     <row r="201" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="87"/>
-      <c r="C201" s="88"/>
+      <c r="B201" s="89"/>
+      <c r="C201" s="90"/>
       <c r="D201" s="55"/>
       <c r="E201" s="55"/>
       <c r="F201" s="60"/>
@@ -50789,8 +50793,8 @@
       <c r="H201" s="59"/>
     </row>
     <row r="202" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B202" s="89"/>
-      <c r="C202" s="90"/>
+      <c r="B202" s="87"/>
+      <c r="C202" s="88"/>
       <c r="D202" s="56"/>
       <c r="E202" s="56"/>
       <c r="F202" s="53"/>
@@ -50798,8 +50802,8 @@
       <c r="H202" s="58"/>
     </row>
     <row r="203" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B203" s="87"/>
-      <c r="C203" s="88"/>
+      <c r="B203" s="89"/>
+      <c r="C203" s="90"/>
       <c r="D203" s="55"/>
       <c r="E203" s="55"/>
       <c r="F203" s="60"/>
@@ -50807,8 +50811,8 @@
       <c r="H203" s="59"/>
     </row>
     <row r="204" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B204" s="89"/>
-      <c r="C204" s="90"/>
+      <c r="B204" s="87"/>
+      <c r="C204" s="88"/>
       <c r="D204" s="56"/>
       <c r="E204" s="56"/>
       <c r="F204" s="53"/>
@@ -50816,8 +50820,8 @@
       <c r="H204" s="58"/>
     </row>
     <row r="205" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B205" s="87"/>
-      <c r="C205" s="88"/>
+      <c r="B205" s="89"/>
+      <c r="C205" s="90"/>
       <c r="D205" s="55"/>
       <c r="E205" s="55"/>
       <c r="F205" s="60"/>
@@ -50825,8 +50829,8 @@
       <c r="H205" s="59"/>
     </row>
     <row r="206" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B206" s="89"/>
-      <c r="C206" s="90"/>
+      <c r="B206" s="87"/>
+      <c r="C206" s="88"/>
       <c r="D206" s="56"/>
       <c r="E206" s="56"/>
       <c r="F206" s="53"/>
@@ -50834,8 +50838,8 @@
       <c r="H206" s="58"/>
     </row>
     <row r="207" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B207" s="87"/>
-      <c r="C207" s="88"/>
+      <c r="B207" s="89"/>
+      <c r="C207" s="90"/>
       <c r="D207" s="55"/>
       <c r="E207" s="55"/>
       <c r="F207" s="60"/>
@@ -50843,8 +50847,8 @@
       <c r="H207" s="59"/>
     </row>
     <row r="208" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B208" s="89"/>
-      <c r="C208" s="90"/>
+      <c r="B208" s="87"/>
+      <c r="C208" s="88"/>
       <c r="D208" s="56"/>
       <c r="E208" s="56"/>
       <c r="F208" s="53"/>
@@ -50852,8 +50856,8 @@
       <c r="H208" s="58"/>
     </row>
     <row r="209" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B209" s="87"/>
-      <c r="C209" s="88"/>
+      <c r="B209" s="89"/>
+      <c r="C209" s="90"/>
       <c r="D209" s="55"/>
       <c r="E209" s="55"/>
       <c r="F209" s="60"/>
@@ -50861,8 +50865,8 @@
       <c r="H209" s="59"/>
     </row>
     <row r="210" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B210" s="89"/>
-      <c r="C210" s="90"/>
+      <c r="B210" s="87"/>
+      <c r="C210" s="88"/>
       <c r="D210" s="56"/>
       <c r="E210" s="56"/>
       <c r="F210" s="53"/>
@@ -50870,8 +50874,8 @@
       <c r="H210" s="58"/>
     </row>
     <row r="211" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B211" s="87"/>
-      <c r="C211" s="88"/>
+      <c r="B211" s="89"/>
+      <c r="C211" s="90"/>
       <c r="D211" s="55"/>
       <c r="E211" s="55"/>
       <c r="F211" s="60"/>
@@ -50879,8 +50883,8 @@
       <c r="H211" s="59"/>
     </row>
     <row r="212" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B212" s="89"/>
-      <c r="C212" s="90"/>
+      <c r="B212" s="87"/>
+      <c r="C212" s="88"/>
       <c r="D212" s="56"/>
       <c r="E212" s="56"/>
       <c r="F212" s="53"/>
@@ -50888,8 +50892,8 @@
       <c r="H212" s="58"/>
     </row>
     <row r="213" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B213" s="87"/>
-      <c r="C213" s="88"/>
+      <c r="B213" s="89"/>
+      <c r="C213" s="90"/>
       <c r="D213" s="55"/>
       <c r="E213" s="55"/>
       <c r="F213" s="60"/>
@@ -50897,8 +50901,8 @@
       <c r="H213" s="59"/>
     </row>
     <row r="214" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B214" s="89"/>
-      <c r="C214" s="90"/>
+      <c r="B214" s="87"/>
+      <c r="C214" s="88"/>
       <c r="D214" s="56"/>
       <c r="E214" s="56"/>
       <c r="F214" s="53"/>
@@ -50906,8 +50910,8 @@
       <c r="H214" s="58"/>
     </row>
     <row r="215" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B215" s="87"/>
-      <c r="C215" s="88"/>
+      <c r="B215" s="89"/>
+      <c r="C215" s="90"/>
       <c r="D215" s="55"/>
       <c r="E215" s="55"/>
       <c r="F215" s="60"/>
@@ -50915,8 +50919,8 @@
       <c r="H215" s="59"/>
     </row>
     <row r="216" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B216" s="89"/>
-      <c r="C216" s="90"/>
+      <c r="B216" s="87"/>
+      <c r="C216" s="88"/>
       <c r="D216" s="56"/>
       <c r="E216" s="56"/>
       <c r="F216" s="53"/>
@@ -50924,8 +50928,8 @@
       <c r="H216" s="58"/>
     </row>
     <row r="217" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B217" s="87"/>
-      <c r="C217" s="88"/>
+      <c r="B217" s="89"/>
+      <c r="C217" s="90"/>
       <c r="D217" s="55"/>
       <c r="E217" s="55"/>
       <c r="F217" s="60"/>
@@ -50933,8 +50937,8 @@
       <c r="H217" s="59"/>
     </row>
     <row r="218" spans="2:8" s="8" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B218" s="89"/>
-      <c r="C218" s="90"/>
+      <c r="B218" s="87"/>
+      <c r="C218" s="88"/>
       <c r="D218" s="56"/>
       <c r="E218" s="56"/>
       <c r="F218" s="53"/>
@@ -50942,8 +50946,8 @@
       <c r="H218" s="58"/>
     </row>
     <row r="219" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="87"/>
-      <c r="C219" s="88"/>
+      <c r="B219" s="89"/>
+      <c r="C219" s="90"/>
       <c r="D219" s="55"/>
       <c r="E219" s="55"/>
       <c r="F219" s="60"/>
@@ -50951,8 +50955,8 @@
       <c r="H219" s="59"/>
     </row>
     <row r="220" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B220" s="89"/>
-      <c r="C220" s="90"/>
+      <c r="B220" s="87"/>
+      <c r="C220" s="88"/>
       <c r="D220" s="56"/>
       <c r="E220" s="56"/>
       <c r="F220" s="53"/>
@@ -50960,8 +50964,8 @@
       <c r="H220" s="58"/>
     </row>
     <row r="221" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="87"/>
-      <c r="C221" s="88"/>
+      <c r="B221" s="89"/>
+      <c r="C221" s="90"/>
       <c r="D221" s="55"/>
       <c r="E221" s="55"/>
       <c r="F221" s="60"/>
@@ -50969,8 +50973,8 @@
       <c r="H221" s="59"/>
     </row>
     <row r="222" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="89"/>
-      <c r="C222" s="90"/>
+      <c r="B222" s="87"/>
+      <c r="C222" s="88"/>
       <c r="D222" s="56"/>
       <c r="E222" s="56"/>
       <c r="F222" s="53"/>
@@ -50978,8 +50982,8 @@
       <c r="H222" s="58"/>
     </row>
     <row r="223" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="87"/>
-      <c r="C223" s="88"/>
+      <c r="B223" s="89"/>
+      <c r="C223" s="90"/>
       <c r="D223" s="55"/>
       <c r="E223" s="55"/>
       <c r="F223" s="60"/>
@@ -50987,8 +50991,8 @@
       <c r="H223" s="59"/>
     </row>
     <row r="224" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="89"/>
-      <c r="C224" s="90"/>
+      <c r="B224" s="87"/>
+      <c r="C224" s="88"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
       <c r="F224" s="53"/>
@@ -50996,8 +51000,8 @@
       <c r="H224" s="58"/>
     </row>
     <row r="225" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="87"/>
-      <c r="C225" s="88"/>
+      <c r="B225" s="89"/>
+      <c r="C225" s="90"/>
       <c r="D225" s="55"/>
       <c r="E225" s="55"/>
       <c r="F225" s="60"/>
@@ -51005,8 +51009,8 @@
       <c r="H225" s="59"/>
     </row>
     <row r="226" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="89"/>
-      <c r="C226" s="90"/>
+      <c r="B226" s="87"/>
+      <c r="C226" s="88"/>
       <c r="D226" s="56"/>
       <c r="E226" s="56"/>
       <c r="F226" s="53"/>
@@ -51014,8 +51018,8 @@
       <c r="H226" s="58"/>
     </row>
     <row r="227" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="87"/>
-      <c r="C227" s="88"/>
+      <c r="B227" s="89"/>
+      <c r="C227" s="90"/>
       <c r="D227" s="55"/>
       <c r="E227" s="55"/>
       <c r="F227" s="60"/>
@@ -51023,8 +51027,8 @@
       <c r="H227" s="59"/>
     </row>
     <row r="228" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="89"/>
-      <c r="C228" s="90"/>
+      <c r="B228" s="87"/>
+      <c r="C228" s="88"/>
       <c r="D228" s="56"/>
       <c r="E228" s="56"/>
       <c r="F228" s="53"/>
@@ -51032,8 +51036,8 @@
       <c r="H228" s="58"/>
     </row>
     <row r="229" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="87"/>
-      <c r="C229" s="88"/>
+      <c r="B229" s="89"/>
+      <c r="C229" s="90"/>
       <c r="D229" s="55"/>
       <c r="E229" s="55"/>
       <c r="F229" s="60"/>
@@ -51041,8 +51045,8 @@
       <c r="H229" s="59"/>
     </row>
     <row r="230" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="89"/>
-      <c r="C230" s="90"/>
+      <c r="B230" s="87"/>
+      <c r="C230" s="88"/>
       <c r="D230" s="56"/>
       <c r="E230" s="56"/>
       <c r="F230" s="53"/>
@@ -51050,8 +51054,8 @@
       <c r="H230" s="58"/>
     </row>
     <row r="231" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="87"/>
-      <c r="C231" s="88"/>
+      <c r="B231" s="89"/>
+      <c r="C231" s="90"/>
       <c r="D231" s="55"/>
       <c r="E231" s="55"/>
       <c r="F231" s="60"/>
@@ -51059,8 +51063,8 @@
       <c r="H231" s="59"/>
     </row>
     <row r="232" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="89"/>
-      <c r="C232" s="90"/>
+      <c r="B232" s="87"/>
+      <c r="C232" s="88"/>
       <c r="D232" s="56"/>
       <c r="E232" s="56"/>
       <c r="F232" s="53"/>
@@ -51068,8 +51072,8 @@
       <c r="H232" s="58"/>
     </row>
     <row r="233" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="87"/>
-      <c r="C233" s="88"/>
+      <c r="B233" s="89"/>
+      <c r="C233" s="90"/>
       <c r="D233" s="55"/>
       <c r="E233" s="55"/>
       <c r="F233" s="60"/>
@@ -51077,8 +51081,8 @@
       <c r="H233" s="59"/>
     </row>
     <row r="234" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B234" s="89"/>
-      <c r="C234" s="90"/>
+      <c r="B234" s="87"/>
+      <c r="C234" s="88"/>
       <c r="D234" s="56"/>
       <c r="E234" s="56"/>
       <c r="F234" s="53"/>
@@ -51086,8 +51090,8 @@
       <c r="H234" s="58"/>
     </row>
     <row r="235" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B235" s="87"/>
-      <c r="C235" s="88"/>
+      <c r="B235" s="89"/>
+      <c r="C235" s="90"/>
       <c r="D235" s="55"/>
       <c r="E235" s="55"/>
       <c r="F235" s="60"/>
@@ -51095,8 +51099,8 @@
       <c r="H235" s="59"/>
     </row>
     <row r="236" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B236" s="89"/>
-      <c r="C236" s="90"/>
+      <c r="B236" s="87"/>
+      <c r="C236" s="88"/>
       <c r="D236" s="56"/>
       <c r="E236" s="56"/>
       <c r="F236" s="53"/>
@@ -51104,8 +51108,8 @@
       <c r="H236" s="58"/>
     </row>
     <row r="237" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="87"/>
-      <c r="C237" s="88"/>
+      <c r="B237" s="89"/>
+      <c r="C237" s="90"/>
       <c r="D237" s="55"/>
       <c r="E237" s="55"/>
       <c r="F237" s="60"/>
@@ -51113,8 +51117,8 @@
       <c r="H237" s="59"/>
     </row>
     <row r="238" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="89"/>
-      <c r="C238" s="90"/>
+      <c r="B238" s="87"/>
+      <c r="C238" s="88"/>
       <c r="D238" s="56"/>
       <c r="E238" s="56"/>
       <c r="F238" s="53"/>
@@ -51122,8 +51126,8 @@
       <c r="H238" s="58"/>
     </row>
     <row r="239" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="87"/>
-      <c r="C239" s="88"/>
+      <c r="B239" s="89"/>
+      <c r="C239" s="90"/>
       <c r="D239" s="55"/>
       <c r="E239" s="55"/>
       <c r="F239" s="60"/>
@@ -51131,8 +51135,8 @@
       <c r="H239" s="59"/>
     </row>
     <row r="240" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B240" s="89"/>
-      <c r="C240" s="90"/>
+      <c r="B240" s="87"/>
+      <c r="C240" s="88"/>
       <c r="D240" s="56"/>
       <c r="E240" s="56"/>
       <c r="F240" s="53"/>
@@ -51140,8 +51144,8 @@
       <c r="H240" s="58"/>
     </row>
     <row r="241" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="87"/>
-      <c r="C241" s="88"/>
+      <c r="B241" s="89"/>
+      <c r="C241" s="90"/>
       <c r="D241" s="55"/>
       <c r="E241" s="55"/>
       <c r="F241" s="60"/>
@@ -51149,8 +51153,8 @@
       <c r="H241" s="59"/>
     </row>
     <row r="242" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="89"/>
-      <c r="C242" s="90"/>
+      <c r="B242" s="87"/>
+      <c r="C242" s="88"/>
       <c r="D242" s="56"/>
       <c r="E242" s="56"/>
       <c r="F242" s="53"/>
@@ -51158,8 +51162,8 @@
       <c r="H242" s="58"/>
     </row>
     <row r="243" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="87"/>
-      <c r="C243" s="88"/>
+      <c r="B243" s="89"/>
+      <c r="C243" s="90"/>
       <c r="D243" s="55"/>
       <c r="E243" s="55"/>
       <c r="F243" s="60"/>
@@ -51167,8 +51171,8 @@
       <c r="H243" s="59"/>
     </row>
     <row r="244" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="89"/>
-      <c r="C244" s="90"/>
+      <c r="B244" s="87"/>
+      <c r="C244" s="88"/>
       <c r="D244" s="56"/>
       <c r="E244" s="56"/>
       <c r="F244" s="53"/>
@@ -51176,8 +51180,8 @@
       <c r="H244" s="58"/>
     </row>
     <row r="245" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="87"/>
-      <c r="C245" s="88"/>
+      <c r="B245" s="89"/>
+      <c r="C245" s="90"/>
       <c r="D245" s="55"/>
       <c r="E245" s="55"/>
       <c r="F245" s="60"/>
@@ -51185,8 +51189,8 @@
       <c r="H245" s="59"/>
     </row>
     <row r="246" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="89"/>
-      <c r="C246" s="90"/>
+      <c r="B246" s="87"/>
+      <c r="C246" s="88"/>
       <c r="D246" s="56"/>
       <c r="E246" s="56"/>
       <c r="F246" s="53"/>
@@ -51194,8 +51198,8 @@
       <c r="H246" s="58"/>
     </row>
     <row r="247" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="87"/>
-      <c r="C247" s="88"/>
+      <c r="B247" s="89"/>
+      <c r="C247" s="90"/>
       <c r="D247" s="55"/>
       <c r="E247" s="55"/>
       <c r="F247" s="60"/>
@@ -51203,8 +51207,8 @@
       <c r="H247" s="59"/>
     </row>
     <row r="248" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="89"/>
-      <c r="C248" s="90"/>
+      <c r="B248" s="87"/>
+      <c r="C248" s="88"/>
       <c r="D248" s="56"/>
       <c r="E248" s="56"/>
       <c r="F248" s="53"/>
@@ -51212,8 +51216,8 @@
       <c r="H248" s="58"/>
     </row>
     <row r="249" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="87"/>
-      <c r="C249" s="88"/>
+      <c r="B249" s="89"/>
+      <c r="C249" s="90"/>
       <c r="D249" s="55"/>
       <c r="E249" s="55"/>
       <c r="F249" s="60"/>
@@ -51221,8 +51225,8 @@
       <c r="H249" s="59"/>
     </row>
     <row r="250" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="89"/>
-      <c r="C250" s="90"/>
+      <c r="B250" s="87"/>
+      <c r="C250" s="88"/>
       <c r="D250" s="56"/>
       <c r="E250" s="56"/>
       <c r="F250" s="53"/>
@@ -51230,8 +51234,8 @@
       <c r="H250" s="58"/>
     </row>
     <row r="251" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="87"/>
-      <c r="C251" s="88"/>
+      <c r="B251" s="89"/>
+      <c r="C251" s="90"/>
       <c r="D251" s="55"/>
       <c r="E251" s="55"/>
       <c r="F251" s="60"/>
@@ -51239,8 +51243,8 @@
       <c r="H251" s="59"/>
     </row>
     <row r="252" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B252" s="89"/>
-      <c r="C252" s="90"/>
+      <c r="B252" s="87"/>
+      <c r="C252" s="88"/>
       <c r="D252" s="56"/>
       <c r="E252" s="56"/>
       <c r="F252" s="53"/>
@@ -51248,8 +51252,8 @@
       <c r="H252" s="58"/>
     </row>
     <row r="253" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="87"/>
-      <c r="C253" s="88"/>
+      <c r="B253" s="89"/>
+      <c r="C253" s="90"/>
       <c r="D253" s="55"/>
       <c r="E253" s="55"/>
       <c r="F253" s="60"/>
@@ -51257,8 +51261,8 @@
       <c r="H253" s="59"/>
     </row>
     <row r="254" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="89"/>
-      <c r="C254" s="90"/>
+      <c r="B254" s="87"/>
+      <c r="C254" s="88"/>
       <c r="D254" s="56"/>
       <c r="E254" s="56"/>
       <c r="F254" s="53"/>
@@ -51266,8 +51270,8 @@
       <c r="H254" s="58"/>
     </row>
     <row r="255" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B255" s="87"/>
-      <c r="C255" s="88"/>
+      <c r="B255" s="89"/>
+      <c r="C255" s="90"/>
       <c r="D255" s="55"/>
       <c r="E255" s="55"/>
       <c r="F255" s="60"/>
@@ -51275,8 +51279,8 @@
       <c r="H255" s="59"/>
     </row>
     <row r="256" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B256" s="89"/>
-      <c r="C256" s="90"/>
+      <c r="B256" s="87"/>
+      <c r="C256" s="88"/>
       <c r="D256" s="56"/>
       <c r="E256" s="56"/>
       <c r="F256" s="53"/>
@@ -51284,8 +51288,8 @@
       <c r="H256" s="58"/>
     </row>
     <row r="257" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="87"/>
-      <c r="C257" s="88"/>
+      <c r="B257" s="89"/>
+      <c r="C257" s="90"/>
       <c r="D257" s="55"/>
       <c r="E257" s="55"/>
       <c r="F257" s="60"/>
@@ -51293,8 +51297,8 @@
       <c r="H257" s="59"/>
     </row>
     <row r="258" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="89"/>
-      <c r="C258" s="90"/>
+      <c r="B258" s="87"/>
+      <c r="C258" s="88"/>
       <c r="D258" s="56"/>
       <c r="E258" s="56"/>
       <c r="F258" s="53"/>
@@ -51302,8 +51306,8 @@
       <c r="H258" s="58"/>
     </row>
     <row r="259" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="87"/>
-      <c r="C259" s="88"/>
+      <c r="B259" s="89"/>
+      <c r="C259" s="90"/>
       <c r="D259" s="55"/>
       <c r="E259" s="55"/>
       <c r="F259" s="60"/>
@@ -51311,8 +51315,8 @@
       <c r="H259" s="59"/>
     </row>
     <row r="260" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="89"/>
-      <c r="C260" s="90"/>
+      <c r="B260" s="87"/>
+      <c r="C260" s="88"/>
       <c r="D260" s="56"/>
       <c r="E260" s="56"/>
       <c r="F260" s="53"/>
@@ -51320,8 +51324,8 @@
       <c r="H260" s="58"/>
     </row>
     <row r="261" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="87"/>
-      <c r="C261" s="88"/>
+      <c r="B261" s="89"/>
+      <c r="C261" s="90"/>
       <c r="D261" s="55"/>
       <c r="E261" s="55"/>
       <c r="F261" s="60"/>
@@ -51329,8 +51333,8 @@
       <c r="H261" s="59"/>
     </row>
     <row r="262" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="89"/>
-      <c r="C262" s="90"/>
+      <c r="B262" s="87"/>
+      <c r="C262" s="88"/>
       <c r="D262" s="56"/>
       <c r="E262" s="56"/>
       <c r="F262" s="53"/>
@@ -51338,8 +51342,8 @@
       <c r="H262" s="58"/>
     </row>
     <row r="263" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="87"/>
-      <c r="C263" s="88"/>
+      <c r="B263" s="89"/>
+      <c r="C263" s="90"/>
       <c r="D263" s="55"/>
       <c r="E263" s="55"/>
       <c r="F263" s="60"/>
@@ -51347,8 +51351,8 @@
       <c r="H263" s="59"/>
     </row>
     <row r="264" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="89"/>
-      <c r="C264" s="90"/>
+      <c r="B264" s="87"/>
+      <c r="C264" s="88"/>
       <c r="D264" s="56"/>
       <c r="E264" s="56"/>
       <c r="F264" s="53"/>
@@ -51356,8 +51360,8 @@
       <c r="H264" s="58"/>
     </row>
     <row r="265" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="87"/>
-      <c r="C265" s="88"/>
+      <c r="B265" s="89"/>
+      <c r="C265" s="90"/>
       <c r="D265" s="55"/>
       <c r="E265" s="55"/>
       <c r="F265" s="60"/>
@@ -51365,8 +51369,8 @@
       <c r="H265" s="59"/>
     </row>
     <row r="266" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="89"/>
-      <c r="C266" s="90"/>
+      <c r="B266" s="87"/>
+      <c r="C266" s="88"/>
       <c r="D266" s="56"/>
       <c r="E266" s="56"/>
       <c r="F266" s="53"/>
@@ -51374,8 +51378,8 @@
       <c r="H266" s="58"/>
     </row>
     <row r="267" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B267" s="87"/>
-      <c r="C267" s="88"/>
+      <c r="B267" s="89"/>
+      <c r="C267" s="90"/>
       <c r="D267" s="55"/>
       <c r="E267" s="55"/>
       <c r="F267" s="60"/>
@@ -51383,8 +51387,8 @@
       <c r="H267" s="59"/>
     </row>
     <row r="268" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B268" s="89"/>
-      <c r="C268" s="90"/>
+      <c r="B268" s="87"/>
+      <c r="C268" s="88"/>
       <c r="D268" s="56"/>
       <c r="E268" s="56"/>
       <c r="F268" s="53"/>
@@ -51392,8 +51396,8 @@
       <c r="H268" s="58"/>
     </row>
     <row r="269" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B269" s="87"/>
-      <c r="C269" s="88"/>
+      <c r="B269" s="89"/>
+      <c r="C269" s="90"/>
       <c r="D269" s="55"/>
       <c r="E269" s="55"/>
       <c r="F269" s="60"/>
@@ -51401,8 +51405,8 @@
       <c r="H269" s="59"/>
     </row>
     <row r="270" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B270" s="89"/>
-      <c r="C270" s="90"/>
+      <c r="B270" s="87"/>
+      <c r="C270" s="88"/>
       <c r="D270" s="56"/>
       <c r="E270" s="56"/>
       <c r="F270" s="53"/>
@@ -51410,8 +51414,8 @@
       <c r="H270" s="58"/>
     </row>
     <row r="271" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="87"/>
-      <c r="C271" s="88"/>
+      <c r="B271" s="89"/>
+      <c r="C271" s="90"/>
       <c r="D271" s="55"/>
       <c r="E271" s="55"/>
       <c r="F271" s="60"/>
@@ -51419,8 +51423,8 @@
       <c r="H271" s="59"/>
     </row>
     <row r="272" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="89"/>
-      <c r="C272" s="90"/>
+      <c r="B272" s="87"/>
+      <c r="C272" s="88"/>
       <c r="D272" s="56"/>
       <c r="E272" s="56"/>
       <c r="F272" s="53"/>
@@ -51428,8 +51432,8 @@
       <c r="H272" s="58"/>
     </row>
     <row r="273" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="87"/>
-      <c r="C273" s="88"/>
+      <c r="B273" s="89"/>
+      <c r="C273" s="90"/>
       <c r="D273" s="55"/>
       <c r="E273" s="55"/>
       <c r="F273" s="60"/>
@@ -51437,8 +51441,8 @@
       <c r="H273" s="59"/>
     </row>
     <row r="274" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="89"/>
-      <c r="C274" s="90"/>
+      <c r="B274" s="87"/>
+      <c r="C274" s="88"/>
       <c r="D274" s="56"/>
       <c r="E274" s="56"/>
       <c r="F274" s="53"/>
@@ -51446,8 +51450,8 @@
       <c r="H274" s="58"/>
     </row>
     <row r="275" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="87"/>
-      <c r="C275" s="88"/>
+      <c r="B275" s="89"/>
+      <c r="C275" s="90"/>
       <c r="D275" s="55"/>
       <c r="E275" s="55"/>
       <c r="F275" s="60"/>
@@ -51455,8 +51459,8 @@
       <c r="H275" s="59"/>
     </row>
     <row r="276" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="89"/>
-      <c r="C276" s="90"/>
+      <c r="B276" s="87"/>
+      <c r="C276" s="88"/>
       <c r="D276" s="56"/>
       <c r="E276" s="56"/>
       <c r="F276" s="53"/>
@@ -51464,8 +51468,8 @@
       <c r="H276" s="58"/>
     </row>
     <row r="277" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B277" s="87"/>
-      <c r="C277" s="88"/>
+      <c r="B277" s="89"/>
+      <c r="C277" s="90"/>
       <c r="D277" s="55"/>
       <c r="E277" s="55"/>
       <c r="F277" s="60"/>
@@ -51473,8 +51477,8 @@
       <c r="H277" s="59"/>
     </row>
     <row r="278" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B278" s="89"/>
-      <c r="C278" s="90"/>
+      <c r="B278" s="87"/>
+      <c r="C278" s="88"/>
       <c r="D278" s="56"/>
       <c r="E278" s="56"/>
       <c r="F278" s="53"/>
@@ -51482,8 +51486,8 @@
       <c r="H278" s="58"/>
     </row>
     <row r="279" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="87"/>
-      <c r="C279" s="88"/>
+      <c r="B279" s="89"/>
+      <c r="C279" s="90"/>
       <c r="D279" s="55"/>
       <c r="E279" s="55"/>
       <c r="F279" s="60"/>
@@ -51491,8 +51495,8 @@
       <c r="H279" s="59"/>
     </row>
     <row r="280" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="89"/>
-      <c r="C280" s="90"/>
+      <c r="B280" s="87"/>
+      <c r="C280" s="88"/>
       <c r="D280" s="56"/>
       <c r="E280" s="56"/>
       <c r="F280" s="53"/>
@@ -51500,8 +51504,8 @@
       <c r="H280" s="58"/>
     </row>
     <row r="281" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B281" s="87"/>
-      <c r="C281" s="88"/>
+      <c r="B281" s="89"/>
+      <c r="C281" s="90"/>
       <c r="D281" s="55"/>
       <c r="E281" s="55"/>
       <c r="F281" s="60"/>
@@ -51509,8 +51513,8 @@
       <c r="H281" s="59"/>
     </row>
     <row r="282" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B282" s="89"/>
-      <c r="C282" s="90"/>
+      <c r="B282" s="87"/>
+      <c r="C282" s="88"/>
       <c r="D282" s="56"/>
       <c r="E282" s="56"/>
       <c r="F282" s="53"/>
@@ -51518,8 +51522,8 @@
       <c r="H282" s="58"/>
     </row>
     <row r="283" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="87"/>
-      <c r="C283" s="88"/>
+      <c r="B283" s="89"/>
+      <c r="C283" s="90"/>
       <c r="D283" s="55"/>
       <c r="E283" s="55"/>
       <c r="F283" s="60"/>
@@ -51527,8 +51531,8 @@
       <c r="H283" s="59"/>
     </row>
     <row r="284" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="89"/>
-      <c r="C284" s="90"/>
+      <c r="B284" s="87"/>
+      <c r="C284" s="88"/>
       <c r="D284" s="56"/>
       <c r="E284" s="56"/>
       <c r="F284" s="53"/>
@@ -51536,8 +51540,8 @@
       <c r="H284" s="58"/>
     </row>
     <row r="285" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B285" s="87"/>
-      <c r="C285" s="88"/>
+      <c r="B285" s="89"/>
+      <c r="C285" s="90"/>
       <c r="D285" s="55"/>
       <c r="E285" s="55"/>
       <c r="F285" s="60"/>
@@ -51545,8 +51549,8 @@
       <c r="H285" s="59"/>
     </row>
     <row r="286" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="89"/>
-      <c r="C286" s="90"/>
+      <c r="B286" s="87"/>
+      <c r="C286" s="88"/>
       <c r="D286" s="56"/>
       <c r="E286" s="56"/>
       <c r="F286" s="53"/>
@@ -51554,8 +51558,8 @@
       <c r="H286" s="58"/>
     </row>
     <row r="287" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="87"/>
-      <c r="C287" s="88"/>
+      <c r="B287" s="89"/>
+      <c r="C287" s="90"/>
       <c r="D287" s="55"/>
       <c r="E287" s="55"/>
       <c r="F287" s="60"/>
@@ -51563,8 +51567,8 @@
       <c r="H287" s="59"/>
     </row>
     <row r="288" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="89"/>
-      <c r="C288" s="90"/>
+      <c r="B288" s="87"/>
+      <c r="C288" s="88"/>
       <c r="D288" s="56"/>
       <c r="E288" s="56"/>
       <c r="F288" s="53"/>
@@ -51572,8 +51576,8 @@
       <c r="H288" s="58"/>
     </row>
     <row r="289" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="87"/>
-      <c r="C289" s="88"/>
+      <c r="B289" s="89"/>
+      <c r="C289" s="90"/>
       <c r="D289" s="55"/>
       <c r="E289" s="55"/>
       <c r="F289" s="60"/>
@@ -51581,8 +51585,8 @@
       <c r="H289" s="59"/>
     </row>
     <row r="290" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B290" s="89"/>
-      <c r="C290" s="90"/>
+      <c r="B290" s="87"/>
+      <c r="C290" s="88"/>
       <c r="D290" s="56"/>
       <c r="E290" s="56"/>
       <c r="F290" s="53"/>
@@ -51590,8 +51594,8 @@
       <c r="H290" s="58"/>
     </row>
     <row r="291" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B291" s="87"/>
-      <c r="C291" s="88"/>
+      <c r="B291" s="89"/>
+      <c r="C291" s="90"/>
       <c r="D291" s="55"/>
       <c r="E291" s="55"/>
       <c r="F291" s="60"/>
@@ -51599,8 +51603,8 @@
       <c r="H291" s="59"/>
     </row>
     <row r="292" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B292" s="89"/>
-      <c r="C292" s="90"/>
+      <c r="B292" s="87"/>
+      <c r="C292" s="88"/>
       <c r="D292" s="56"/>
       <c r="E292" s="56"/>
       <c r="F292" s="53"/>
@@ -51608,8 +51612,8 @@
       <c r="H292" s="58"/>
     </row>
     <row r="293" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B293" s="87"/>
-      <c r="C293" s="88"/>
+      <c r="B293" s="89"/>
+      <c r="C293" s="90"/>
       <c r="D293" s="55"/>
       <c r="E293" s="55"/>
       <c r="F293" s="60"/>
@@ -51617,8 +51621,8 @@
       <c r="H293" s="59"/>
     </row>
     <row r="294" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B294" s="89"/>
-      <c r="C294" s="90"/>
+      <c r="B294" s="87"/>
+      <c r="C294" s="88"/>
       <c r="D294" s="56"/>
       <c r="E294" s="56"/>
       <c r="F294" s="53"/>
@@ -51626,8 +51630,8 @@
       <c r="H294" s="58"/>
     </row>
     <row r="295" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B295" s="87"/>
-      <c r="C295" s="88"/>
+      <c r="B295" s="89"/>
+      <c r="C295" s="90"/>
       <c r="D295" s="55"/>
       <c r="E295" s="55"/>
       <c r="F295" s="60"/>
@@ -51635,8 +51639,8 @@
       <c r="H295" s="59"/>
     </row>
     <row r="296" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B296" s="89"/>
-      <c r="C296" s="90"/>
+      <c r="B296" s="87"/>
+      <c r="C296" s="88"/>
       <c r="D296" s="56"/>
       <c r="E296" s="56"/>
       <c r="F296" s="53"/>
@@ -51644,8 +51648,8 @@
       <c r="H296" s="58"/>
     </row>
     <row r="297" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B297" s="87"/>
-      <c r="C297" s="88"/>
+      <c r="B297" s="89"/>
+      <c r="C297" s="90"/>
       <c r="D297" s="55"/>
       <c r="E297" s="55"/>
       <c r="F297" s="60"/>
@@ -51653,8 +51657,8 @@
       <c r="H297" s="59"/>
     </row>
     <row r="298" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="89"/>
-      <c r="C298" s="90"/>
+      <c r="B298" s="87"/>
+      <c r="C298" s="88"/>
       <c r="D298" s="56"/>
       <c r="E298" s="56"/>
       <c r="F298" s="53"/>
@@ -51662,8 +51666,8 @@
       <c r="H298" s="58"/>
     </row>
     <row r="299" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B299" s="87"/>
-      <c r="C299" s="88"/>
+      <c r="B299" s="89"/>
+      <c r="C299" s="90"/>
       <c r="D299" s="55"/>
       <c r="E299" s="55"/>
       <c r="F299" s="60"/>
@@ -51671,8 +51675,8 @@
       <c r="H299" s="59"/>
     </row>
     <row r="300" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B300" s="89"/>
-      <c r="C300" s="90"/>
+      <c r="B300" s="87"/>
+      <c r="C300" s="88"/>
       <c r="D300" s="56"/>
       <c r="E300" s="56"/>
       <c r="F300" s="53"/>
@@ -51680,288 +51684,8 @@
       <c r="H300" s="58"/>
     </row>
   </sheetData>
-  <sheetProtection password="CEBA" sheet="1" objects="1" scenarios="1" formatCells="0" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <sheetProtection formatCells="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <mergeCells count="292">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B182:C182"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B197:C197"/>
-    <mergeCell ref="B198:C198"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B227:C227"/>
-    <mergeCell ref="B228:C228"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B221:C221"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B234:C234"/>
-    <mergeCell ref="B235:C235"/>
-    <mergeCell ref="B236:C236"/>
-    <mergeCell ref="B237:C237"/>
-    <mergeCell ref="B238:C238"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="B230:C230"/>
-    <mergeCell ref="B231:C231"/>
-    <mergeCell ref="B232:C232"/>
-    <mergeCell ref="B233:C233"/>
-    <mergeCell ref="B244:C244"/>
-    <mergeCell ref="B245:C245"/>
-    <mergeCell ref="B246:C246"/>
-    <mergeCell ref="B247:C247"/>
-    <mergeCell ref="B248:C248"/>
-    <mergeCell ref="B239:C239"/>
-    <mergeCell ref="B240:C240"/>
-    <mergeCell ref="B241:C241"/>
-    <mergeCell ref="B242:C242"/>
-    <mergeCell ref="B243:C243"/>
-    <mergeCell ref="B254:C254"/>
-    <mergeCell ref="B255:C255"/>
-    <mergeCell ref="B256:C256"/>
-    <mergeCell ref="B257:C257"/>
-    <mergeCell ref="B258:C258"/>
-    <mergeCell ref="B249:C249"/>
-    <mergeCell ref="B250:C250"/>
-    <mergeCell ref="B251:C251"/>
-    <mergeCell ref="B252:C252"/>
-    <mergeCell ref="B253:C253"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B265:C265"/>
-    <mergeCell ref="B266:C266"/>
-    <mergeCell ref="B267:C267"/>
-    <mergeCell ref="B268:C268"/>
-    <mergeCell ref="B259:C259"/>
-    <mergeCell ref="B260:C260"/>
-    <mergeCell ref="B261:C261"/>
-    <mergeCell ref="B262:C262"/>
-    <mergeCell ref="B263:C263"/>
-    <mergeCell ref="B274:C274"/>
-    <mergeCell ref="B275:C275"/>
-    <mergeCell ref="B276:C276"/>
-    <mergeCell ref="B277:C277"/>
-    <mergeCell ref="B278:C278"/>
-    <mergeCell ref="B269:C269"/>
-    <mergeCell ref="B270:C270"/>
-    <mergeCell ref="B271:C271"/>
-    <mergeCell ref="B272:C272"/>
-    <mergeCell ref="B273:C273"/>
-    <mergeCell ref="B284:C284"/>
-    <mergeCell ref="B285:C285"/>
-    <mergeCell ref="B286:C286"/>
-    <mergeCell ref="B287:C287"/>
-    <mergeCell ref="B288:C288"/>
-    <mergeCell ref="B279:C279"/>
-    <mergeCell ref="B280:C280"/>
-    <mergeCell ref="B281:C281"/>
-    <mergeCell ref="B282:C282"/>
-    <mergeCell ref="B283:C283"/>
     <mergeCell ref="B299:C299"/>
     <mergeCell ref="B300:C300"/>
     <mergeCell ref="B294:C294"/>
@@ -51974,6 +51698,286 @@
     <mergeCell ref="B291:C291"/>
     <mergeCell ref="B292:C292"/>
     <mergeCell ref="B293:C293"/>
+    <mergeCell ref="B284:C284"/>
+    <mergeCell ref="B285:C285"/>
+    <mergeCell ref="B286:C286"/>
+    <mergeCell ref="B287:C287"/>
+    <mergeCell ref="B288:C288"/>
+    <mergeCell ref="B279:C279"/>
+    <mergeCell ref="B280:C280"/>
+    <mergeCell ref="B281:C281"/>
+    <mergeCell ref="B282:C282"/>
+    <mergeCell ref="B283:C283"/>
+    <mergeCell ref="B274:C274"/>
+    <mergeCell ref="B275:C275"/>
+    <mergeCell ref="B276:C276"/>
+    <mergeCell ref="B277:C277"/>
+    <mergeCell ref="B278:C278"/>
+    <mergeCell ref="B269:C269"/>
+    <mergeCell ref="B270:C270"/>
+    <mergeCell ref="B271:C271"/>
+    <mergeCell ref="B272:C272"/>
+    <mergeCell ref="B273:C273"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B265:C265"/>
+    <mergeCell ref="B266:C266"/>
+    <mergeCell ref="B267:C267"/>
+    <mergeCell ref="B268:C268"/>
+    <mergeCell ref="B259:C259"/>
+    <mergeCell ref="B260:C260"/>
+    <mergeCell ref="B261:C261"/>
+    <mergeCell ref="B262:C262"/>
+    <mergeCell ref="B263:C263"/>
+    <mergeCell ref="B254:C254"/>
+    <mergeCell ref="B255:C255"/>
+    <mergeCell ref="B256:C256"/>
+    <mergeCell ref="B257:C257"/>
+    <mergeCell ref="B258:C258"/>
+    <mergeCell ref="B249:C249"/>
+    <mergeCell ref="B250:C250"/>
+    <mergeCell ref="B251:C251"/>
+    <mergeCell ref="B252:C252"/>
+    <mergeCell ref="B253:C253"/>
+    <mergeCell ref="B244:C244"/>
+    <mergeCell ref="B245:C245"/>
+    <mergeCell ref="B246:C246"/>
+    <mergeCell ref="B247:C247"/>
+    <mergeCell ref="B248:C248"/>
+    <mergeCell ref="B239:C239"/>
+    <mergeCell ref="B240:C240"/>
+    <mergeCell ref="B241:C241"/>
+    <mergeCell ref="B242:C242"/>
+    <mergeCell ref="B243:C243"/>
+    <mergeCell ref="B234:C234"/>
+    <mergeCell ref="B235:C235"/>
+    <mergeCell ref="B236:C236"/>
+    <mergeCell ref="B237:C237"/>
+    <mergeCell ref="B238:C238"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="B230:C230"/>
+    <mergeCell ref="B231:C231"/>
+    <mergeCell ref="B232:C232"/>
+    <mergeCell ref="B233:C233"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B227:C227"/>
+    <mergeCell ref="B228:C228"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B221:C221"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:C198"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B187:C187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F300">
     <cfRule type="expression" dxfId="2" priority="1">
@@ -52033,12 +52037,12 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="85">
         <f>Projekt_Name</f>
         <v>0</v>
       </c>
       <c r="D2" s="93"/>
-      <c r="E2" s="82"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>

</xml_diff>